<commit_message>
GS 1.1 to 1.8 25/0/92020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Raja Files/Padam Inputs/TS 1.1 Padam Input Template.xlsx
+++ b/TS Jatai Working/Raja Files/Padam Inputs/TS 1.1 Padam Input Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\padam_excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\Raja Files\Padam Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -4138,8 +4138,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y1580"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1034" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="T1462" sqref="T1462"/>
     </sheetView>

</xml_diff>

<commit_message>
Changes in Jatai and Jatai working 30/09/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Raja Files/Padam Inputs/TS 1.1 Padam Input Template.xlsx
+++ b/TS Jatai Working/Raja Files/Padam Inputs/TS 1.1 Padam Input Template.xlsx
@@ -4138,10 +4138,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y1580"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1034" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="T1462" sqref="T1462"/>
+      <selection pane="bottomLeft" activeCell="Y8" sqref="Y8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
TS 1.1 and Rules Table 17/10/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Raja Files/Padam Inputs/TS 1.1 Padam Input Template.xlsx
+++ b/TS Jatai Working/Raja Files/Padam Inputs/TS 1.1 Padam Input Template.xlsx
@@ -15,7 +15,7 @@
     <sheet name="TS 1.1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'TS 1.1'!$A$1:$X$621</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'TS 1.1'!$C$1:$X$1531</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4186" uniqueCount="1225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4177" uniqueCount="1218">
   <si>
     <t>PS</t>
   </si>
@@ -3413,9 +3413,6 @@
     <t>Vis</t>
   </si>
   <si>
-    <t>ViS</t>
-  </si>
-  <si>
     <t>vaqrq.ShavRu#ddham |</t>
   </si>
   <si>
@@ -3440,18 +3437,9 @@
     <t>NRE</t>
   </si>
   <si>
-    <t>N(gm)+R(gm)</t>
-  </si>
-  <si>
-    <t>N(gm)+S(gm)</t>
-  </si>
-  <si>
     <t>NSE+NRE</t>
   </si>
   <si>
-    <t>ntN</t>
-  </si>
-  <si>
     <t>GS Ref</t>
   </si>
   <si>
@@ -3500,9 +3488,6 @@
     <t>PS-8-8</t>
   </si>
   <si>
-    <t>Rev</t>
-  </si>
-  <si>
     <t>ngmv</t>
   </si>
   <si>
@@ -3668,40 +3653,34 @@
     <t>GD-88</t>
   </si>
   <si>
-    <t>r</t>
-  </si>
-  <si>
     <t>PS-11.8</t>
   </si>
   <si>
     <t>viqraqphSiqnniti# vi - raqphSiqnn |</t>
   </si>
   <si>
-    <t>ngm</t>
-  </si>
-  <si>
-    <t>s</t>
-  </si>
-  <si>
     <t>syAqlAditi# syAlat ||</t>
   </si>
   <si>
-    <t>N(s)</t>
-  </si>
-  <si>
     <t>NE+NRE</t>
   </si>
   <si>
     <t>IDyaq itIDya#H ||</t>
   </si>
   <si>
-    <t>N(gm)</t>
-  </si>
-  <si>
     <t>Table  Process</t>
   </si>
   <si>
     <t>Padam Split Expansion</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>N+R</t>
+  </si>
+  <si>
+    <t>N+S</t>
   </si>
 </sst>
 </file>
@@ -3873,7 +3852,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -4050,6 +4029,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4336,7 +4318,7 @@
     <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="X2" sqref="X2"/>
+      <selection pane="bottomLeft" activeCell="S1006" sqref="S1006"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -4826,7 +4808,7 @@
         <v>9</v>
       </c>
       <c r="H1" s="54" t="s">
-        <v>1141</v>
+        <v>1137</v>
       </c>
       <c r="I1" s="17" t="s">
         <v>815</v>
@@ -4859,22 +4841,22 @@
         <v>11</v>
       </c>
       <c r="S1" s="15" t="s">
-        <v>1223</v>
+        <v>1213</v>
       </c>
       <c r="T1" s="15" t="s">
-        <v>1155</v>
+        <v>1151</v>
       </c>
       <c r="U1" s="15" t="s">
-        <v>1161</v>
+        <v>1156</v>
       </c>
       <c r="V1" s="15" t="s">
-        <v>1162</v>
+        <v>1157</v>
       </c>
       <c r="W1" s="15" t="s">
-        <v>1163</v>
+        <v>1158</v>
       </c>
       <c r="X1" s="62" t="s">
-        <v>1224</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="2" spans="1:24" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4886,7 +4868,7 @@
       <c r="F2" s="37"/>
       <c r="G2" s="37"/>
       <c r="H2" s="58" t="s">
-        <v>1164</v>
+        <v>1159</v>
       </c>
       <c r="I2" s="11" t="s">
         <v>817</v>
@@ -4926,7 +4908,7 @@
       <c r="F3" s="37"/>
       <c r="G3" s="37"/>
       <c r="H3" s="58" t="s">
-        <v>1164</v>
+        <v>1159</v>
       </c>
       <c r="I3" s="11" t="s">
         <v>817</v>
@@ -4968,7 +4950,7 @@
       <c r="F4" s="37"/>
       <c r="G4" s="37"/>
       <c r="H4" s="58" t="s">
-        <v>1164</v>
+        <v>1159</v>
       </c>
       <c r="I4" s="11" t="s">
         <v>817</v>
@@ -5010,7 +4992,7 @@
       <c r="F5" s="37"/>
       <c r="G5" s="37"/>
       <c r="H5" s="58" t="s">
-        <v>1164</v>
+        <v>1159</v>
       </c>
       <c r="I5" s="11" t="s">
         <v>817</v>
@@ -5871,7 +5853,7 @@
       <c r="F26" s="37"/>
       <c r="G26" s="37"/>
       <c r="H26" s="58" t="s">
-        <v>1165</v>
+        <v>1160</v>
       </c>
       <c r="I26" s="11" t="s">
         <v>817</v>
@@ -5913,7 +5895,7 @@
       <c r="F27" s="37"/>
       <c r="G27" s="37"/>
       <c r="H27" s="58" t="s">
-        <v>1165</v>
+        <v>1160</v>
       </c>
       <c r="I27" s="11" t="s">
         <v>817</v>
@@ -5952,7 +5934,7 @@
       <c r="F28" s="36"/>
       <c r="G28" s="36"/>
       <c r="H28" s="58" t="s">
-        <v>1165</v>
+        <v>1160</v>
       </c>
       <c r="I28" s="11" t="s">
         <v>817</v>
@@ -5994,7 +5976,7 @@
       <c r="F29" s="37"/>
       <c r="G29" s="37"/>
       <c r="H29" s="58" t="s">
-        <v>1165</v>
+        <v>1160</v>
       </c>
       <c r="I29" s="11" t="s">
         <v>817</v>
@@ -6036,7 +6018,7 @@
       <c r="F30" s="37"/>
       <c r="G30" s="37"/>
       <c r="H30" s="58" t="s">
-        <v>1165</v>
+        <v>1160</v>
       </c>
       <c r="I30" s="11" t="s">
         <v>817</v>
@@ -6078,7 +6060,7 @@
       <c r="F31" s="37"/>
       <c r="G31" s="37"/>
       <c r="H31" s="58" t="s">
-        <v>1165</v>
+        <v>1160</v>
       </c>
       <c r="I31" s="11" t="s">
         <v>817</v>
@@ -6928,7 +6910,7 @@
       <c r="F52" s="37"/>
       <c r="G52" s="37"/>
       <c r="H52" s="58" t="s">
-        <v>1166</v>
+        <v>1161</v>
       </c>
       <c r="I52" s="11" t="s">
         <v>818</v>
@@ -6969,7 +6951,7 @@
       <c r="F53" s="36"/>
       <c r="G53" s="36"/>
       <c r="H53" s="58" t="s">
-        <v>1166</v>
+        <v>1161</v>
       </c>
       <c r="I53" s="11" t="s">
         <v>818</v>
@@ -7011,7 +6993,7 @@
       <c r="F54" s="37"/>
       <c r="G54" s="37"/>
       <c r="H54" s="58" t="s">
-        <v>1166</v>
+        <v>1161</v>
       </c>
       <c r="I54" s="11" t="s">
         <v>818</v>
@@ -7053,7 +7035,7 @@
       <c r="F55" s="37"/>
       <c r="G55" s="37"/>
       <c r="H55" s="58" t="s">
-        <v>1166</v>
+        <v>1161</v>
       </c>
       <c r="I55" s="11" t="s">
         <v>818</v>
@@ -7095,7 +7077,7 @@
       <c r="F56" s="37"/>
       <c r="G56" s="37"/>
       <c r="H56" s="58" t="s">
-        <v>1166</v>
+        <v>1161</v>
       </c>
       <c r="I56" s="11" t="s">
         <v>818</v>
@@ -7137,7 +7119,7 @@
       <c r="F57" s="37"/>
       <c r="G57" s="37"/>
       <c r="H57" s="58" t="s">
-        <v>1166</v>
+        <v>1161</v>
       </c>
       <c r="I57" s="11" t="s">
         <v>818</v>
@@ -7976,7 +7958,7 @@
       <c r="F78" s="36"/>
       <c r="G78" s="36"/>
       <c r="H78" s="58" t="s">
-        <v>1167</v>
+        <v>1162</v>
       </c>
       <c r="I78" s="11" t="s">
         <v>818</v>
@@ -8018,7 +8000,7 @@
       <c r="F79" s="37"/>
       <c r="G79" s="37"/>
       <c r="H79" s="58" t="s">
-        <v>1167</v>
+        <v>1162</v>
       </c>
       <c r="I79" s="11" t="s">
         <v>818</v>
@@ -8057,7 +8039,7 @@
       <c r="F80" s="36"/>
       <c r="G80" s="36"/>
       <c r="H80" s="58" t="s">
-        <v>1167</v>
+        <v>1162</v>
       </c>
       <c r="I80" s="11" t="s">
         <v>818</v>
@@ -8096,7 +8078,7 @@
       <c r="F81" s="36"/>
       <c r="G81" s="36"/>
       <c r="H81" s="58" t="s">
-        <v>1167</v>
+        <v>1162</v>
       </c>
       <c r="I81" s="11" t="s">
         <v>818</v>
@@ -8135,7 +8117,7 @@
       <c r="F82" s="36"/>
       <c r="G82" s="36"/>
       <c r="H82" s="58" t="s">
-        <v>1167</v>
+        <v>1162</v>
       </c>
       <c r="I82" s="11" t="s">
         <v>818</v>
@@ -8174,7 +8156,7 @@
       <c r="F83" s="36"/>
       <c r="G83" s="36"/>
       <c r="H83" s="58" t="s">
-        <v>1167</v>
+        <v>1162</v>
       </c>
       <c r="I83" s="11" t="s">
         <v>818</v>
@@ -8213,7 +8195,7 @@
       <c r="F84" s="36"/>
       <c r="G84" s="36"/>
       <c r="H84" s="58" t="s">
-        <v>1167</v>
+        <v>1162</v>
       </c>
       <c r="I84" s="11" t="s">
         <v>818</v>
@@ -9387,14 +9369,14 @@
     <row r="115" spans="4:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D115" s="42"/>
       <c r="E115" s="59" t="s">
-        <v>1195</v>
+        <v>1190</v>
       </c>
       <c r="F115" s="59" t="s">
-        <v>1196</v>
+        <v>1191</v>
       </c>
       <c r="G115" s="36"/>
       <c r="H115" s="55" t="s">
-        <v>1142</v>
+        <v>1138</v>
       </c>
       <c r="I115" s="11" t="s">
         <v>819</v>
@@ -9432,14 +9414,14 @@
     <row r="116" spans="4:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D116" s="42"/>
       <c r="E116" s="59" t="s">
-        <v>1195</v>
+        <v>1190</v>
       </c>
       <c r="F116" s="59" t="s">
-        <v>1196</v>
+        <v>1191</v>
       </c>
       <c r="G116" s="36"/>
       <c r="H116" s="55" t="s">
-        <v>1142</v>
+        <v>1138</v>
       </c>
       <c r="I116" s="11" t="s">
         <v>819</v>
@@ -9477,14 +9459,14 @@
     <row r="117" spans="4:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D117" s="42"/>
       <c r="E117" s="59" t="s">
-        <v>1195</v>
+        <v>1190</v>
       </c>
       <c r="F117" s="59" t="s">
-        <v>1196</v>
+        <v>1191</v>
       </c>
       <c r="G117" s="36"/>
       <c r="H117" s="55" t="s">
-        <v>1142</v>
+        <v>1138</v>
       </c>
       <c r="I117" s="11" t="s">
         <v>819</v>
@@ -9520,14 +9502,14 @@
     <row r="118" spans="4:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D118" s="42"/>
       <c r="E118" s="59" t="s">
-        <v>1195</v>
+        <v>1190</v>
       </c>
       <c r="F118" s="59" t="s">
-        <v>1196</v>
+        <v>1191</v>
       </c>
       <c r="G118" s="36"/>
       <c r="H118" s="55" t="s">
-        <v>1142</v>
+        <v>1138</v>
       </c>
       <c r="I118" s="11" t="s">
         <v>819</v>
@@ -9562,14 +9544,14 @@
     <row r="119" spans="4:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D119" s="42"/>
       <c r="E119" s="59" t="s">
-        <v>1195</v>
+        <v>1190</v>
       </c>
       <c r="F119" s="59" t="s">
-        <v>1196</v>
+        <v>1191</v>
       </c>
       <c r="G119" s="36"/>
       <c r="H119" s="55" t="s">
-        <v>1142</v>
+        <v>1138</v>
       </c>
       <c r="I119" s="11" t="s">
         <v>819</v>
@@ -9867,7 +9849,7 @@
       <c r="F127" s="36"/>
       <c r="G127" s="36"/>
       <c r="H127" s="59" t="s">
-        <v>1168</v>
+        <v>1163</v>
       </c>
       <c r="I127" s="11" t="s">
         <v>819</v>
@@ -9905,7 +9887,7 @@
       <c r="F128" s="36"/>
       <c r="G128" s="36"/>
       <c r="H128" s="59" t="s">
-        <v>1168</v>
+        <v>1163</v>
       </c>
       <c r="I128" s="11" t="s">
         <v>819</v>
@@ -9943,7 +9925,7 @@
       <c r="F129" s="36"/>
       <c r="G129" s="36"/>
       <c r="H129" s="59" t="s">
-        <v>1168</v>
+        <v>1163</v>
       </c>
       <c r="I129" s="11" t="s">
         <v>819</v>
@@ -9984,7 +9966,7 @@
       <c r="F130" s="36"/>
       <c r="G130" s="36"/>
       <c r="H130" s="59" t="s">
-        <v>1168</v>
+        <v>1163</v>
       </c>
       <c r="I130" s="11" t="s">
         <v>819</v>
@@ -10022,7 +10004,7 @@
       <c r="F131" s="36"/>
       <c r="G131" s="36"/>
       <c r="H131" s="59" t="s">
-        <v>1168</v>
+        <v>1163</v>
       </c>
       <c r="I131" s="11" t="s">
         <v>819</v>
@@ -10689,7 +10671,7 @@
       <c r="E149" s="36"/>
       <c r="F149" s="36"/>
       <c r="G149" s="59" t="s">
-        <v>1212</v>
+        <v>1207</v>
       </c>
       <c r="H149" s="36"/>
       <c r="I149" s="11" t="s">
@@ -10725,12 +10707,12 @@
     </row>
     <row r="150" spans="4:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D150" s="60" t="s">
-        <v>1197</v>
+        <v>1192</v>
       </c>
       <c r="E150" s="36"/>
       <c r="F150" s="36"/>
       <c r="G150" s="59" t="s">
-        <v>1212</v>
+        <v>1207</v>
       </c>
       <c r="H150" s="36"/>
       <c r="I150" s="11" t="s">
@@ -10760,9 +10742,7 @@
       <c r="S150" s="9" t="s">
         <v>1127</v>
       </c>
-      <c r="T150" s="9" t="s">
-        <v>1213</v>
-      </c>
+      <c r="T150" s="9"/>
       <c r="U150" s="9"/>
       <c r="V150" s="9"/>
       <c r="W150" s="9"/>
@@ -10772,7 +10752,7 @@
       <c r="E151" s="36"/>
       <c r="F151" s="36"/>
       <c r="G151" s="59" t="s">
-        <v>1212</v>
+        <v>1207</v>
       </c>
       <c r="H151" s="36"/>
       <c r="I151" s="11" t="s">
@@ -11704,10 +11684,10 @@
       <c r="E176" s="36"/>
       <c r="F176" s="36"/>
       <c r="G176" s="59" t="s">
-        <v>1207</v>
+        <v>1202</v>
       </c>
       <c r="H176" s="55" t="s">
-        <v>1143</v>
+        <v>1139</v>
       </c>
       <c r="I176" s="11" t="s">
         <v>820</v>
@@ -11749,10 +11729,10 @@
       <c r="E177" s="36"/>
       <c r="F177" s="36"/>
       <c r="G177" s="59" t="s">
-        <v>1207</v>
+        <v>1202</v>
       </c>
       <c r="H177" s="55" t="s">
-        <v>1143</v>
+        <v>1139</v>
       </c>
       <c r="I177" s="11" t="s">
         <v>820</v>
@@ -11789,10 +11769,10 @@
       <c r="E178" s="36"/>
       <c r="F178" s="36"/>
       <c r="G178" s="59" t="s">
-        <v>1207</v>
+        <v>1202</v>
       </c>
       <c r="H178" s="55" t="s">
-        <v>1143</v>
+        <v>1139</v>
       </c>
       <c r="I178" s="11" t="s">
         <v>820</v>
@@ -11943,7 +11923,7 @@
       <c r="F182" s="36"/>
       <c r="G182" s="36"/>
       <c r="H182" s="59" t="s">
-        <v>1169</v>
+        <v>1164</v>
       </c>
       <c r="I182" s="11" t="s">
         <v>820</v>
@@ -11981,7 +11961,7 @@
       <c r="F183" s="36"/>
       <c r="G183" s="36"/>
       <c r="H183" s="59" t="s">
-        <v>1169</v>
+        <v>1164</v>
       </c>
       <c r="I183" s="11" t="s">
         <v>820</v>
@@ -12019,7 +11999,7 @@
       <c r="F184" s="36"/>
       <c r="G184" s="36"/>
       <c r="H184" s="59" t="s">
-        <v>1169</v>
+        <v>1164</v>
       </c>
       <c r="I184" s="11" t="s">
         <v>820</v>
@@ -12059,7 +12039,7 @@
       <c r="F185" s="36"/>
       <c r="G185" s="36"/>
       <c r="H185" s="59" t="s">
-        <v>1169</v>
+        <v>1164</v>
       </c>
       <c r="I185" s="11" t="s">
         <v>820</v>
@@ -12097,7 +12077,7 @@
       <c r="F186" s="36"/>
       <c r="G186" s="36"/>
       <c r="H186" s="59" t="s">
-        <v>1169</v>
+        <v>1164</v>
       </c>
       <c r="I186" s="11" t="s">
         <v>820</v>
@@ -12135,7 +12115,7 @@
       <c r="F187" s="36"/>
       <c r="G187" s="36"/>
       <c r="H187" s="59" t="s">
-        <v>1169</v>
+        <v>1164</v>
       </c>
       <c r="I187" s="11" t="s">
         <v>820</v>
@@ -12660,7 +12640,7 @@
       <c r="F201" s="36"/>
       <c r="G201" s="36"/>
       <c r="H201" s="59" t="s">
-        <v>1170</v>
+        <v>1165</v>
       </c>
       <c r="I201" s="11" t="s">
         <v>821</v>
@@ -12698,7 +12678,7 @@
       <c r="F202" s="36"/>
       <c r="G202" s="36"/>
       <c r="H202" s="59" t="s">
-        <v>1170</v>
+        <v>1165</v>
       </c>
       <c r="I202" s="11" t="s">
         <v>821</v>
@@ -12736,7 +12716,7 @@
       <c r="F203" s="36"/>
       <c r="G203" s="36"/>
       <c r="H203" s="59" t="s">
-        <v>1170</v>
+        <v>1165</v>
       </c>
       <c r="I203" s="11" t="s">
         <v>821</v>
@@ -12774,7 +12754,7 @@
       <c r="F204" s="36"/>
       <c r="G204" s="36"/>
       <c r="H204" s="59" t="s">
-        <v>1170</v>
+        <v>1165</v>
       </c>
       <c r="I204" s="11" t="s">
         <v>821</v>
@@ -12812,7 +12792,7 @@
       <c r="F205" s="36"/>
       <c r="G205" s="36"/>
       <c r="H205" s="59" t="s">
-        <v>1170</v>
+        <v>1165</v>
       </c>
       <c r="I205" s="11" t="s">
         <v>821</v>
@@ -12850,7 +12830,7 @@
       <c r="F206" s="36"/>
       <c r="G206" s="36"/>
       <c r="H206" s="59" t="s">
-        <v>1170</v>
+        <v>1165</v>
       </c>
       <c r="I206" s="11" t="s">
         <v>821</v>
@@ -12888,7 +12868,7 @@
       <c r="F207" s="36"/>
       <c r="G207" s="36"/>
       <c r="H207" s="59" t="s">
-        <v>1170</v>
+        <v>1165</v>
       </c>
       <c r="I207" s="11" t="s">
         <v>821</v>
@@ -12926,7 +12906,7 @@
       <c r="F208" s="36"/>
       <c r="G208" s="36"/>
       <c r="H208" s="59" t="s">
-        <v>1170</v>
+        <v>1165</v>
       </c>
       <c r="I208" s="11" t="s">
         <v>821</v>
@@ -12964,7 +12944,7 @@
       <c r="F209" s="36"/>
       <c r="G209" s="36"/>
       <c r="H209" s="59" t="s">
-        <v>1170</v>
+        <v>1165</v>
       </c>
       <c r="I209" s="11" t="s">
         <v>821</v>
@@ -13002,7 +12982,7 @@
       <c r="F210" s="36"/>
       <c r="G210" s="36"/>
       <c r="H210" s="59" t="s">
-        <v>1170</v>
+        <v>1165</v>
       </c>
       <c r="I210" s="11" t="s">
         <v>821</v>
@@ -13040,7 +13020,7 @@
       <c r="F211" s="36"/>
       <c r="G211" s="36"/>
       <c r="H211" s="59" t="s">
-        <v>1170</v>
+        <v>1165</v>
       </c>
       <c r="I211" s="11" t="s">
         <v>821</v>
@@ -13079,7 +13059,7 @@
       <c r="F212" s="36"/>
       <c r="G212" s="36"/>
       <c r="H212" s="59" t="s">
-        <v>1170</v>
+        <v>1165</v>
       </c>
       <c r="I212" s="11" t="s">
         <v>821</v>
@@ -13684,7 +13664,7 @@
     </row>
     <row r="228" spans="4:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D228" s="60" t="s">
-        <v>1197</v>
+        <v>1192</v>
       </c>
       <c r="E228" s="36"/>
       <c r="F228" s="36"/>
@@ -13715,11 +13695,9 @@
       <c r="Q228" s="9"/>
       <c r="R228" s="9"/>
       <c r="S228" s="9" t="s">
-        <v>1128</v>
-      </c>
-      <c r="T228" s="9" t="s">
-        <v>1213</v>
-      </c>
+        <v>1127</v>
+      </c>
+      <c r="T228" s="9"/>
       <c r="U228" s="9"/>
       <c r="V228" s="9"/>
       <c r="W228" s="9"/>
@@ -14131,7 +14109,7 @@
       <c r="F240" s="36"/>
       <c r="G240" s="36"/>
       <c r="H240" s="59" t="s">
-        <v>1171</v>
+        <v>1166</v>
       </c>
       <c r="I240" s="11" t="s">
         <v>821</v>
@@ -14169,7 +14147,7 @@
       <c r="F241" s="36"/>
       <c r="G241" s="36"/>
       <c r="H241" s="59" t="s">
-        <v>1171</v>
+        <v>1166</v>
       </c>
       <c r="I241" s="11" t="s">
         <v>822</v>
@@ -14207,7 +14185,7 @@
       <c r="F242" s="36"/>
       <c r="G242" s="36"/>
       <c r="H242" s="59" t="s">
-        <v>1171</v>
+        <v>1166</v>
       </c>
       <c r="I242" s="11" t="s">
         <v>822</v>
@@ -14245,7 +14223,7 @@
       <c r="F243" s="36"/>
       <c r="G243" s="36"/>
       <c r="H243" s="59" t="s">
-        <v>1171</v>
+        <v>1166</v>
       </c>
       <c r="I243" s="11" t="s">
         <v>822</v>
@@ -14389,7 +14367,7 @@
       <c r="D247" s="42"/>
       <c r="E247" s="36"/>
       <c r="F247" s="59" t="s">
-        <v>1203</v>
+        <v>1198</v>
       </c>
       <c r="G247" s="36"/>
       <c r="H247" s="36"/>
@@ -14432,7 +14410,7 @@
       <c r="D248" s="42"/>
       <c r="E248" s="36"/>
       <c r="F248" s="59" t="s">
-        <v>1203</v>
+        <v>1198</v>
       </c>
       <c r="G248" s="36"/>
       <c r="H248" s="36"/>
@@ -14773,7 +14751,7 @@
       <c r="F257" s="36"/>
       <c r="G257" s="36"/>
       <c r="H257" s="59" t="s">
-        <v>1172</v>
+        <v>1167</v>
       </c>
       <c r="I257" s="11" t="s">
         <v>822</v>
@@ -14811,7 +14789,7 @@
       <c r="F258" s="36"/>
       <c r="G258" s="36"/>
       <c r="H258" s="59" t="s">
-        <v>1172</v>
+        <v>1167</v>
       </c>
       <c r="I258" s="11" t="s">
         <v>822</v>
@@ -14849,7 +14827,7 @@
       <c r="F259" s="36"/>
       <c r="G259" s="36"/>
       <c r="H259" s="59" t="s">
-        <v>1172</v>
+        <v>1167</v>
       </c>
       <c r="I259" s="11" t="s">
         <v>822</v>
@@ -14887,7 +14865,7 @@
       <c r="F260" s="36"/>
       <c r="G260" s="36"/>
       <c r="H260" s="59" t="s">
-        <v>1172</v>
+        <v>1167</v>
       </c>
       <c r="I260" s="11" t="s">
         <v>822</v>
@@ -14925,7 +14903,7 @@
       <c r="F261" s="36"/>
       <c r="G261" s="36"/>
       <c r="H261" s="59" t="s">
-        <v>1172</v>
+        <v>1167</v>
       </c>
       <c r="I261" s="11" t="s">
         <v>822</v>
@@ -15139,13 +15117,13 @@
     </row>
     <row r="267" spans="4:23" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D267" s="56" t="s">
-        <v>1156</v>
+        <v>1152</v>
       </c>
       <c r="E267" s="36"/>
       <c r="F267" s="36"/>
       <c r="G267" s="36"/>
       <c r="H267" s="59" t="s">
-        <v>1173</v>
+        <v>1168</v>
       </c>
       <c r="I267" s="11" t="s">
         <v>822</v>
@@ -15185,7 +15163,7 @@
       <c r="F268" s="36"/>
       <c r="G268" s="36"/>
       <c r="H268" s="59" t="s">
-        <v>1173</v>
+        <v>1168</v>
       </c>
       <c r="I268" s="11" t="s">
         <v>822</v>
@@ -15225,7 +15203,7 @@
       <c r="F269" s="36"/>
       <c r="G269" s="36"/>
       <c r="H269" s="59" t="s">
-        <v>1173</v>
+        <v>1168</v>
       </c>
       <c r="I269" s="11" t="s">
         <v>822</v>
@@ -15265,7 +15243,7 @@
       <c r="F270" s="36"/>
       <c r="G270" s="36"/>
       <c r="H270" s="59" t="s">
-        <v>1173</v>
+        <v>1168</v>
       </c>
       <c r="I270" s="11" t="s">
         <v>822</v>
@@ -15560,7 +15538,7 @@
       <c r="F278" s="36"/>
       <c r="G278" s="36"/>
       <c r="H278" s="59" t="s">
-        <v>1174</v>
+        <v>1169</v>
       </c>
       <c r="I278" s="11" t="s">
         <v>822</v>
@@ -15600,7 +15578,7 @@
       <c r="F279" s="36"/>
       <c r="G279" s="36"/>
       <c r="H279" s="59" t="s">
-        <v>1174</v>
+        <v>1169</v>
       </c>
       <c r="I279" s="11" t="s">
         <v>822</v>
@@ -15638,7 +15616,7 @@
       <c r="F280" s="36"/>
       <c r="G280" s="36"/>
       <c r="H280" s="59" t="s">
-        <v>1174</v>
+        <v>1169</v>
       </c>
       <c r="I280" s="11" t="s">
         <v>822</v>
@@ -15676,7 +15654,7 @@
       <c r="F281" s="36"/>
       <c r="G281" s="36"/>
       <c r="H281" s="59" t="s">
-        <v>1174</v>
+        <v>1169</v>
       </c>
       <c r="I281" s="11" t="s">
         <v>822</v>
@@ -15714,7 +15692,7 @@
       <c r="F282" s="36"/>
       <c r="G282" s="36"/>
       <c r="H282" s="59" t="s">
-        <v>1174</v>
+        <v>1169</v>
       </c>
       <c r="I282" s="11" t="s">
         <v>822</v>
@@ -15906,7 +15884,7 @@
       <c r="F287" s="36"/>
       <c r="G287" s="36"/>
       <c r="H287" s="59" t="s">
-        <v>1175</v>
+        <v>1170</v>
       </c>
       <c r="I287" s="11" t="s">
         <v>823</v>
@@ -15943,7 +15921,7 @@
       <c r="F288" s="36"/>
       <c r="G288" s="36"/>
       <c r="H288" s="59" t="s">
-        <v>1175</v>
+        <v>1170</v>
       </c>
       <c r="I288" s="11" t="s">
         <v>823</v>
@@ -15981,7 +15959,7 @@
       <c r="F289" s="36"/>
       <c r="G289" s="36"/>
       <c r="H289" s="59" t="s">
-        <v>1175</v>
+        <v>1170</v>
       </c>
       <c r="I289" s="11" t="s">
         <v>823</v>
@@ -16019,7 +15997,7 @@
       <c r="F290" s="36"/>
       <c r="G290" s="36"/>
       <c r="H290" s="59" t="s">
-        <v>1175</v>
+        <v>1170</v>
       </c>
       <c r="I290" s="11" t="s">
         <v>823</v>
@@ -16059,7 +16037,7 @@
       <c r="F291" s="36"/>
       <c r="G291" s="36"/>
       <c r="H291" s="59" t="s">
-        <v>1175</v>
+        <v>1170</v>
       </c>
       <c r="I291" s="11" t="s">
         <v>823</v>
@@ -16282,7 +16260,7 @@
       <c r="F297" s="36"/>
       <c r="G297" s="36"/>
       <c r="H297" s="55" t="s">
-        <v>1144</v>
+        <v>1140</v>
       </c>
       <c r="I297" s="11" t="s">
         <v>823</v>
@@ -16320,7 +16298,7 @@
       <c r="F298" s="36"/>
       <c r="G298" s="36"/>
       <c r="H298" s="55" t="s">
-        <v>1144</v>
+        <v>1140</v>
       </c>
       <c r="I298" s="11" t="s">
         <v>823</v>
@@ -16357,10 +16335,10 @@
       <c r="E299" s="36"/>
       <c r="F299" s="36"/>
       <c r="G299" s="59" t="s">
-        <v>1210</v>
+        <v>1205</v>
       </c>
       <c r="H299" s="55" t="s">
-        <v>1144</v>
+        <v>1140</v>
       </c>
       <c r="I299" s="11" t="s">
         <v>823</v>
@@ -16404,10 +16382,10 @@
       <c r="E300" s="36"/>
       <c r="F300" s="36"/>
       <c r="G300" s="59" t="s">
-        <v>1210</v>
+        <v>1205</v>
       </c>
       <c r="H300" s="55" t="s">
-        <v>1144</v>
+        <v>1140</v>
       </c>
       <c r="I300" s="11" t="s">
         <v>823</v>
@@ -16451,10 +16429,10 @@
       <c r="E301" s="36"/>
       <c r="F301" s="36"/>
       <c r="G301" s="59" t="s">
-        <v>1210</v>
+        <v>1205</v>
       </c>
       <c r="H301" s="55" t="s">
-        <v>1144</v>
+        <v>1140</v>
       </c>
       <c r="I301" s="11" t="s">
         <v>823</v>
@@ -18461,7 +18439,7 @@
       <c r="F355" s="36"/>
       <c r="G355" s="36"/>
       <c r="H355" s="59" t="s">
-        <v>1176</v>
+        <v>1171</v>
       </c>
       <c r="I355" s="11" t="s">
         <v>824</v>
@@ -18499,7 +18477,7 @@
       <c r="F356" s="36"/>
       <c r="G356" s="36"/>
       <c r="H356" s="59" t="s">
-        <v>1176</v>
+        <v>1171</v>
       </c>
       <c r="I356" s="11" t="s">
         <v>824</v>
@@ -18537,7 +18515,7 @@
       <c r="F357" s="36"/>
       <c r="G357" s="36"/>
       <c r="H357" s="59" t="s">
-        <v>1176</v>
+        <v>1171</v>
       </c>
       <c r="I357" s="11" t="s">
         <v>824</v>
@@ -18576,7 +18554,7 @@
       <c r="F358" s="36"/>
       <c r="G358" s="36"/>
       <c r="H358" s="59" t="s">
-        <v>1176</v>
+        <v>1171</v>
       </c>
       <c r="I358" s="11" t="s">
         <v>824</v>
@@ -18614,7 +18592,7 @@
       <c r="F359" s="36"/>
       <c r="G359" s="36"/>
       <c r="H359" s="59" t="s">
-        <v>1176</v>
+        <v>1171</v>
       </c>
       <c r="I359" s="11" t="s">
         <v>824</v>
@@ -18652,7 +18630,7 @@
       <c r="F360" s="36"/>
       <c r="G360" s="36"/>
       <c r="H360" s="59" t="s">
-        <v>1176</v>
+        <v>1171</v>
       </c>
       <c r="I360" s="11" t="s">
         <v>824</v>
@@ -18690,7 +18668,7 @@
       <c r="F361" s="36"/>
       <c r="G361" s="36"/>
       <c r="H361" s="59" t="s">
-        <v>1176</v>
+        <v>1171</v>
       </c>
       <c r="I361" s="11" t="s">
         <v>824</v>
@@ -18728,7 +18706,7 @@
       <c r="F362" s="36"/>
       <c r="G362" s="36"/>
       <c r="H362" s="59" t="s">
-        <v>1176</v>
+        <v>1171</v>
       </c>
       <c r="I362" s="11" t="s">
         <v>824</v>
@@ -18771,7 +18749,7 @@
       <c r="F363" s="36"/>
       <c r="G363" s="36"/>
       <c r="H363" s="59" t="s">
-        <v>1176</v>
+        <v>1171</v>
       </c>
       <c r="I363" s="11" t="s">
         <v>824</v>
@@ -18809,7 +18787,7 @@
       <c r="F364" s="36"/>
       <c r="G364" s="36"/>
       <c r="H364" s="59" t="s">
-        <v>1176</v>
+        <v>1171</v>
       </c>
       <c r="I364" s="11" t="s">
         <v>824</v>
@@ -18847,7 +18825,7 @@
       <c r="F365" s="36"/>
       <c r="G365" s="36"/>
       <c r="H365" s="59" t="s">
-        <v>1176</v>
+        <v>1171</v>
       </c>
       <c r="I365" s="11" t="s">
         <v>824</v>
@@ -18887,7 +18865,7 @@
       <c r="F366" s="36"/>
       <c r="G366" s="36"/>
       <c r="H366" s="59" t="s">
-        <v>1176</v>
+        <v>1171</v>
       </c>
       <c r="I366" s="11" t="s">
         <v>824</v>
@@ -18925,7 +18903,7 @@
       <c r="F367" s="36"/>
       <c r="G367" s="36"/>
       <c r="H367" s="59" t="s">
-        <v>1176</v>
+        <v>1171</v>
       </c>
       <c r="I367" s="11" t="s">
         <v>824</v>
@@ -18963,7 +18941,7 @@
       <c r="F368" s="36"/>
       <c r="G368" s="36"/>
       <c r="H368" s="59" t="s">
-        <v>1176</v>
+        <v>1171</v>
       </c>
       <c r="I368" s="11" t="s">
         <v>824</v>
@@ -19003,7 +18981,7 @@
       <c r="F369" s="36"/>
       <c r="G369" s="36"/>
       <c r="H369" s="59" t="s">
-        <v>1176</v>
+        <v>1171</v>
       </c>
       <c r="I369" s="11" t="s">
         <v>824</v>
@@ -19041,7 +19019,7 @@
       <c r="F370" s="36"/>
       <c r="G370" s="36"/>
       <c r="H370" s="59" t="s">
-        <v>1176</v>
+        <v>1171</v>
       </c>
       <c r="I370" s="11" t="s">
         <v>824</v>
@@ -19084,7 +19062,7 @@
       <c r="F371" s="36"/>
       <c r="G371" s="36"/>
       <c r="H371" s="59" t="s">
-        <v>1176</v>
+        <v>1171</v>
       </c>
       <c r="I371" s="11" t="s">
         <v>824</v>
@@ -19122,7 +19100,7 @@
       <c r="F372" s="36"/>
       <c r="G372" s="36"/>
       <c r="H372" s="59" t="s">
-        <v>1176</v>
+        <v>1171</v>
       </c>
       <c r="I372" s="11" t="s">
         <v>824</v>
@@ -19255,7 +19233,7 @@
         <v>89</v>
       </c>
       <c r="N375" s="48" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="O375" s="9" t="s">
         <v>0</v>
@@ -19406,7 +19384,7 @@
         <v>93</v>
       </c>
       <c r="N379" s="48" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="O379" s="9" t="s">
         <v>0</v>
@@ -21451,7 +21429,7 @@
       <c r="D435" s="42"/>
       <c r="E435" s="36"/>
       <c r="F435" s="59" t="s">
-        <v>1203</v>
+        <v>1198</v>
       </c>
       <c r="G435" s="36"/>
       <c r="H435" s="36"/>
@@ -21494,7 +21472,7 @@
       <c r="D436" s="42"/>
       <c r="E436" s="36"/>
       <c r="F436" s="59" t="s">
-        <v>1203</v>
+        <v>1198</v>
       </c>
       <c r="G436" s="36"/>
       <c r="H436" s="36"/>
@@ -22655,7 +22633,7 @@
       <c r="F467" s="36"/>
       <c r="G467" s="36"/>
       <c r="H467" s="59" t="s">
-        <v>1177</v>
+        <v>1172</v>
       </c>
       <c r="I467" s="11" t="s">
         <v>826</v>
@@ -22695,7 +22673,7 @@
       <c r="F468" s="36"/>
       <c r="G468" s="36"/>
       <c r="H468" s="59" t="s">
-        <v>1177</v>
+        <v>1172</v>
       </c>
       <c r="I468" s="11" t="s">
         <v>826</v>
@@ -22734,7 +22712,7 @@
       <c r="F469" s="36"/>
       <c r="G469" s="36"/>
       <c r="H469" s="59" t="s">
-        <v>1177</v>
+        <v>1172</v>
       </c>
       <c r="I469" s="11" t="s">
         <v>826</v>
@@ -22772,7 +22750,7 @@
       <c r="F470" s="36"/>
       <c r="G470" s="36"/>
       <c r="H470" s="59" t="s">
-        <v>1177</v>
+        <v>1172</v>
       </c>
       <c r="I470" s="11" t="s">
         <v>826</v>
@@ -22815,7 +22793,7 @@
       <c r="F471" s="36"/>
       <c r="G471" s="36"/>
       <c r="H471" s="59" t="s">
-        <v>1177</v>
+        <v>1172</v>
       </c>
       <c r="I471" s="11" t="s">
         <v>826</v>
@@ -22853,7 +22831,7 @@
       <c r="F472" s="36"/>
       <c r="G472" s="36"/>
       <c r="H472" s="59" t="s">
-        <v>1177</v>
+        <v>1172</v>
       </c>
       <c r="I472" s="11" t="s">
         <v>826</v>
@@ -26014,7 +25992,7 @@
       <c r="F557" s="36"/>
       <c r="G557" s="36"/>
       <c r="H557" s="59" t="s">
-        <v>1178</v>
+        <v>1173</v>
       </c>
       <c r="I557" s="11" t="s">
         <v>827</v>
@@ -26053,7 +26031,7 @@
       <c r="F558" s="36"/>
       <c r="G558" s="36"/>
       <c r="H558" s="59" t="s">
-        <v>1178</v>
+        <v>1173</v>
       </c>
       <c r="I558" s="11" t="s">
         <v>827</v>
@@ -26096,7 +26074,7 @@
       <c r="F559" s="36"/>
       <c r="G559" s="36"/>
       <c r="H559" s="59" t="s">
-        <v>1178</v>
+        <v>1173</v>
       </c>
       <c r="I559" s="11" t="s">
         <v>827</v>
@@ -26136,7 +26114,7 @@
       <c r="F560" s="36"/>
       <c r="G560" s="36"/>
       <c r="H560" s="59" t="s">
-        <v>1178</v>
+        <v>1173</v>
       </c>
       <c r="I560" s="11" t="s">
         <v>827</v>
@@ -26323,7 +26301,7 @@
     </row>
     <row r="565" spans="4:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D565" s="60" t="s">
-        <v>1214</v>
+        <v>1208</v>
       </c>
       <c r="E565" s="36"/>
       <c r="F565" s="36"/>
@@ -28055,7 +28033,7 @@
       <c r="F611" s="36"/>
       <c r="G611" s="36"/>
       <c r="H611" s="59" t="s">
-        <v>1145</v>
+        <v>1141</v>
       </c>
       <c r="I611" s="11" t="s">
         <v>828</v>
@@ -28089,13 +28067,13 @@
     </row>
     <row r="612" spans="4:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D612" s="52" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="E612" s="36"/>
       <c r="F612" s="36"/>
       <c r="G612" s="36"/>
       <c r="H612" s="59" t="s">
-        <v>1145</v>
+        <v>1141</v>
       </c>
       <c r="I612" s="11" t="s">
         <v>828</v>
@@ -28133,7 +28111,7 @@
       <c r="F613" s="36"/>
       <c r="G613" s="36"/>
       <c r="H613" s="55" t="s">
-        <v>1145</v>
+        <v>1141</v>
       </c>
       <c r="I613" s="11" t="s">
         <v>828</v>
@@ -28175,7 +28153,7 @@
       <c r="F614" s="36"/>
       <c r="G614" s="36"/>
       <c r="H614" s="59" t="s">
-        <v>1145</v>
+        <v>1141</v>
       </c>
       <c r="I614" s="11" t="s">
         <v>828</v>
@@ -28849,7 +28827,7 @@
         <v>72</v>
       </c>
       <c r="N632" s="20" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="O632" s="23"/>
       <c r="P632" s="24" t="s">
@@ -29433,7 +29411,7 @@
       <c r="F648" s="36"/>
       <c r="G648" s="36"/>
       <c r="H648" s="59" t="s">
-        <v>1179</v>
+        <v>1174</v>
       </c>
       <c r="I648" s="11" t="s">
         <v>829</v>
@@ -29471,7 +29449,7 @@
       <c r="F649" s="36"/>
       <c r="G649" s="36"/>
       <c r="H649" s="59" t="s">
-        <v>1179</v>
+        <v>1174</v>
       </c>
       <c r="I649" s="11" t="s">
         <v>829</v>
@@ -29509,7 +29487,7 @@
       <c r="F650" s="36"/>
       <c r="G650" s="36"/>
       <c r="H650" s="59" t="s">
-        <v>1179</v>
+        <v>1174</v>
       </c>
       <c r="I650" s="11" t="s">
         <v>829</v>
@@ -29547,7 +29525,7 @@
       <c r="F651" s="36"/>
       <c r="G651" s="36"/>
       <c r="H651" s="59" t="s">
-        <v>1179</v>
+        <v>1174</v>
       </c>
       <c r="I651" s="11" t="s">
         <v>829</v>
@@ -29590,7 +29568,7 @@
       <c r="F652" s="36"/>
       <c r="G652" s="36"/>
       <c r="H652" s="59" t="s">
-        <v>1179</v>
+        <v>1174</v>
       </c>
       <c r="I652" s="11" t="s">
         <v>829</v>
@@ -29628,7 +29606,7 @@
       <c r="F653" s="36"/>
       <c r="G653" s="36"/>
       <c r="H653" s="59" t="s">
-        <v>1179</v>
+        <v>1174</v>
       </c>
       <c r="I653" s="11" t="s">
         <v>829</v>
@@ -32389,7 +32367,7 @@
       <c r="F730" s="36"/>
       <c r="G730" s="36"/>
       <c r="H730" s="59" t="s">
-        <v>1180</v>
+        <v>1175</v>
       </c>
       <c r="I730" s="11" t="s">
         <v>830</v>
@@ -32426,7 +32404,7 @@
       <c r="F731" s="36"/>
       <c r="G731" s="36"/>
       <c r="H731" s="59" t="s">
-        <v>1180</v>
+        <v>1175</v>
       </c>
       <c r="I731" s="11" t="s">
         <v>830</v>
@@ -32463,7 +32441,7 @@
       <c r="F732" s="36"/>
       <c r="G732" s="36"/>
       <c r="H732" s="59" t="s">
-        <v>1180</v>
+        <v>1175</v>
       </c>
       <c r="I732" s="11" t="s">
         <v>830</v>
@@ -32500,7 +32478,7 @@
       <c r="F733" s="36"/>
       <c r="G733" s="36"/>
       <c r="H733" s="59" t="s">
-        <v>1180</v>
+        <v>1175</v>
       </c>
       <c r="I733" s="11" t="s">
         <v>831</v>
@@ -32537,7 +32515,7 @@
       <c r="F734" s="36"/>
       <c r="G734" s="36"/>
       <c r="H734" s="59" t="s">
-        <v>1180</v>
+        <v>1175</v>
       </c>
       <c r="I734" s="11" t="s">
         <v>831</v>
@@ -32574,7 +32552,7 @@
       <c r="F735" s="36"/>
       <c r="G735" s="36"/>
       <c r="H735" s="59" t="s">
-        <v>1180</v>
+        <v>1175</v>
       </c>
       <c r="I735" s="11" t="s">
         <v>831</v>
@@ -33457,7 +33435,7 @@
       <c r="F760" s="36"/>
       <c r="G760" s="36"/>
       <c r="H760" s="59" t="s">
-        <v>1181</v>
+        <v>1176</v>
       </c>
       <c r="I760" s="11" t="s">
         <v>831</v>
@@ -33494,7 +33472,7 @@
       <c r="F761" s="36"/>
       <c r="G761" s="36"/>
       <c r="H761" s="59" t="s">
-        <v>1181</v>
+        <v>1176</v>
       </c>
       <c r="I761" s="11" t="s">
         <v>831</v>
@@ -33531,7 +33509,7 @@
       <c r="F762" s="36"/>
       <c r="G762" s="36"/>
       <c r="H762" s="59" t="s">
-        <v>1181</v>
+        <v>1176</v>
       </c>
       <c r="I762" s="11" t="s">
         <v>831</v>
@@ -33568,7 +33546,7 @@
       <c r="F763" s="36"/>
       <c r="G763" s="36"/>
       <c r="H763" s="59" t="s">
-        <v>1181</v>
+        <v>1176</v>
       </c>
       <c r="I763" s="11" t="s">
         <v>831</v>
@@ -33605,7 +33583,7 @@
       <c r="F764" s="36"/>
       <c r="G764" s="36"/>
       <c r="H764" s="59" t="s">
-        <v>1181</v>
+        <v>1176</v>
       </c>
       <c r="I764" s="11" t="s">
         <v>831</v>
@@ -33642,7 +33620,7 @@
       <c r="F765" s="36"/>
       <c r="G765" s="36"/>
       <c r="H765" s="59" t="s">
-        <v>1181</v>
+        <v>1176</v>
       </c>
       <c r="I765" s="11" t="s">
         <v>831</v>
@@ -33856,7 +33834,7 @@
       <c r="S770" s="9"/>
       <c r="T770" s="9"/>
       <c r="U770" s="9" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="V770" s="9"/>
       <c r="W770" s="9"/>
@@ -33904,7 +33882,7 @@
     <row r="772" spans="5:24" x14ac:dyDescent="0.25">
       <c r="E772" s="36"/>
       <c r="F772" s="59" t="s">
-        <v>1206</v>
+        <v>1201</v>
       </c>
       <c r="G772" s="36"/>
       <c r="H772" s="36"/>
@@ -33943,7 +33921,7 @@
     <row r="773" spans="5:24" x14ac:dyDescent="0.25">
       <c r="E773" s="36"/>
       <c r="F773" s="59" t="s">
-        <v>1206</v>
+        <v>1201</v>
       </c>
       <c r="G773" s="36"/>
       <c r="H773" s="36"/>
@@ -34299,7 +34277,7 @@
       <c r="V782" s="9"/>
       <c r="W782" s="9"/>
       <c r="X782" s="18" t="s">
-        <v>1215</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="783" spans="5:24" x14ac:dyDescent="0.25">
@@ -34599,7 +34577,7 @@
     </row>
     <row r="791" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D791" s="9" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="E791" s="36"/>
       <c r="F791" s="36"/>
@@ -34699,7 +34677,7 @@
         <v>161</v>
       </c>
       <c r="N793" s="34" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="O793" s="8"/>
       <c r="P793" s="9" t="s">
@@ -34975,7 +34953,7 @@
       <c r="F801" s="36"/>
       <c r="G801" s="36"/>
       <c r="H801" s="55" t="s">
-        <v>1146</v>
+        <v>1142</v>
       </c>
       <c r="I801" s="11" t="s">
         <v>832</v>
@@ -35002,7 +34980,7 @@
       <c r="Q801" s="9"/>
       <c r="R801" s="9"/>
       <c r="S801" s="9" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="T801" s="9"/>
       <c r="U801" s="9"/>
@@ -35014,7 +34992,7 @@
       <c r="F802" s="36"/>
       <c r="G802" s="36"/>
       <c r="H802" s="55" t="s">
-        <v>1146</v>
+        <v>1142</v>
       </c>
       <c r="I802" s="11" t="s">
         <v>832</v>
@@ -35053,7 +35031,7 @@
       <c r="F803" s="36"/>
       <c r="G803" s="36"/>
       <c r="H803" s="55" t="s">
-        <v>1146</v>
+        <v>1142</v>
       </c>
       <c r="I803" s="11" t="s">
         <v>832</v>
@@ -35080,7 +35058,7 @@
       <c r="Q803" s="9"/>
       <c r="R803" s="9"/>
       <c r="S803" s="9" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="T803" s="9"/>
       <c r="U803" s="9"/>
@@ -36642,7 +36620,7 @@
       <c r="F846" s="36"/>
       <c r="G846" s="36"/>
       <c r="H846" s="55" t="s">
-        <v>1147</v>
+        <v>1143</v>
       </c>
       <c r="I846" s="11" t="s">
         <v>833</v>
@@ -36681,13 +36659,13 @@
     </row>
     <row r="847" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D847" s="51" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="E847" s="36"/>
       <c r="F847" s="36"/>
       <c r="G847" s="36"/>
       <c r="H847" s="55" t="s">
-        <v>1147</v>
+        <v>1143</v>
       </c>
       <c r="I847" s="11" t="s">
         <v>833</v>
@@ -36726,7 +36704,7 @@
       <c r="F848" s="36"/>
       <c r="G848" s="36"/>
       <c r="H848" s="55" t="s">
-        <v>1147</v>
+        <v>1143</v>
       </c>
       <c r="I848" s="11" t="s">
         <v>833</v>
@@ -36867,7 +36845,7 @@
       <c r="Q851" s="9"/>
       <c r="R851" s="9"/>
       <c r="S851" s="9" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="T851" s="9"/>
       <c r="U851" s="9"/>
@@ -37707,7 +37685,7 @@
     </row>
     <row r="875" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D875" s="60" t="s">
-        <v>1197</v>
+        <v>1192</v>
       </c>
       <c r="E875" s="36"/>
       <c r="F875" s="36"/>
@@ -37742,9 +37720,7 @@
       <c r="S875" s="9" t="s">
         <v>1127</v>
       </c>
-      <c r="T875" s="9" t="s">
-        <v>1213</v>
-      </c>
+      <c r="T875" s="9"/>
       <c r="U875" s="9"/>
       <c r="V875" s="9"/>
       <c r="W875" s="9"/>
@@ -38678,7 +38654,7 @@
       <c r="F902" s="36"/>
       <c r="G902" s="36"/>
       <c r="H902" s="59" t="s">
-        <v>1182</v>
+        <v>1177</v>
       </c>
       <c r="I902" s="11" t="s">
         <v>834</v>
@@ -38715,7 +38691,7 @@
       <c r="F903" s="36"/>
       <c r="G903" s="36"/>
       <c r="H903" s="59" t="s">
-        <v>1182</v>
+        <v>1177</v>
       </c>
       <c r="I903" s="11" t="s">
         <v>834</v>
@@ -38754,7 +38730,7 @@
       <c r="F904" s="36"/>
       <c r="G904" s="36"/>
       <c r="H904" s="59" t="s">
-        <v>1182</v>
+        <v>1177</v>
       </c>
       <c r="I904" s="11" t="s">
         <v>834</v>
@@ -38791,7 +38767,7 @@
       <c r="F905" s="36"/>
       <c r="G905" s="36"/>
       <c r="H905" s="59" t="s">
-        <v>1182</v>
+        <v>1177</v>
       </c>
       <c r="I905" s="11" t="s">
         <v>834</v>
@@ -38833,7 +38809,7 @@
       <c r="F906" s="36"/>
       <c r="G906" s="36"/>
       <c r="H906" s="59" t="s">
-        <v>1182</v>
+        <v>1177</v>
       </c>
       <c r="I906" s="11" t="s">
         <v>834</v>
@@ -38870,7 +38846,7 @@
       <c r="F907" s="36"/>
       <c r="G907" s="36"/>
       <c r="H907" s="59" t="s">
-        <v>1182</v>
+        <v>1177</v>
       </c>
       <c r="I907" s="11" t="s">
         <v>834</v>
@@ -38907,7 +38883,7 @@
       <c r="F908" s="36"/>
       <c r="G908" s="36"/>
       <c r="H908" s="59" t="s">
-        <v>1182</v>
+        <v>1177</v>
       </c>
       <c r="I908" s="11" t="s">
         <v>834</v>
@@ -38944,7 +38920,7 @@
       <c r="F909" s="36"/>
       <c r="G909" s="36"/>
       <c r="H909" s="59" t="s">
-        <v>1182</v>
+        <v>1177</v>
       </c>
       <c r="I909" s="11" t="s">
         <v>834</v>
@@ -38972,11 +38948,11 @@
       <c r="P909" s="9"/>
       <c r="Q909" s="9"/>
       <c r="R909" s="9"/>
-      <c r="S909" s="57" t="s">
-        <v>1140</v>
-      </c>
-      <c r="T909" s="14" t="s">
-        <v>1157</v>
+      <c r="S909" s="9" t="s">
+        <v>1215</v>
+      </c>
+      <c r="T909" s="57" t="s">
+        <v>1047</v>
       </c>
       <c r="U909" s="9"/>
       <c r="V909" s="9"/>
@@ -38987,7 +38963,7 @@
       <c r="F910" s="36"/>
       <c r="G910" s="36"/>
       <c r="H910" s="59" t="s">
-        <v>1182</v>
+        <v>1177</v>
       </c>
       <c r="I910" s="11" t="s">
         <v>834</v>
@@ -39024,7 +39000,7 @@
       <c r="F911" s="36"/>
       <c r="G911" s="36"/>
       <c r="H911" s="59" t="s">
-        <v>1182</v>
+        <v>1177</v>
       </c>
       <c r="I911" s="11" t="s">
         <v>834</v>
@@ -39061,7 +39037,7 @@
       <c r="F912" s="36"/>
       <c r="G912" s="36"/>
       <c r="H912" s="59" t="s">
-        <v>1182</v>
+        <v>1177</v>
       </c>
       <c r="I912" s="11" t="s">
         <v>834</v>
@@ -39098,7 +39074,7 @@
       <c r="F913" s="36"/>
       <c r="G913" s="36"/>
       <c r="H913" s="59" t="s">
-        <v>1182</v>
+        <v>1177</v>
       </c>
       <c r="I913" s="11" t="s">
         <v>834</v>
@@ -40772,7 +40748,7 @@
         <v>166</v>
       </c>
       <c r="N959" s="50" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="O959" s="8"/>
       <c r="P959" s="9" t="s">
@@ -41653,7 +41629,7 @@
       <c r="F984" s="36"/>
       <c r="G984" s="36"/>
       <c r="H984" s="59" t="s">
-        <v>1183</v>
+        <v>1178</v>
       </c>
       <c r="I984" s="11" t="s">
         <v>835</v>
@@ -41690,7 +41666,7 @@
       <c r="F985" s="36"/>
       <c r="G985" s="36"/>
       <c r="H985" s="59" t="s">
-        <v>1183</v>
+        <v>1178</v>
       </c>
       <c r="I985" s="11" t="s">
         <v>835</v>
@@ -41727,7 +41703,7 @@
       <c r="F986" s="36"/>
       <c r="G986" s="36"/>
       <c r="H986" s="59" t="s">
-        <v>1183</v>
+        <v>1178</v>
       </c>
       <c r="I986" s="11" t="s">
         <v>835</v>
@@ -41769,7 +41745,7 @@
       <c r="F987" s="36"/>
       <c r="G987" s="36"/>
       <c r="H987" s="59" t="s">
-        <v>1183</v>
+        <v>1178</v>
       </c>
       <c r="I987" s="11" t="s">
         <v>835</v>
@@ -41806,7 +41782,7 @@
       <c r="F988" s="36"/>
       <c r="G988" s="36"/>
       <c r="H988" s="59" t="s">
-        <v>1183</v>
+        <v>1178</v>
       </c>
       <c r="I988" s="11" t="s">
         <v>835</v>
@@ -42348,7 +42324,7 @@
       <c r="F1003" s="36"/>
       <c r="G1003" s="36"/>
       <c r="H1003" s="55" t="s">
-        <v>1148</v>
+        <v>1144</v>
       </c>
       <c r="I1003" s="11" t="s">
         <v>835</v>
@@ -42382,17 +42358,17 @@
     </row>
     <row r="1004" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D1004" s="60" t="s">
-        <v>1201</v>
+        <v>1196</v>
       </c>
       <c r="E1004" s="36"/>
       <c r="F1004" s="59" t="s">
-        <v>1202</v>
+        <v>1197</v>
       </c>
       <c r="G1004" s="59" t="s">
-        <v>1208</v>
+        <v>1203</v>
       </c>
       <c r="H1004" s="55" t="s">
-        <v>1148</v>
+        <v>1144</v>
       </c>
       <c r="I1004" s="11" t="s">
         <v>835</v>
@@ -42431,17 +42407,17 @@
     </row>
     <row r="1005" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D1005" s="60" t="s">
-        <v>1201</v>
+        <v>1196</v>
       </c>
       <c r="E1005" s="36"/>
       <c r="F1005" s="59" t="s">
-        <v>1202</v>
+        <v>1197</v>
       </c>
       <c r="G1005" s="59" t="s">
-        <v>1208</v>
+        <v>1203</v>
       </c>
       <c r="H1005" s="55" t="s">
-        <v>1148</v>
+        <v>1144</v>
       </c>
       <c r="I1005" s="11" t="s">
         <v>835</v>
@@ -42468,11 +42444,9 @@
       <c r="Q1005" s="9"/>
       <c r="R1005" s="9"/>
       <c r="S1005" s="9" t="s">
-        <v>1128</v>
-      </c>
-      <c r="T1005" s="9" t="s">
-        <v>1157</v>
-      </c>
+        <v>1127</v>
+      </c>
+      <c r="T1005" s="9"/>
       <c r="U1005" s="9"/>
       <c r="V1005" s="9"/>
       <c r="W1005" s="9"/>
@@ -42482,7 +42456,7 @@
       <c r="F1006" s="36"/>
       <c r="G1006" s="36"/>
       <c r="H1006" s="55" t="s">
-        <v>1148</v>
+        <v>1144</v>
       </c>
       <c r="I1006" s="11" t="s">
         <v>835</v>
@@ -42659,7 +42633,7 @@
       <c r="F1011" s="36"/>
       <c r="G1011" s="36"/>
       <c r="H1011" s="55" t="s">
-        <v>1148</v>
+        <v>1144</v>
       </c>
       <c r="I1011" s="11" t="s">
         <v>836</v>
@@ -42693,17 +42667,17 @@
     </row>
     <row r="1012" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D1012" s="60" t="s">
-        <v>1201</v>
+        <v>1196</v>
       </c>
       <c r="E1012" s="36"/>
       <c r="F1012" s="59" t="s">
-        <v>1202</v>
+        <v>1197</v>
       </c>
       <c r="G1012" s="59" t="s">
-        <v>1208</v>
+        <v>1203</v>
       </c>
       <c r="H1012" s="55" t="s">
-        <v>1148</v>
+        <v>1144</v>
       </c>
       <c r="I1012" s="11" t="s">
         <v>836</v>
@@ -42742,17 +42716,17 @@
     </row>
     <row r="1013" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D1013" s="60" t="s">
-        <v>1201</v>
+        <v>1196</v>
       </c>
       <c r="E1013" s="36"/>
       <c r="F1013" s="59" t="s">
-        <v>1202</v>
+        <v>1197</v>
       </c>
       <c r="G1013" s="59" t="s">
-        <v>1208</v>
+        <v>1203</v>
       </c>
       <c r="H1013" s="55" t="s">
-        <v>1148</v>
+        <v>1144</v>
       </c>
       <c r="I1013" s="11" t="s">
         <v>836</v>
@@ -42781,9 +42755,7 @@
       <c r="S1013" s="9" t="s">
         <v>1127</v>
       </c>
-      <c r="T1013" s="9" t="s">
-        <v>1157</v>
-      </c>
+      <c r="T1013" s="9"/>
       <c r="U1013" s="9"/>
       <c r="V1013" s="9"/>
       <c r="W1013" s="9"/>
@@ -42793,7 +42765,7 @@
       <c r="F1014" s="36"/>
       <c r="G1014" s="36"/>
       <c r="H1014" s="55" t="s">
-        <v>1148</v>
+        <v>1144</v>
       </c>
       <c r="I1014" s="11" t="s">
         <v>836</v>
@@ -43087,7 +43059,7 @@
       <c r="F1022" s="36"/>
       <c r="G1022" s="36"/>
       <c r="H1022" s="55" t="s">
-        <v>1148</v>
+        <v>1144</v>
       </c>
       <c r="I1022" s="11" t="s">
         <v>836</v>
@@ -43121,17 +43093,17 @@
     </row>
     <row r="1023" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D1023" s="60" t="s">
-        <v>1201</v>
+        <v>1196</v>
       </c>
       <c r="E1023" s="36"/>
       <c r="F1023" s="59" t="s">
-        <v>1202</v>
+        <v>1197</v>
       </c>
       <c r="G1023" s="59" t="s">
-        <v>1208</v>
+        <v>1203</v>
       </c>
       <c r="H1023" s="55" t="s">
-        <v>1148</v>
+        <v>1144</v>
       </c>
       <c r="I1023" s="11" t="s">
         <v>836</v>
@@ -43170,17 +43142,17 @@
     </row>
     <row r="1024" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D1024" s="60" t="s">
-        <v>1201</v>
+        <v>1196</v>
       </c>
       <c r="E1024" s="36"/>
       <c r="F1024" s="59" t="s">
-        <v>1202</v>
+        <v>1197</v>
       </c>
       <c r="G1024" s="59" t="s">
-        <v>1208</v>
+        <v>1203</v>
       </c>
       <c r="H1024" s="55" t="s">
-        <v>1148</v>
+        <v>1144</v>
       </c>
       <c r="I1024" s="11" t="s">
         <v>836</v>
@@ -43209,9 +43181,7 @@
       <c r="S1024" s="9" t="s">
         <v>1127</v>
       </c>
-      <c r="T1024" s="9" t="s">
-        <v>1157</v>
-      </c>
+      <c r="T1024" s="9"/>
       <c r="U1024" s="9"/>
       <c r="V1024" s="9"/>
       <c r="W1024" s="9"/>
@@ -43221,7 +43191,7 @@
       <c r="F1025" s="36"/>
       <c r="G1025" s="36"/>
       <c r="H1025" s="55" t="s">
-        <v>1148</v>
+        <v>1144</v>
       </c>
       <c r="I1025" s="11" t="s">
         <v>836</v>
@@ -43730,7 +43700,7 @@
       <c r="F1039" s="36"/>
       <c r="G1039" s="36"/>
       <c r="H1039" s="59" t="s">
-        <v>1149</v>
+        <v>1145</v>
       </c>
       <c r="I1039" s="11" t="s">
         <v>836</v>
@@ -43767,7 +43737,7 @@
       <c r="F1040" s="36"/>
       <c r="G1040" s="36"/>
       <c r="H1040" s="59" t="s">
-        <v>1149</v>
+        <v>1145</v>
       </c>
       <c r="I1040" s="11" t="s">
         <v>836</v>
@@ -43804,7 +43774,7 @@
       <c r="F1041" s="36"/>
       <c r="G1041" s="36"/>
       <c r="H1041" s="55" t="s">
-        <v>1149</v>
+        <v>1145</v>
       </c>
       <c r="I1041" s="11" t="s">
         <v>836</v>
@@ -43833,7 +43803,7 @@
       <c r="S1041" s="9"/>
       <c r="T1041" s="9"/>
       <c r="U1041" s="9" t="s">
-        <v>1139</v>
+        <v>1136</v>
       </c>
       <c r="V1041" s="9"/>
       <c r="W1041" s="9"/>
@@ -43843,7 +43813,7 @@
       <c r="F1042" s="36"/>
       <c r="G1042" s="36"/>
       <c r="H1042" s="59" t="s">
-        <v>1149</v>
+        <v>1145</v>
       </c>
       <c r="I1042" s="11" t="s">
         <v>836</v>
@@ -45205,7 +45175,7 @@
     </row>
     <row r="1080" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D1080" s="60" t="s">
-        <v>1197</v>
+        <v>1192</v>
       </c>
       <c r="E1080" s="36"/>
       <c r="F1080" s="36"/>
@@ -45238,9 +45208,7 @@
       <c r="S1080" s="9" t="s">
         <v>1127</v>
       </c>
-      <c r="T1080" s="9" t="s">
-        <v>1213</v>
-      </c>
+      <c r="T1080" s="9"/>
       <c r="U1080" s="9"/>
       <c r="V1080" s="9"/>
       <c r="W1080" s="9"/>
@@ -45325,7 +45293,7 @@
       <c r="F1083" s="36"/>
       <c r="G1083" s="36"/>
       <c r="H1083" s="59" t="s">
-        <v>1184</v>
+        <v>1179</v>
       </c>
       <c r="I1083" s="11" t="s">
         <v>837</v>
@@ -45362,7 +45330,7 @@
       <c r="F1084" s="36"/>
       <c r="G1084" s="36"/>
       <c r="H1084" s="59" t="s">
-        <v>1184</v>
+        <v>1179</v>
       </c>
       <c r="I1084" s="11" t="s">
         <v>837</v>
@@ -45401,7 +45369,7 @@
       <c r="F1085" s="36"/>
       <c r="G1085" s="36"/>
       <c r="H1085" s="59" t="s">
-        <v>1184</v>
+        <v>1179</v>
       </c>
       <c r="I1085" s="11" t="s">
         <v>837</v>
@@ -45438,7 +45406,7 @@
       <c r="F1086" s="36"/>
       <c r="G1086" s="36"/>
       <c r="H1086" s="59" t="s">
-        <v>1184</v>
+        <v>1179</v>
       </c>
       <c r="I1086" s="11" t="s">
         <v>837</v>
@@ -45475,7 +45443,7 @@
       <c r="F1087" s="36"/>
       <c r="G1087" s="36"/>
       <c r="H1087" s="59" t="s">
-        <v>1184</v>
+        <v>1179</v>
       </c>
       <c r="I1087" s="11" t="s">
         <v>837</v>
@@ -45512,7 +45480,7 @@
       <c r="F1088" s="36"/>
       <c r="G1088" s="36"/>
       <c r="H1088" s="59" t="s">
-        <v>1184</v>
+        <v>1179</v>
       </c>
       <c r="I1088" s="11" t="s">
         <v>837</v>
@@ -45549,7 +45517,7 @@
       <c r="F1089" s="36"/>
       <c r="G1089" s="36"/>
       <c r="H1089" s="59" t="s">
-        <v>1184</v>
+        <v>1179</v>
       </c>
       <c r="I1089" s="11" t="s">
         <v>837</v>
@@ -45591,7 +45559,7 @@
       <c r="F1090" s="36"/>
       <c r="G1090" s="36"/>
       <c r="H1090" s="59" t="s">
-        <v>1184</v>
+        <v>1179</v>
       </c>
       <c r="I1090" s="11" t="s">
         <v>837</v>
@@ -45633,7 +45601,7 @@
       <c r="F1091" s="36"/>
       <c r="G1091" s="36"/>
       <c r="H1091" s="59" t="s">
-        <v>1184</v>
+        <v>1179</v>
       </c>
       <c r="I1091" s="11" t="s">
         <v>837</v>
@@ -45672,7 +45640,7 @@
       <c r="F1092" s="36"/>
       <c r="G1092" s="36"/>
       <c r="H1092" s="59" t="s">
-        <v>1184</v>
+        <v>1179</v>
       </c>
       <c r="I1092" s="11" t="s">
         <v>837</v>
@@ -45709,7 +45677,7 @@
       <c r="F1093" s="36"/>
       <c r="G1093" s="36"/>
       <c r="H1093" s="59" t="s">
-        <v>1184</v>
+        <v>1179</v>
       </c>
       <c r="I1093" s="11" t="s">
         <v>837</v>
@@ -45891,7 +45859,7 @@
       <c r="F1098" s="36"/>
       <c r="G1098" s="36"/>
       <c r="H1098" s="59" t="s">
-        <v>1185</v>
+        <v>1180</v>
       </c>
       <c r="I1098" s="11" t="s">
         <v>837</v>
@@ -45935,7 +45903,7 @@
       <c r="F1099" s="36"/>
       <c r="G1099" s="36"/>
       <c r="H1099" s="59" t="s">
-        <v>1185</v>
+        <v>1180</v>
       </c>
       <c r="I1099" s="11" t="s">
         <v>837</v>
@@ -45972,7 +45940,7 @@
       <c r="F1100" s="36"/>
       <c r="G1100" s="36"/>
       <c r="H1100" s="59" t="s">
-        <v>1185</v>
+        <v>1180</v>
       </c>
       <c r="I1100" s="11" t="s">
         <v>837</v>
@@ -46009,7 +45977,7 @@
       <c r="F1101" s="36"/>
       <c r="G1101" s="36"/>
       <c r="H1101" s="59" t="s">
-        <v>1185</v>
+        <v>1180</v>
       </c>
       <c r="I1101" s="11" t="s">
         <v>837</v>
@@ -46048,7 +46016,7 @@
       <c r="F1102" s="36"/>
       <c r="G1102" s="36"/>
       <c r="H1102" s="59" t="s">
-        <v>1185</v>
+        <v>1180</v>
       </c>
       <c r="I1102" s="11" t="s">
         <v>837</v>
@@ -46085,7 +46053,7 @@
       <c r="F1103" s="36"/>
       <c r="G1103" s="36"/>
       <c r="H1103" s="59" t="s">
-        <v>1185</v>
+        <v>1180</v>
       </c>
       <c r="I1103" s="11" t="s">
         <v>837</v>
@@ -46124,7 +46092,7 @@
       <c r="F1104" s="36"/>
       <c r="G1104" s="36"/>
       <c r="H1104" s="59" t="s">
-        <v>1185</v>
+        <v>1180</v>
       </c>
       <c r="I1104" s="11" t="s">
         <v>837</v>
@@ -46161,7 +46129,7 @@
       <c r="F1105" s="36"/>
       <c r="G1105" s="36"/>
       <c r="H1105" s="59" t="s">
-        <v>1185</v>
+        <v>1180</v>
       </c>
       <c r="I1105" s="11" t="s">
         <v>837</v>
@@ -46198,7 +46166,7 @@
       <c r="F1106" s="36"/>
       <c r="G1106" s="36"/>
       <c r="H1106" s="59" t="s">
-        <v>1185</v>
+        <v>1180</v>
       </c>
       <c r="I1106" s="11" t="s">
         <v>837</v>
@@ -46235,7 +46203,7 @@
       <c r="F1107" s="36"/>
       <c r="G1107" s="36"/>
       <c r="H1107" s="59" t="s">
-        <v>1185</v>
+        <v>1180</v>
       </c>
       <c r="I1107" s="11" t="s">
         <v>837</v>
@@ -46272,7 +46240,7 @@
       <c r="F1108" s="36"/>
       <c r="G1108" s="36"/>
       <c r="H1108" s="59" t="s">
-        <v>1185</v>
+        <v>1180</v>
       </c>
       <c r="I1108" s="11" t="s">
         <v>837</v>
@@ -46741,7 +46709,7 @@
       <c r="F1121" s="36"/>
       <c r="G1121" s="36"/>
       <c r="H1121" s="55" t="s">
-        <v>1150</v>
+        <v>1146</v>
       </c>
       <c r="I1121" s="11" t="s">
         <v>837</v>
@@ -46778,7 +46746,7 @@
       <c r="F1122" s="36"/>
       <c r="G1122" s="36"/>
       <c r="H1122" s="55" t="s">
-        <v>1150</v>
+        <v>1146</v>
       </c>
       <c r="I1122" s="11" t="s">
         <v>837</v>
@@ -46807,7 +46775,7 @@
       <c r="S1122" s="9"/>
       <c r="T1122" s="9"/>
       <c r="U1122" s="9" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="V1122" s="9"/>
       <c r="W1122" s="9"/>
@@ -46817,7 +46785,7 @@
       <c r="F1123" s="36"/>
       <c r="G1123" s="36"/>
       <c r="H1123" s="55" t="s">
-        <v>1150</v>
+        <v>1146</v>
       </c>
       <c r="I1123" s="11" t="s">
         <v>837</v>
@@ -47219,7 +47187,7 @@
       <c r="F1134" s="36"/>
       <c r="G1134" s="36"/>
       <c r="H1134" s="59" t="s">
-        <v>1186</v>
+        <v>1181</v>
       </c>
       <c r="I1134" s="11" t="s">
         <v>837</v>
@@ -47261,7 +47229,7 @@
       <c r="F1135" s="36"/>
       <c r="G1135" s="36"/>
       <c r="H1135" s="59" t="s">
-        <v>1186</v>
+        <v>1181</v>
       </c>
       <c r="I1135" s="11" t="s">
         <v>837</v>
@@ -47300,7 +47268,7 @@
       <c r="F1136" s="36"/>
       <c r="G1136" s="36"/>
       <c r="H1136" s="59" t="s">
-        <v>1186</v>
+        <v>1181</v>
       </c>
       <c r="I1136" s="11" t="s">
         <v>837</v>
@@ -47337,7 +47305,7 @@
       <c r="F1137" s="36"/>
       <c r="G1137" s="36"/>
       <c r="H1137" s="59" t="s">
-        <v>1186</v>
+        <v>1181</v>
       </c>
       <c r="I1137" s="11" t="s">
         <v>837</v>
@@ -47379,7 +47347,7 @@
       <c r="F1138" s="36"/>
       <c r="G1138" s="36"/>
       <c r="H1138" s="59" t="s">
-        <v>1186</v>
+        <v>1181</v>
       </c>
       <c r="I1138" s="11" t="s">
         <v>837</v>
@@ -47777,7 +47745,7 @@
       <c r="F1149" s="36"/>
       <c r="G1149" s="36"/>
       <c r="H1149" s="55" t="s">
-        <v>1151</v>
+        <v>1147</v>
       </c>
       <c r="I1149" s="11" t="s">
         <v>838</v>
@@ -47819,7 +47787,7 @@
       <c r="F1150" s="36"/>
       <c r="G1150" s="36"/>
       <c r="H1150" s="55" t="s">
-        <v>1151</v>
+        <v>1147</v>
       </c>
       <c r="I1150" s="11" t="s">
         <v>838</v>
@@ -47858,7 +47826,7 @@
       <c r="F1151" s="36"/>
       <c r="G1151" s="36"/>
       <c r="H1151" s="55" t="s">
-        <v>1151</v>
+        <v>1147</v>
       </c>
       <c r="I1151" s="11" t="s">
         <v>838</v>
@@ -47900,7 +47868,7 @@
       <c r="F1152" s="36"/>
       <c r="G1152" s="36"/>
       <c r="H1152" s="55" t="s">
-        <v>1151</v>
+        <v>1147</v>
       </c>
       <c r="I1152" s="11" t="s">
         <v>838</v>
@@ -47939,7 +47907,7 @@
       <c r="F1153" s="36"/>
       <c r="G1153" s="36"/>
       <c r="H1153" s="55" t="s">
-        <v>1151</v>
+        <v>1147</v>
       </c>
       <c r="I1153" s="11" t="s">
         <v>838</v>
@@ -47966,11 +47934,11 @@
       <c r="Q1153" s="9"/>
       <c r="R1153" s="9"/>
       <c r="S1153" s="9" t="s">
-        <v>1158</v>
+        <v>1153</v>
       </c>
       <c r="T1153" s="9"/>
       <c r="V1153" s="9" t="s">
-        <v>1137</v>
+        <v>1216</v>
       </c>
       <c r="W1153" s="9"/>
     </row>
@@ -47979,7 +47947,7 @@
       <c r="F1154" s="36"/>
       <c r="G1154" s="36"/>
       <c r="H1154" s="55" t="s">
-        <v>1151</v>
+        <v>1147</v>
       </c>
       <c r="I1154" s="11" t="s">
         <v>838</v>
@@ -48016,7 +47984,7 @@
       <c r="F1155" s="36"/>
       <c r="G1155" s="36"/>
       <c r="H1155" s="55" t="s">
-        <v>1151</v>
+        <v>1147</v>
       </c>
       <c r="I1155" s="11" t="s">
         <v>838</v>
@@ -48053,7 +48021,7 @@
       <c r="F1156" s="36"/>
       <c r="G1156" s="36"/>
       <c r="H1156" s="55" t="s">
-        <v>1151</v>
+        <v>1147</v>
       </c>
       <c r="I1156" s="11" t="s">
         <v>838</v>
@@ -48095,7 +48063,7 @@
       <c r="F1157" s="36"/>
       <c r="G1157" s="36"/>
       <c r="H1157" s="55" t="s">
-        <v>1151</v>
+        <v>1147</v>
       </c>
       <c r="I1157" s="11" t="s">
         <v>838</v>
@@ -48122,11 +48090,11 @@
       <c r="Q1157" s="9"/>
       <c r="R1157" s="9"/>
       <c r="S1157" s="9" t="s">
-        <v>1158</v>
+        <v>1153</v>
       </c>
       <c r="T1157" s="9"/>
       <c r="V1157" s="9" t="s">
-        <v>1138</v>
+        <v>1217</v>
       </c>
       <c r="W1157" s="9"/>
     </row>
@@ -48135,7 +48103,7 @@
       <c r="F1158" s="36"/>
       <c r="G1158" s="36"/>
       <c r="H1158" s="55" t="s">
-        <v>1151</v>
+        <v>1147</v>
       </c>
       <c r="I1158" s="11" t="s">
         <v>838</v>
@@ -48439,7 +48407,7 @@
       <c r="F1166" s="36"/>
       <c r="G1166" s="36"/>
       <c r="H1166" s="55" t="s">
-        <v>1152</v>
+        <v>1148</v>
       </c>
       <c r="I1166" s="11" t="s">
         <v>838</v>
@@ -48477,7 +48445,7 @@
       <c r="F1167" s="36"/>
       <c r="G1167" s="36"/>
       <c r="H1167" s="55" t="s">
-        <v>1152</v>
+        <v>1148</v>
       </c>
       <c r="I1167" s="11" t="s">
         <v>838</v>
@@ -48514,7 +48482,7 @@
       <c r="F1168" s="36"/>
       <c r="G1168" s="36"/>
       <c r="H1168" s="55" t="s">
-        <v>1152</v>
+        <v>1148</v>
       </c>
       <c r="I1168" s="11" t="s">
         <v>838</v>
@@ -50716,7 +50684,7 @@
       <c r="F1229" s="36"/>
       <c r="G1229" s="36"/>
       <c r="H1229" s="59" t="s">
-        <v>1187</v>
+        <v>1182</v>
       </c>
       <c r="I1229" s="11" t="s">
         <v>839</v>
@@ -50753,7 +50721,7 @@
       <c r="F1230" s="36"/>
       <c r="G1230" s="36"/>
       <c r="H1230" s="59" t="s">
-        <v>1187</v>
+        <v>1182</v>
       </c>
       <c r="I1230" s="11" t="s">
         <v>839</v>
@@ -50790,7 +50758,7 @@
       <c r="F1231" s="36"/>
       <c r="G1231" s="36"/>
       <c r="H1231" s="59" t="s">
-        <v>1187</v>
+        <v>1182</v>
       </c>
       <c r="I1231" s="11" t="s">
         <v>839</v>
@@ -50827,7 +50795,7 @@
       <c r="F1232" s="36"/>
       <c r="G1232" s="36"/>
       <c r="H1232" s="59" t="s">
-        <v>1187</v>
+        <v>1182</v>
       </c>
       <c r="I1232" s="11" t="s">
         <v>839</v>
@@ -50864,7 +50832,7 @@
       <c r="F1233" s="36"/>
       <c r="G1233" s="36"/>
       <c r="H1233" s="59" t="s">
-        <v>1187</v>
+        <v>1182</v>
       </c>
       <c r="I1233" s="11" t="s">
         <v>839</v>
@@ -52165,7 +52133,7 @@
       <c r="F1269" s="36"/>
       <c r="G1269" s="36"/>
       <c r="H1269" s="55" t="s">
-        <v>1153</v>
+        <v>1149</v>
       </c>
       <c r="I1269" s="11" t="s">
         <v>840</v>
@@ -52199,12 +52167,12 @@
     </row>
     <row r="1270" spans="5:24" x14ac:dyDescent="0.25">
       <c r="E1270" s="59" t="s">
-        <v>1199</v>
+        <v>1194</v>
       </c>
       <c r="F1270" s="36"/>
       <c r="G1270" s="36"/>
       <c r="H1270" s="55" t="s">
-        <v>1153</v>
+        <v>1149</v>
       </c>
       <c r="I1270" s="11" t="s">
         <v>840</v>
@@ -52235,7 +52203,7 @@
       <c r="S1270" s="9"/>
       <c r="T1270" s="9"/>
       <c r="U1270" s="9" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="V1270" s="9"/>
       <c r="W1270" s="9"/>
@@ -52245,12 +52213,12 @@
     </row>
     <row r="1271" spans="5:24" x14ac:dyDescent="0.25">
       <c r="E1271" s="59" t="s">
-        <v>1199</v>
+        <v>1194</v>
       </c>
       <c r="F1271" s="36"/>
       <c r="G1271" s="36"/>
       <c r="H1271" s="55" t="s">
-        <v>1153</v>
+        <v>1149</v>
       </c>
       <c r="I1271" s="11" t="s">
         <v>840</v>
@@ -53226,9 +53194,7 @@
       <c r="S1297" s="9" t="s">
         <v>1127</v>
       </c>
-      <c r="T1297" s="9" t="s">
-        <v>1217</v>
-      </c>
+      <c r="T1297" s="9"/>
       <c r="U1297" s="9"/>
       <c r="V1297" s="9"/>
       <c r="W1297" s="9"/>
@@ -53626,11 +53592,11 @@
     <row r="1309" spans="5:24" x14ac:dyDescent="0.25">
       <c r="E1309" s="36"/>
       <c r="F1309" s="59" t="s">
-        <v>1205</v>
+        <v>1200</v>
       </c>
       <c r="G1309" s="36"/>
       <c r="H1309" s="59" t="s">
-        <v>1188</v>
+        <v>1183</v>
       </c>
       <c r="I1309" s="11" t="s">
         <v>841</v>
@@ -53664,11 +53630,11 @@
     <row r="1310" spans="5:24" x14ac:dyDescent="0.25">
       <c r="E1310" s="36"/>
       <c r="F1310" s="59" t="s">
-        <v>1205</v>
+        <v>1200</v>
       </c>
       <c r="G1310" s="36"/>
       <c r="H1310" s="59" t="s">
-        <v>1188</v>
+        <v>1183</v>
       </c>
       <c r="I1310" s="11" t="s">
         <v>841</v>
@@ -53703,11 +53669,11 @@
     <row r="1311" spans="5:24" x14ac:dyDescent="0.25">
       <c r="E1311" s="36"/>
       <c r="F1311" s="59" t="s">
-        <v>1205</v>
+        <v>1200</v>
       </c>
       <c r="G1311" s="36"/>
       <c r="H1311" s="59" t="s">
-        <v>1188</v>
+        <v>1183</v>
       </c>
       <c r="I1311" s="11" t="s">
         <v>841</v>
@@ -53729,10 +53695,10 @@
       <c r="N1311" s="5" t="s">
         <v>1006</v>
       </c>
-      <c r="O1311" s="9" t="s">
+      <c r="O1311" s="57" t="s">
         <v>917</v>
       </c>
-      <c r="P1311" s="9"/>
+      <c r="P1311" s="57"/>
       <c r="Q1311" s="9"/>
       <c r="R1311" s="9"/>
       <c r="S1311" s="9"/>
@@ -53769,8 +53735,8 @@
       <c r="N1312" s="26" t="s">
         <v>671</v>
       </c>
-      <c r="O1312" s="8"/>
-      <c r="P1312" s="9"/>
+      <c r="O1312" s="63"/>
+      <c r="P1312" s="57"/>
       <c r="Q1312" s="9"/>
       <c r="R1312" s="9"/>
       <c r="S1312" s="9"/>
@@ -54249,7 +54215,7 @@
       <c r="F1326" s="36"/>
       <c r="G1326" s="36"/>
       <c r="H1326" s="59" t="s">
-        <v>1189</v>
+        <v>1184</v>
       </c>
       <c r="I1326" s="11" t="s">
         <v>841</v>
@@ -54286,7 +54252,7 @@
       <c r="F1327" s="36"/>
       <c r="G1327" s="36"/>
       <c r="H1327" s="59" t="s">
-        <v>1189</v>
+        <v>1184</v>
       </c>
       <c r="I1327" s="11" t="s">
         <v>841</v>
@@ -54323,7 +54289,7 @@
       <c r="F1328" s="36"/>
       <c r="G1328" s="36"/>
       <c r="H1328" s="59" t="s">
-        <v>1189</v>
+        <v>1184</v>
       </c>
       <c r="I1328" s="11" t="s">
         <v>841</v>
@@ -54365,7 +54331,7 @@
       <c r="F1329" s="36"/>
       <c r="G1329" s="36"/>
       <c r="H1329" s="59" t="s">
-        <v>1189</v>
+        <v>1184</v>
       </c>
       <c r="I1329" s="11" t="s">
         <v>841</v>
@@ -54402,7 +54368,7 @@
       <c r="F1330" s="36"/>
       <c r="G1330" s="36"/>
       <c r="H1330" s="59" t="s">
-        <v>1189</v>
+        <v>1184</v>
       </c>
       <c r="I1330" s="11" t="s">
         <v>841</v>
@@ -54444,7 +54410,7 @@
       <c r="F1331" s="36"/>
       <c r="G1331" s="36"/>
       <c r="H1331" s="59" t="s">
-        <v>1189</v>
+        <v>1184</v>
       </c>
       <c r="I1331" s="11" t="s">
         <v>841</v>
@@ -54481,7 +54447,7 @@
       <c r="F1332" s="36"/>
       <c r="G1332" s="36"/>
       <c r="H1332" s="59" t="s">
-        <v>1189</v>
+        <v>1184</v>
       </c>
       <c r="I1332" s="11" t="s">
         <v>841</v>
@@ -54518,7 +54484,7 @@
       <c r="F1333" s="36"/>
       <c r="G1333" s="36"/>
       <c r="H1333" s="59" t="s">
-        <v>1189</v>
+        <v>1184</v>
       </c>
       <c r="I1333" s="11" t="s">
         <v>841</v>
@@ -54556,7 +54522,7 @@
       <c r="F1334" s="36"/>
       <c r="G1334" s="36"/>
       <c r="H1334" s="59" t="s">
-        <v>1189</v>
+        <v>1184</v>
       </c>
       <c r="I1334" s="11" t="s">
         <v>841</v>
@@ -54589,7 +54555,7 @@
       <c r="V1334" s="9"/>
       <c r="W1334" s="9"/>
       <c r="X1334" s="61" t="s">
-        <v>1218</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="1335" spans="5:24" x14ac:dyDescent="0.25">
@@ -55498,7 +55464,7 @@
       <c r="F1359" s="36"/>
       <c r="G1359" s="36"/>
       <c r="H1359" s="59" t="s">
-        <v>1190</v>
+        <v>1185</v>
       </c>
       <c r="I1359" s="11" t="s">
         <v>842</v>
@@ -55535,7 +55501,7 @@
       <c r="F1360" s="36"/>
       <c r="G1360" s="36"/>
       <c r="H1360" s="59" t="s">
-        <v>1190</v>
+        <v>1185</v>
       </c>
       <c r="I1360" s="11" t="s">
         <v>842</v>
@@ -55572,7 +55538,7 @@
       <c r="F1361" s="36"/>
       <c r="G1361" s="36"/>
       <c r="H1361" s="59" t="s">
-        <v>1190</v>
+        <v>1185</v>
       </c>
       <c r="I1361" s="11" t="s">
         <v>842</v>
@@ -55609,7 +55575,7 @@
       <c r="F1362" s="36"/>
       <c r="G1362" s="36"/>
       <c r="H1362" s="59" t="s">
-        <v>1190</v>
+        <v>1185</v>
       </c>
       <c r="I1362" s="11" t="s">
         <v>842</v>
@@ -55651,7 +55617,7 @@
       <c r="F1363" s="36"/>
       <c r="G1363" s="36"/>
       <c r="H1363" s="59" t="s">
-        <v>1190</v>
+        <v>1185</v>
       </c>
       <c r="I1363" s="11" t="s">
         <v>842</v>
@@ -55868,7 +55834,7 @@
       <c r="F1369" s="36"/>
       <c r="G1369" s="36"/>
       <c r="H1369" s="59" t="s">
-        <v>1191</v>
+        <v>1186</v>
       </c>
       <c r="I1369" s="11" t="s">
         <v>842</v>
@@ -55905,7 +55871,7 @@
       <c r="F1370" s="36"/>
       <c r="G1370" s="36"/>
       <c r="H1370" s="59" t="s">
-        <v>1191</v>
+        <v>1186</v>
       </c>
       <c r="I1370" s="11" t="s">
         <v>842</v>
@@ -55942,7 +55908,7 @@
       <c r="F1371" s="36"/>
       <c r="G1371" s="36"/>
       <c r="H1371" s="59" t="s">
-        <v>1191</v>
+        <v>1186</v>
       </c>
       <c r="I1371" s="11" t="s">
         <v>842</v>
@@ -55969,9 +55935,9 @@
       <c r="Q1371" s="9"/>
       <c r="R1371" s="9"/>
       <c r="S1371" s="9" t="s">
-        <v>1159</v>
-      </c>
-      <c r="T1371" s="14"/>
+        <v>1154</v>
+      </c>
+      <c r="T1371" s="9"/>
       <c r="U1371" s="9"/>
       <c r="V1371" s="9"/>
       <c r="W1371" s="9"/>
@@ -55981,7 +55947,7 @@
       <c r="F1372" s="36"/>
       <c r="G1372" s="36"/>
       <c r="H1372" s="59" t="s">
-        <v>1191</v>
+        <v>1186</v>
       </c>
       <c r="I1372" s="11" t="s">
         <v>842</v>
@@ -56010,9 +55976,7 @@
       <c r="S1372" s="9" t="s">
         <v>1127</v>
       </c>
-      <c r="T1372" s="9" t="s">
-        <v>1219</v>
-      </c>
+      <c r="T1372" s="9"/>
       <c r="U1372" s="9"/>
       <c r="V1372" s="9"/>
       <c r="W1372" s="9"/>
@@ -56022,7 +55986,7 @@
       <c r="F1373" s="36"/>
       <c r="G1373" s="36"/>
       <c r="H1373" s="59" t="s">
-        <v>1191</v>
+        <v>1186</v>
       </c>
       <c r="I1373" s="11" t="s">
         <v>842</v>
@@ -56059,7 +56023,7 @@
       <c r="F1374" s="36"/>
       <c r="G1374" s="36"/>
       <c r="H1374" s="59" t="s">
-        <v>1191</v>
+        <v>1186</v>
       </c>
       <c r="I1374" s="11" t="s">
         <v>842</v>
@@ -56283,7 +56247,7 @@
       <c r="F1380" s="36"/>
       <c r="G1380" s="36"/>
       <c r="H1380" s="59" t="s">
-        <v>1192</v>
+        <v>1187</v>
       </c>
       <c r="I1380" s="11" t="s">
         <v>842</v>
@@ -56325,7 +56289,7 @@
       <c r="F1381" s="36"/>
       <c r="G1381" s="36"/>
       <c r="H1381" s="59" t="s">
-        <v>1192</v>
+        <v>1187</v>
       </c>
       <c r="I1381" s="11" t="s">
         <v>842</v>
@@ -56367,7 +56331,7 @@
       <c r="F1382" s="36"/>
       <c r="G1382" s="36"/>
       <c r="H1382" s="59" t="s">
-        <v>1192</v>
+        <v>1187</v>
       </c>
       <c r="I1382" s="11" t="s">
         <v>842</v>
@@ -56404,7 +56368,7 @@
       <c r="F1383" s="36"/>
       <c r="G1383" s="36"/>
       <c r="H1383" s="59" t="s">
-        <v>1192</v>
+        <v>1187</v>
       </c>
       <c r="I1383" s="11" t="s">
         <v>842</v>
@@ -56441,7 +56405,7 @@
       <c r="F1384" s="36"/>
       <c r="G1384" s="36"/>
       <c r="H1384" s="59" t="s">
-        <v>1192</v>
+        <v>1187</v>
       </c>
       <c r="I1384" s="11" t="s">
         <v>842</v>
@@ -57139,7 +57103,7 @@
       <c r="F1403" s="36"/>
       <c r="G1403" s="36"/>
       <c r="H1403" s="59" t="s">
-        <v>1193</v>
+        <v>1188</v>
       </c>
       <c r="I1403" s="11" t="s">
         <v>842</v>
@@ -57176,7 +57140,7 @@
       <c r="F1404" s="36"/>
       <c r="G1404" s="36"/>
       <c r="H1404" s="59" t="s">
-        <v>1193</v>
+        <v>1188</v>
       </c>
       <c r="I1404" s="11" t="s">
         <v>842</v>
@@ -57213,7 +57177,7 @@
       <c r="F1405" s="36"/>
       <c r="G1405" s="36"/>
       <c r="H1405" s="59" t="s">
-        <v>1193</v>
+        <v>1188</v>
       </c>
       <c r="I1405" s="11" t="s">
         <v>842</v>
@@ -57250,7 +57214,7 @@
       <c r="F1406" s="36"/>
       <c r="G1406" s="36"/>
       <c r="H1406" s="59" t="s">
-        <v>1193</v>
+        <v>1188</v>
       </c>
       <c r="I1406" s="11" t="s">
         <v>842</v>
@@ -57289,7 +57253,7 @@
       <c r="F1407" s="36"/>
       <c r="G1407" s="36"/>
       <c r="H1407" s="59" t="s">
-        <v>1193</v>
+        <v>1188</v>
       </c>
       <c r="I1407" s="11" t="s">
         <v>842</v>
@@ -57326,7 +57290,7 @@
       <c r="F1408" s="36"/>
       <c r="G1408" s="36"/>
       <c r="H1408" s="59" t="s">
-        <v>1193</v>
+        <v>1188</v>
       </c>
       <c r="I1408" s="11" t="s">
         <v>842</v>
@@ -59177,10 +59141,10 @@
       <c r="E1459" s="36"/>
       <c r="F1459" s="36"/>
       <c r="G1459" s="59" t="s">
-        <v>1209</v>
+        <v>1204</v>
       </c>
       <c r="H1459" s="59" t="s">
-        <v>1194</v>
+        <v>1189</v>
       </c>
       <c r="I1459" s="11" t="s">
         <v>844</v>
@@ -59207,7 +59171,7 @@
       <c r="Q1459" s="9"/>
       <c r="R1459" s="9"/>
       <c r="S1459" s="9" t="s">
-        <v>1160</v>
+        <v>1155</v>
       </c>
       <c r="T1459" s="9"/>
       <c r="U1459" s="9"/>
@@ -59218,10 +59182,10 @@
       <c r="E1460" s="36"/>
       <c r="F1460" s="36"/>
       <c r="G1460" s="59" t="s">
-        <v>1209</v>
+        <v>1204</v>
       </c>
       <c r="H1460" s="59" t="s">
-        <v>1194</v>
+        <v>1189</v>
       </c>
       <c r="I1460" s="11" t="s">
         <v>844</v>
@@ -59255,14 +59219,14 @@
     </row>
     <row r="1461" spans="5:24" x14ac:dyDescent="0.25">
       <c r="E1461" s="59" t="s">
-        <v>1198</v>
+        <v>1193</v>
       </c>
       <c r="F1461" s="36"/>
       <c r="G1461" s="59" t="s">
-        <v>1209</v>
+        <v>1204</v>
       </c>
       <c r="H1461" s="59" t="s">
-        <v>1194</v>
+        <v>1189</v>
       </c>
       <c r="I1461" s="11" t="s">
         <v>844</v>
@@ -59289,21 +59253,21 @@
       <c r="Q1461" s="9"/>
       <c r="R1461" s="9"/>
       <c r="S1461" s="9" t="s">
-        <v>1159</v>
-      </c>
-      <c r="T1461" s="14"/>
+        <v>1154</v>
+      </c>
+      <c r="T1461" s="9"/>
       <c r="U1461" s="9"/>
       <c r="V1461" s="9"/>
       <c r="W1461" s="9"/>
     </row>
     <row r="1462" spans="5:24" x14ac:dyDescent="0.25">
       <c r="E1462" s="59" t="s">
-        <v>1198</v>
+        <v>1193</v>
       </c>
       <c r="F1462" s="36"/>
       <c r="G1462" s="36"/>
       <c r="H1462" s="59" t="s">
-        <v>1194</v>
+        <v>1189</v>
       </c>
       <c r="I1462" s="11" t="s">
         <v>844</v>
@@ -59330,9 +59294,9 @@
       <c r="Q1462" s="9"/>
       <c r="R1462" s="9"/>
       <c r="S1462" s="9" t="s">
-        <v>1159</v>
-      </c>
-      <c r="T1462" s="14"/>
+        <v>1154</v>
+      </c>
+      <c r="T1462" s="9"/>
       <c r="U1462" s="9"/>
       <c r="V1462" s="9"/>
       <c r="W1462" s="9"/>
@@ -59342,7 +59306,7 @@
       <c r="F1463" s="36"/>
       <c r="G1463" s="36"/>
       <c r="H1463" s="59" t="s">
-        <v>1194</v>
+        <v>1189</v>
       </c>
       <c r="I1463" s="11" t="s">
         <v>844</v>
@@ -59406,7 +59370,7 @@
       <c r="S1464" s="9"/>
       <c r="T1464" s="9"/>
       <c r="U1464" s="9" t="s">
-        <v>1220</v>
+        <v>1211</v>
       </c>
       <c r="V1464" s="9"/>
       <c r="W1464" s="9"/>
@@ -59780,7 +59744,7 @@
       <c r="F1475" s="36"/>
       <c r="G1475" s="36"/>
       <c r="H1475" s="59" t="s">
-        <v>1154</v>
+        <v>1150</v>
       </c>
       <c r="I1475" s="11" t="s">
         <v>844</v>
@@ -59817,7 +59781,7 @@
       <c r="F1476" s="36"/>
       <c r="G1476" s="36"/>
       <c r="H1476" s="59" t="s">
-        <v>1154</v>
+        <v>1150</v>
       </c>
       <c r="I1476" s="11" t="s">
         <v>844</v>
@@ -59854,7 +59818,7 @@
       <c r="F1477" s="36"/>
       <c r="G1477" s="36"/>
       <c r="H1477" s="59" t="s">
-        <v>1154</v>
+        <v>1150</v>
       </c>
       <c r="I1477" s="11" t="s">
         <v>844</v>
@@ -59891,7 +59855,7 @@
       <c r="F1478" s="36"/>
       <c r="G1478" s="36"/>
       <c r="H1478" s="59" t="s">
-        <v>1154</v>
+        <v>1150</v>
       </c>
       <c r="I1478" s="11" t="s">
         <v>844</v>
@@ -59928,7 +59892,7 @@
       <c r="F1479" s="36"/>
       <c r="G1479" s="36"/>
       <c r="H1479" s="59" t="s">
-        <v>1154</v>
+        <v>1150</v>
       </c>
       <c r="I1479" s="11" t="s">
         <v>844</v>
@@ -59965,7 +59929,7 @@
       <c r="F1480" s="36"/>
       <c r="G1480" s="36"/>
       <c r="H1480" s="59" t="s">
-        <v>1154</v>
+        <v>1150</v>
       </c>
       <c r="I1480" s="11" t="s">
         <v>844</v>
@@ -60076,7 +60040,7 @@
     </row>
     <row r="1483" spans="5:24" x14ac:dyDescent="0.25">
       <c r="E1483" s="59" t="s">
-        <v>1200</v>
+        <v>1195</v>
       </c>
       <c r="F1483" s="36"/>
       <c r="G1483" s="36"/>
@@ -60113,7 +60077,7 @@
     </row>
     <row r="1484" spans="5:24" x14ac:dyDescent="0.25">
       <c r="E1484" s="59" t="s">
-        <v>1200</v>
+        <v>1195</v>
       </c>
       <c r="F1484" s="36"/>
       <c r="G1484" s="36"/>
@@ -60807,7 +60771,7 @@
     <row r="1503" spans="5:24" x14ac:dyDescent="0.25">
       <c r="E1503" s="36"/>
       <c r="F1503" s="59" t="s">
-        <v>1204</v>
+        <v>1199</v>
       </c>
       <c r="G1503" s="36"/>
       <c r="H1503" s="36"/>
@@ -60844,7 +60808,7 @@
     <row r="1504" spans="5:24" x14ac:dyDescent="0.25">
       <c r="E1504" s="36"/>
       <c r="F1504" s="59" t="s">
-        <v>1204</v>
+        <v>1199</v>
       </c>
       <c r="G1504" s="36"/>
       <c r="H1504" s="36"/>
@@ -60952,7 +60916,7 @@
       <c r="S1506" s="9"/>
       <c r="T1506" s="9"/>
       <c r="U1506" s="9" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="V1506" s="9"/>
       <c r="W1506" s="9"/>
@@ -61213,14 +61177,14 @@
       <c r="V1513" s="9"/>
       <c r="W1513" s="9"/>
       <c r="X1513" s="61" t="s">
-        <v>1221</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="1514" spans="4:24" x14ac:dyDescent="0.25">
       <c r="E1514" s="36"/>
       <c r="F1514" s="36"/>
       <c r="G1514" s="59" t="s">
-        <v>1211</v>
+        <v>1206</v>
       </c>
       <c r="H1514" s="36"/>
       <c r="I1514" s="11" t="s">
@@ -61257,7 +61221,7 @@
       <c r="E1515" s="36"/>
       <c r="F1515" s="36"/>
       <c r="G1515" s="59" t="s">
-        <v>1211</v>
+        <v>1206</v>
       </c>
       <c r="H1515" s="36"/>
       <c r="I1515" s="11" t="s">
@@ -61294,7 +61258,7 @@
       <c r="E1516" s="36"/>
       <c r="F1516" s="36"/>
       <c r="G1516" s="59" t="s">
-        <v>1211</v>
+        <v>1206</v>
       </c>
       <c r="H1516" s="36"/>
       <c r="I1516" s="11" t="s">
@@ -61547,7 +61511,7 @@
       <c r="Q1522" s="9"/>
       <c r="R1522" s="9"/>
       <c r="S1522" s="9" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="T1522" s="9"/>
       <c r="U1522" s="9"/>
@@ -61796,12 +61760,12 @@
       <c r="Q1529" s="9"/>
       <c r="R1529" s="9"/>
       <c r="S1529" s="9" t="s">
-        <v>1216</v>
+        <v>1153</v>
       </c>
       <c r="T1529" s="9"/>
       <c r="U1529" s="9"/>
       <c r="V1529" s="9" t="s">
-        <v>1222</v>
+        <v>1215</v>
       </c>
       <c r="W1529" s="9"/>
     </row>

</xml_diff>

<commit_message>
Files changes Excel format+Rule processing 18/10/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Raja Files/Padam Inputs/TS 1.1 Padam Input Template.xlsx
+++ b/TS Jatai Working/Raja Files/Padam Inputs/TS 1.1 Padam Input Template.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4177" uniqueCount="1218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4192" uniqueCount="1230">
   <si>
     <t>PS</t>
   </si>
@@ -3677,10 +3677,46 @@
     <t>N</t>
   </si>
   <si>
-    <t>N+R</t>
-  </si>
-  <si>
     <t>N+S</t>
+  </si>
+  <si>
+    <t>P+N</t>
+  </si>
+  <si>
+    <t>P[r]+S[r]+n[r]</t>
+  </si>
+  <si>
+    <t>P[r]+S[H]+N[r]</t>
+  </si>
+  <si>
+    <t>P[Sh]+S[r]+N[Sh]</t>
+  </si>
+  <si>
+    <t>P[Sh]</t>
+  </si>
+  <si>
+    <t>P[r]+S[H]</t>
+  </si>
+  <si>
+    <t>N[N]</t>
+  </si>
+  <si>
+    <t>P[s]</t>
+  </si>
+  <si>
+    <t>P[r]+S[r]+N[r]</t>
+  </si>
+  <si>
+    <t>P[r]+S[r]</t>
+  </si>
+  <si>
+    <t>S+N</t>
+  </si>
+  <si>
+    <t>N[r]</t>
+  </si>
+  <si>
+    <t>S[s]+N[s]</t>
   </si>
 </sst>
 </file>
@@ -4315,10 +4351,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X1580"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="S1006" sqref="S1006"/>
+      <selection pane="bottomLeft" activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -4339,7 +4375,7 @@
     <col min="16" max="17" width="5.7109375" style="1" customWidth="1"/>
     <col min="18" max="18" width="6.28515625" style="1" customWidth="1"/>
     <col min="19" max="19" width="12.42578125" style="1" customWidth="1"/>
-    <col min="20" max="20" width="10" style="1" customWidth="1"/>
+    <col min="20" max="20" width="35.42578125" style="1" customWidth="1"/>
     <col min="21" max="22" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="11.7109375" style="1" hidden="1" customWidth="1"/>
     <col min="24" max="24" width="62.85546875" style="6" bestFit="1" customWidth="1"/>
@@ -10742,7 +10778,9 @@
       <c r="S150" s="9" t="s">
         <v>1127</v>
       </c>
-      <c r="T150" s="9"/>
+      <c r="T150" s="9" t="s">
+        <v>1218</v>
+      </c>
       <c r="U150" s="9"/>
       <c r="V150" s="9"/>
       <c r="W150" s="9"/>
@@ -13697,7 +13735,9 @@
       <c r="S228" s="9" t="s">
         <v>1127</v>
       </c>
-      <c r="T228" s="9"/>
+      <c r="T228" s="9" t="s">
+        <v>1218</v>
+      </c>
       <c r="U228" s="9"/>
       <c r="V228" s="9"/>
       <c r="W228" s="9"/>
@@ -15152,7 +15192,9 @@
       <c r="S267" s="9" t="s">
         <v>1127</v>
       </c>
-      <c r="T267" s="9"/>
+      <c r="T267" s="9" t="s">
+        <v>1219</v>
+      </c>
       <c r="U267" s="9"/>
       <c r="V267" s="9"/>
       <c r="W267" s="9"/>
@@ -34979,9 +35021,7 @@
       <c r="P801" s="9"/>
       <c r="Q801" s="9"/>
       <c r="R801" s="9"/>
-      <c r="S801" s="9" t="s">
-        <v>1131</v>
-      </c>
+      <c r="S801" s="9"/>
       <c r="T801" s="9"/>
       <c r="U801" s="9"/>
       <c r="V801" s="9"/>
@@ -35020,8 +35060,12 @@
       <c r="P802" s="9"/>
       <c r="Q802" s="9"/>
       <c r="R802" s="9"/>
-      <c r="S802" s="9"/>
-      <c r="T802" s="9"/>
+      <c r="S802" s="9" t="s">
+        <v>1131</v>
+      </c>
+      <c r="T802" s="9" t="s">
+        <v>1220</v>
+      </c>
       <c r="U802" s="9"/>
       <c r="V802" s="9"/>
       <c r="W802" s="9"/>
@@ -35057,9 +35101,7 @@
       <c r="P803" s="9"/>
       <c r="Q803" s="9"/>
       <c r="R803" s="9"/>
-      <c r="S803" s="9" t="s">
-        <v>1131</v>
-      </c>
+      <c r="S803" s="9"/>
       <c r="T803" s="9"/>
       <c r="U803" s="9"/>
       <c r="V803" s="9"/>
@@ -36847,7 +36889,9 @@
       <c r="S851" s="9" t="s">
         <v>1131</v>
       </c>
-      <c r="T851" s="9"/>
+      <c r="T851" s="9" t="s">
+        <v>1221</v>
+      </c>
       <c r="U851" s="9"/>
       <c r="V851" s="9"/>
       <c r="W851" s="9"/>
@@ -37720,7 +37764,9 @@
       <c r="S875" s="9" t="s">
         <v>1127</v>
       </c>
-      <c r="T875" s="9"/>
+      <c r="T875" s="9" t="s">
+        <v>1222</v>
+      </c>
       <c r="U875" s="9"/>
       <c r="V875" s="9"/>
       <c r="W875" s="9"/>
@@ -38952,7 +38998,7 @@
         <v>1215</v>
       </c>
       <c r="T909" s="57" t="s">
-        <v>1047</v>
+        <v>1223</v>
       </c>
       <c r="U909" s="9"/>
       <c r="V909" s="9"/>
@@ -42446,7 +42492,9 @@
       <c r="S1005" s="9" t="s">
         <v>1127</v>
       </c>
-      <c r="T1005" s="9"/>
+      <c r="T1005" s="9" t="s">
+        <v>1224</v>
+      </c>
       <c r="U1005" s="9"/>
       <c r="V1005" s="9"/>
       <c r="W1005" s="9"/>
@@ -42755,7 +42803,9 @@
       <c r="S1013" s="9" t="s">
         <v>1127</v>
       </c>
-      <c r="T1013" s="9"/>
+      <c r="T1013" s="9" t="s">
+        <v>1224</v>
+      </c>
       <c r="U1013" s="9"/>
       <c r="V1013" s="9"/>
       <c r="W1013" s="9"/>
@@ -43181,7 +43231,9 @@
       <c r="S1024" s="9" t="s">
         <v>1127</v>
       </c>
-      <c r="T1024" s="9"/>
+      <c r="T1024" s="9" t="s">
+        <v>1224</v>
+      </c>
       <c r="U1024" s="9"/>
       <c r="V1024" s="9"/>
       <c r="W1024" s="9"/>
@@ -45208,7 +45260,9 @@
       <c r="S1080" s="9" t="s">
         <v>1127</v>
       </c>
-      <c r="T1080" s="9"/>
+      <c r="T1080" s="9" t="s">
+        <v>1225</v>
+      </c>
       <c r="U1080" s="9"/>
       <c r="V1080" s="9"/>
       <c r="W1080" s="9"/>
@@ -47936,10 +47990,10 @@
       <c r="S1153" s="9" t="s">
         <v>1153</v>
       </c>
-      <c r="T1153" s="9"/>
-      <c r="V1153" s="9" t="s">
-        <v>1216</v>
-      </c>
+      <c r="T1153" s="9" t="s">
+        <v>1217</v>
+      </c>
+      <c r="V1153" s="9"/>
       <c r="W1153" s="9"/>
     </row>
     <row r="1154" spans="5:24" x14ac:dyDescent="0.25">
@@ -48092,9 +48146,11 @@
       <c r="S1157" s="9" t="s">
         <v>1153</v>
       </c>
-      <c r="T1157" s="9"/>
+      <c r="T1157" s="9" t="s">
+        <v>1227</v>
+      </c>
       <c r="V1157" s="9" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="W1157" s="9"/>
     </row>
@@ -48134,7 +48190,9 @@
       <c r="S1158" s="9" t="s">
         <v>1127</v>
       </c>
-      <c r="T1158" s="9"/>
+      <c r="T1158" s="9" t="s">
+        <v>1226</v>
+      </c>
       <c r="U1158" s="9"/>
       <c r="V1158" s="9"/>
       <c r="W1158" s="9"/>
@@ -53194,7 +53252,9 @@
       <c r="S1297" s="9" t="s">
         <v>1127</v>
       </c>
-      <c r="T1297" s="9"/>
+      <c r="T1297" s="9" t="s">
+        <v>1228</v>
+      </c>
       <c r="U1297" s="9"/>
       <c r="V1297" s="9"/>
       <c r="W1297" s="9"/>
@@ -55976,7 +56036,9 @@
       <c r="S1372" s="9" t="s">
         <v>1127</v>
       </c>
-      <c r="T1372" s="9"/>
+      <c r="T1372" s="9" t="s">
+        <v>1229</v>
+      </c>
       <c r="U1372" s="9"/>
       <c r="V1372" s="9"/>
       <c r="W1372" s="9"/>
@@ -61513,7 +61575,9 @@
       <c r="S1522" s="9" t="s">
         <v>1131</v>
       </c>
-      <c r="T1522" s="9"/>
+      <c r="T1522" s="9" t="s">
+        <v>1215</v>
+      </c>
       <c r="U1522" s="9"/>
       <c r="V1522" s="9"/>
       <c r="W1522" s="9"/>
@@ -61762,7 +61826,9 @@
       <c r="S1529" s="9" t="s">
         <v>1153</v>
       </c>
-      <c r="T1529" s="9"/>
+      <c r="T1529" s="9" t="s">
+        <v>1215</v>
+      </c>
       <c r="U1529" s="9"/>
       <c r="V1529" s="9" t="s">
         <v>1215</v>

</xml_diff>

<commit_message>
Changed Jatai files 23/10/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Raja Files/Padam Inputs/TS 1.1 Padam Input Template.xlsx
+++ b/TS Jatai Working/Raja Files/Padam Inputs/TS 1.1 Padam Input Template.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4191" uniqueCount="1229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4191" uniqueCount="1227">
   <si>
     <t>PS</t>
   </si>
@@ -3683,21 +3683,9 @@
     <t>P[r]+S[r]+n[r]</t>
   </si>
   <si>
-    <t>P[r]+S[H]+N[r]</t>
-  </si>
-  <si>
-    <t>P[Sh]+S[r]+N[Sh]</t>
-  </si>
-  <si>
     <t>P[Sh]</t>
   </si>
   <si>
-    <t>P[r]+S[H]</t>
-  </si>
-  <si>
-    <t>N[N]</t>
-  </si>
-  <si>
     <t>P[s]</t>
   </si>
   <si>
@@ -3710,10 +3698,16 @@
     <t>S+N</t>
   </si>
   <si>
-    <t>N[r]</t>
-  </si>
-  <si>
-    <t>S[s]+N[s]</t>
+    <t>P[r]+N[r]</t>
+  </si>
+  <si>
+    <t>P[Sh]+N[Sh]</t>
+  </si>
+  <si>
+    <t>P[r]</t>
+  </si>
+  <si>
+    <t>N[s]</t>
   </si>
 </sst>
 </file>
@@ -4351,7 +4345,7 @@
     <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="W3" sqref="W3"/>
+      <selection pane="bottomLeft" activeCell="T1373" sqref="T1373"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -14921,7 +14915,7 @@
         <v>1127</v>
       </c>
       <c r="T267" s="9" t="s">
-        <v>1218</v>
+        <v>1223</v>
       </c>
       <c r="U267" s="9"/>
       <c r="V267" s="9"/>
@@ -34257,7 +34251,7 @@
         <v>1131</v>
       </c>
       <c r="T802" s="9" t="s">
-        <v>1219</v>
+        <v>1224</v>
       </c>
       <c r="U802" s="9"/>
       <c r="V802" s="9"/>
@@ -36034,7 +36028,7 @@
         <v>1131</v>
       </c>
       <c r="T851" s="9" t="s">
-        <v>1220</v>
+        <v>1218</v>
       </c>
       <c r="U851" s="9"/>
       <c r="V851" s="9"/>
@@ -36885,7 +36879,7 @@
         <v>1127</v>
       </c>
       <c r="T875" s="9" t="s">
-        <v>1221</v>
+        <v>1225</v>
       </c>
       <c r="U875" s="9"/>
       <c r="V875" s="9"/>
@@ -38083,8 +38077,8 @@
       <c r="S909" s="9" t="s">
         <v>1214</v>
       </c>
-      <c r="T909" s="57" t="s">
-        <v>1222</v>
+      <c r="T909" s="9" t="s">
+        <v>1214</v>
       </c>
       <c r="U909" s="9"/>
       <c r="V909" s="9"/>
@@ -41483,7 +41477,7 @@
         <v>1127</v>
       </c>
       <c r="T1005" s="9" t="s">
-        <v>1223</v>
+        <v>1219</v>
       </c>
       <c r="U1005" s="9"/>
       <c r="V1005" s="9"/>
@@ -41786,7 +41780,7 @@
         <v>1127</v>
       </c>
       <c r="T1013" s="9" t="s">
-        <v>1223</v>
+        <v>1219</v>
       </c>
       <c r="U1013" s="9"/>
       <c r="V1013" s="9"/>
@@ -42203,7 +42197,7 @@
         <v>1127</v>
       </c>
       <c r="T1024" s="9" t="s">
-        <v>1223</v>
+        <v>1219</v>
       </c>
       <c r="U1024" s="9"/>
       <c r="V1024" s="9"/>
@@ -44176,7 +44170,7 @@
         <v>1127</v>
       </c>
       <c r="T1080" s="9" t="s">
-        <v>1224</v>
+        <v>1220</v>
       </c>
       <c r="U1080" s="9"/>
       <c r="V1080" s="9"/>
@@ -46985,7 +46979,7 @@
         <v>1153</v>
       </c>
       <c r="T1157" s="9" t="s">
-        <v>1226</v>
+        <v>1222</v>
       </c>
       <c r="V1157" s="9" t="s">
         <v>1215</v>
@@ -47028,7 +47022,7 @@
         <v>1127</v>
       </c>
       <c r="T1158" s="9" t="s">
-        <v>1225</v>
+        <v>1221</v>
       </c>
       <c r="U1158" s="9"/>
       <c r="V1158" s="9"/>
@@ -51951,7 +51945,7 @@
         <v>1127</v>
       </c>
       <c r="T1297" s="9" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="U1297" s="9"/>
       <c r="V1297" s="9"/>
@@ -54660,7 +54654,7 @@
         <v>1127</v>
       </c>
       <c r="T1372" s="9" t="s">
-        <v>1228</v>
+        <v>1226</v>
       </c>
       <c r="U1372" s="9"/>
       <c r="V1372" s="9"/>

</xml_diff>

<commit_message>
TS 3.1 Tamil PP and minor changes 30/10/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Raja Files/Padam Inputs/TS 1.1 Padam Input Template.xlsx
+++ b/TS Jatai Working/Raja Files/Padam Inputs/TS 1.1 Padam Input Template.xlsx
@@ -4334,10 +4334,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V1580"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="V2" sqref="V2"/>
+      <selection pane="bottomLeft" activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Corr for NiH TS 1.1 Template 30/10/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Raja Files/Padam Inputs/TS 1.1 Padam Input Template.xlsx
+++ b/TS Jatai Working/Raja Files/Padam Inputs/TS 1.1 Padam Input Template.xlsx
@@ -4334,10 +4334,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V1580"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="S6" sqref="S6"/>
+      <selection pane="bottomLeft" activeCell="V15" sqref="V15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -33469,7 +33469,7 @@
       <c r="Q802" s="9"/>
       <c r="R802" s="9"/>
       <c r="S802" s="9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="T802" s="9" t="s">
         <v>147</v>
@@ -58561,7 +58561,7 @@
       <c r="Q1522" s="9"/>
       <c r="R1522" s="9"/>
       <c r="S1522" s="9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="T1522" s="9" t="s">
         <v>138</v>

</xml_diff>

<commit_message>
TS Jatai Working changes 30/10/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Raja Files/Padam Inputs/TS 1.1 Padam Input Template.xlsx
+++ b/TS Jatai Working/Raja Files/Padam Inputs/TS 1.1 Padam Input Template.xlsx
@@ -3693,13 +3693,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -3858,199 +3864,205 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4334,10 +4346,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V1580"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="V15" sqref="V15"/>
+      <selection pane="bottomLeft" activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -4840,10 +4852,10 @@
       <c r="L1" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="17" t="s">
+      <c r="M1" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="12" t="s">
+      <c r="N1" s="70" t="s">
         <v>3</v>
       </c>
       <c r="O1" s="13" t="s">

</xml_diff>

<commit_message>
Padam Input Template changes 31/10/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Raja Files/Padam Inputs/TS 1.1 Padam Input Template.xlsx
+++ b/TS Jatai Working/Raja Files/Padam Inputs/TS 1.1 Padam Input Template.xlsx
@@ -4347,9 +4347,9 @@
   <dimension ref="A1:V1580"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A226" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="R3" sqref="R3"/>
+      <selection pane="bottomLeft" activeCell="T229" sqref="T229"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -13275,7 +13275,7 @@
         <v>59</v>
       </c>
       <c r="T228" s="9" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="U228" s="9"/>
     </row>

</xml_diff>

<commit_message>
Padam input and GS edit 05/12/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Raja Files/Padam Inputs/TS 1.1 Padam Input Template.xlsx
+++ b/TS Jatai Working/Raja Files/Padam Inputs/TS 1.1 Padam Input Template.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4226" uniqueCount="1226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4460" uniqueCount="1230">
   <si>
     <t>PS</t>
   </si>
@@ -3692,12 +3692,6 @@
     <t>N[Sh]</t>
   </si>
   <si>
-    <t>Vis,N</t>
-  </si>
-  <si>
-    <t>P[Sh]+N[Sh], S</t>
-  </si>
-  <si>
     <t>S</t>
   </si>
   <si>
@@ -3705,19 +3699,43 @@
   </si>
   <si>
     <t>P,N[v]</t>
+  </si>
+  <si>
+    <t>Vis%N</t>
+  </si>
+  <si>
+    <t>P[Sh]+N[Sh]%S</t>
+  </si>
+  <si>
+    <t>PS-6-5</t>
+  </si>
+  <si>
+    <t>PS-7-5</t>
+  </si>
+  <si>
+    <t>PS-9-22</t>
+  </si>
+  <si>
+    <t>alopa</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -3882,204 +3900,210 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="18" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4364,10 +4388,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V1580"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="S1372" sqref="S1372"/>
+      <selection pane="bottomLeft" activeCell="E1529" sqref="E1529"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -4901,7 +4925,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="2" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="11"/>
@@ -4939,7 +4963,7 @@
       <c r="U2" s="19"/>
       <c r="V2" s="29"/>
     </row>
-    <row r="3" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="11"/>
@@ -4979,7 +5003,7 @@
       <c r="U3" s="19"/>
       <c r="V3" s="29"/>
     </row>
-    <row r="4" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="11"/>
@@ -5019,7 +5043,7 @@
       <c r="U4" s="19"/>
       <c r="V4" s="29"/>
     </row>
-    <row r="5" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="11"/>
@@ -5059,7 +5083,7 @@
       <c r="U5" s="19"/>
       <c r="V5" s="29"/>
     </row>
-    <row r="6" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="6"/>
       <c r="C6" s="11"/>
@@ -5097,7 +5121,7 @@
       <c r="U6" s="19"/>
       <c r="V6" s="29"/>
     </row>
-    <row r="7" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="6"/>
       <c r="C7" s="11"/>
@@ -5135,7 +5159,7 @@
       <c r="U7" s="19"/>
       <c r="V7" s="29"/>
     </row>
-    <row r="8" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
       <c r="C8" s="11"/>
@@ -5177,7 +5201,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="9" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="11"/>
@@ -5215,7 +5239,7 @@
       <c r="U9" s="19"/>
       <c r="V9" s="29"/>
     </row>
-    <row r="10" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="11"/>
@@ -5253,7 +5277,7 @@
       <c r="U10" s="19"/>
       <c r="V10" s="29"/>
     </row>
-    <row r="11" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="11"/>
@@ -5291,7 +5315,7 @@
       <c r="U11" s="19"/>
       <c r="V11" s="29"/>
     </row>
-    <row r="12" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="11"/>
@@ -5329,7 +5353,7 @@
       <c r="U12" s="19"/>
       <c r="V12" s="29"/>
     </row>
-    <row r="13" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="11"/>
@@ -5368,7 +5392,7 @@
       <c r="U13" s="19"/>
       <c r="V13" s="29"/>
     </row>
-    <row r="14" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="6"/>
       <c r="C14" s="11"/>
@@ -5406,7 +5430,7 @@
       <c r="U14" s="19"/>
       <c r="V14" s="29"/>
     </row>
-    <row r="15" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="11"/>
@@ -5448,7 +5472,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="16" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="11"/>
@@ -5486,7 +5510,7 @@
       <c r="U16" s="19"/>
       <c r="V16" s="29"/>
     </row>
-    <row r="17" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="11"/>
@@ -5526,7 +5550,7 @@
       <c r="U17" s="19"/>
       <c r="V17" s="29"/>
     </row>
-    <row r="18" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="11"/>
@@ -5564,7 +5588,7 @@
       <c r="U18" s="19"/>
       <c r="V18" s="29"/>
     </row>
-    <row r="19" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="11"/>
@@ -5602,7 +5626,7 @@
       <c r="U19" s="19"/>
       <c r="V19" s="29"/>
     </row>
-    <row r="20" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="11"/>
@@ -5644,7 +5668,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="21" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="11"/>
@@ -5682,7 +5706,7 @@
       <c r="U21" s="19"/>
       <c r="V21" s="29"/>
     </row>
-    <row r="22" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
       <c r="B22" s="6"/>
       <c r="C22" s="11"/>
@@ -5720,7 +5744,7 @@
       <c r="U22" s="19"/>
       <c r="V22" s="29"/>
     </row>
-    <row r="23" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="11"/>
@@ -5762,7 +5786,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="24" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
       <c r="C24" s="11"/>
@@ -5800,7 +5824,7 @@
       <c r="U24" s="19"/>
       <c r="V24" s="29"/>
     </row>
-    <row r="25" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
       <c r="C25" s="11"/>
@@ -5838,7 +5862,7 @@
       <c r="U25" s="19"/>
       <c r="V25" s="29"/>
     </row>
-    <row r="26" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="6"/>
       <c r="C26" s="11"/>
@@ -5878,7 +5902,7 @@
       <c r="U26" s="19"/>
       <c r="V26" s="29"/>
     </row>
-    <row r="27" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
       <c r="C27" s="11"/>
@@ -5918,7 +5942,7 @@
       <c r="U27" s="19"/>
       <c r="V27" s="29"/>
     </row>
-    <row r="28" spans="1:22" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D28" s="42"/>
       <c r="E28" s="36"/>
       <c r="F28" s="36"/>
@@ -5955,7 +5979,7 @@
       <c r="U28" s="19"/>
       <c r="V28" s="29"/>
     </row>
-    <row r="29" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="6"/>
       <c r="C29" s="11"/>
@@ -5995,7 +6019,7 @@
       <c r="U29" s="19"/>
       <c r="V29" s="29"/>
     </row>
-    <row r="30" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
       <c r="B30" s="6"/>
       <c r="C30" s="11"/>
@@ -6035,7 +6059,7 @@
       <c r="U30" s="19"/>
       <c r="V30" s="29"/>
     </row>
-    <row r="31" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
       <c r="B31" s="6"/>
       <c r="C31" s="11"/>
@@ -6079,7 +6103,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="32" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
       <c r="C32" s="11"/>
@@ -6117,7 +6141,7 @@
       <c r="U32" s="19"/>
       <c r="V32" s="29"/>
     </row>
-    <row r="33" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6"/>
       <c r="B33" s="6"/>
       <c r="C33" s="11"/>
@@ -6155,7 +6179,7 @@
       <c r="U33" s="19"/>
       <c r="V33" s="29"/>
     </row>
-    <row r="34" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6"/>
       <c r="B34" s="6"/>
       <c r="C34" s="11"/>
@@ -6195,7 +6219,7 @@
       <c r="U34" s="19"/>
       <c r="V34" s="29"/>
     </row>
-    <row r="35" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="6"/>
       <c r="B35" s="6"/>
       <c r="C35" s="11"/>
@@ -6233,7 +6257,7 @@
       <c r="U35" s="19"/>
       <c r="V35" s="29"/>
     </row>
-    <row r="36" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
       <c r="B36" s="6"/>
       <c r="C36" s="11"/>
@@ -6271,7 +6295,7 @@
       <c r="U36" s="19"/>
       <c r="V36" s="29"/>
     </row>
-    <row r="37" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="6"/>
       <c r="B37" s="6"/>
       <c r="C37" s="11"/>
@@ -6309,7 +6333,7 @@
       <c r="U37" s="19"/>
       <c r="V37" s="29"/>
     </row>
-    <row r="38" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="11"/>
@@ -6347,7 +6371,7 @@
       <c r="U38" s="19"/>
       <c r="V38" s="29"/>
     </row>
-    <row r="39" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="11"/>
@@ -6389,7 +6413,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="40" spans="1:22" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D40" s="42"/>
       <c r="E40" s="36"/>
       <c r="F40" s="36"/>
@@ -6423,7 +6447,7 @@
       <c r="T40" s="19"/>
       <c r="U40" s="19"/>
     </row>
-    <row r="41" spans="1:22" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D41" s="42"/>
       <c r="E41" s="36"/>
       <c r="F41" s="36"/>
@@ -6458,7 +6482,7 @@
       <c r="U41" s="19"/>
       <c r="V41" s="29"/>
     </row>
-    <row r="42" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="6"/>
       <c r="B42" s="6"/>
       <c r="C42" s="11"/>
@@ -6496,7 +6520,7 @@
       <c r="U42" s="19"/>
       <c r="V42" s="29"/>
     </row>
-    <row r="43" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="6"/>
       <c r="B43" s="6"/>
       <c r="C43" s="11"/>
@@ -6534,7 +6558,7 @@
       <c r="U43" s="19"/>
       <c r="V43" s="29"/>
     </row>
-    <row r="44" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="6"/>
       <c r="B44" s="6"/>
       <c r="C44" s="11"/>
@@ -6576,7 +6600,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="45" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="6"/>
       <c r="B45" s="6"/>
       <c r="C45" s="11"/>
@@ -6613,7 +6637,7 @@
       <c r="U45" s="19"/>
       <c r="V45" s="29"/>
     </row>
-    <row r="46" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="6"/>
       <c r="B46" s="6"/>
       <c r="C46" s="11"/>
@@ -6651,7 +6675,7 @@
       <c r="U46" s="19"/>
       <c r="V46" s="29"/>
     </row>
-    <row r="47" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="6"/>
       <c r="B47" s="6"/>
       <c r="C47" s="11"/>
@@ -6689,7 +6713,7 @@
       <c r="U47" s="19"/>
       <c r="V47" s="29"/>
     </row>
-    <row r="48" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="6"/>
       <c r="B48" s="6"/>
       <c r="C48" s="11"/>
@@ -6731,7 +6755,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="49" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="6"/>
       <c r="B49" s="6"/>
       <c r="C49" s="11"/>
@@ -6769,7 +6793,7 @@
       <c r="U49" s="19"/>
       <c r="V49" s="29"/>
     </row>
-    <row r="50" spans="1:22" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D50" s="42"/>
       <c r="E50" s="36"/>
       <c r="F50" s="36"/>
@@ -6808,7 +6832,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="51" spans="1:22" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D51" s="42"/>
       <c r="E51" s="36"/>
       <c r="F51" s="36"/>
@@ -6843,7 +6867,7 @@
       <c r="U51" s="19"/>
       <c r="V51" s="29"/>
     </row>
-    <row r="52" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="6"/>
       <c r="B52" s="6"/>
       <c r="C52" s="11"/>
@@ -6885,7 +6909,7 @@
       <c r="U52" s="19"/>
       <c r="V52" s="29"/>
     </row>
-    <row r="53" spans="1:22" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D53" s="42"/>
       <c r="E53" s="36"/>
       <c r="F53" s="36"/>
@@ -6922,7 +6946,7 @@
       <c r="U53" s="19"/>
       <c r="V53" s="29"/>
     </row>
-    <row r="54" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="6"/>
       <c r="B54" s="6"/>
       <c r="C54" s="11"/>
@@ -6962,7 +6986,7 @@
       <c r="U54" s="19"/>
       <c r="V54" s="29"/>
     </row>
-    <row r="55" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="6"/>
       <c r="B55" s="6"/>
       <c r="C55" s="11"/>
@@ -7002,7 +7026,7 @@
       <c r="U55" s="19"/>
       <c r="V55" s="29"/>
     </row>
-    <row r="56" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="6"/>
       <c r="B56" s="6"/>
       <c r="C56" s="11"/>
@@ -7042,7 +7066,7 @@
       <c r="U56" s="19"/>
       <c r="V56" s="29"/>
     </row>
-    <row r="57" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="6"/>
       <c r="B57" s="6"/>
       <c r="C57" s="11"/>
@@ -7082,7 +7106,7 @@
       <c r="U57" s="19"/>
       <c r="V57" s="29"/>
     </row>
-    <row r="58" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="6"/>
       <c r="B58" s="6"/>
       <c r="C58" s="11"/>
@@ -7120,7 +7144,7 @@
       <c r="U58" s="19"/>
       <c r="V58" s="29"/>
     </row>
-    <row r="59" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="6"/>
       <c r="B59" s="6"/>
       <c r="C59" s="11"/>
@@ -7158,7 +7182,7 @@
       <c r="U59" s="19"/>
       <c r="V59" s="29"/>
     </row>
-    <row r="60" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="6"/>
       <c r="B60" s="6"/>
       <c r="C60" s="11"/>
@@ -7200,7 +7224,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="61" spans="1:22" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D61" s="42"/>
       <c r="E61" s="36"/>
       <c r="F61" s="36"/>
@@ -7239,7 +7263,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="62" spans="1:22" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D62" s="42"/>
       <c r="E62" s="36"/>
       <c r="F62" s="36"/>
@@ -7274,7 +7298,7 @@
       <c r="U62" s="19"/>
       <c r="V62" s="29"/>
     </row>
-    <row r="63" spans="1:22" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D63" s="42"/>
       <c r="E63" s="36"/>
       <c r="F63" s="36"/>
@@ -7309,7 +7333,7 @@
       <c r="U63" s="19"/>
       <c r="V63" s="29"/>
     </row>
-    <row r="64" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="6"/>
       <c r="B64" s="6"/>
       <c r="C64" s="11"/>
@@ -7347,7 +7371,7 @@
       <c r="U64" s="19"/>
       <c r="V64" s="29"/>
     </row>
-    <row r="65" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="6"/>
       <c r="B65" s="6"/>
       <c r="C65" s="11"/>
@@ -7385,7 +7409,7 @@
       <c r="U65" s="19"/>
       <c r="V65" s="29"/>
     </row>
-    <row r="66" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="6"/>
       <c r="B66" s="6"/>
       <c r="C66" s="11"/>
@@ -7423,7 +7447,7 @@
       <c r="U66" s="19"/>
       <c r="V66" s="29"/>
     </row>
-    <row r="67" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="6"/>
       <c r="B67" s="6"/>
       <c r="C67" s="11"/>
@@ -7461,7 +7485,7 @@
       <c r="U67" s="19"/>
       <c r="V67" s="29"/>
     </row>
-    <row r="68" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="6"/>
       <c r="B68" s="6"/>
       <c r="C68" s="11"/>
@@ -7499,7 +7523,7 @@
       <c r="U68" s="19"/>
       <c r="V68" s="29"/>
     </row>
-    <row r="69" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="6"/>
       <c r="B69" s="6"/>
       <c r="C69" s="11"/>
@@ -7537,7 +7561,7 @@
       <c r="U69" s="19"/>
       <c r="V69" s="29"/>
     </row>
-    <row r="70" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="6"/>
       <c r="B70" s="6"/>
       <c r="C70" s="11"/>
@@ -7575,7 +7599,7 @@
       <c r="U70" s="19"/>
       <c r="V70" s="29"/>
     </row>
-    <row r="71" spans="1:22" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D71" s="42"/>
       <c r="E71" s="36"/>
       <c r="F71" s="36"/>
@@ -7614,7 +7638,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="72" spans="1:22" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D72" s="42"/>
       <c r="E72" s="36"/>
       <c r="F72" s="36"/>
@@ -7649,7 +7673,7 @@
       <c r="U72" s="19"/>
       <c r="V72" s="29"/>
     </row>
-    <row r="73" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="6"/>
       <c r="B73" s="6"/>
       <c r="C73" s="11"/>
@@ -7691,7 +7715,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="74" spans="1:22" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D74" s="42"/>
       <c r="E74" s="36"/>
       <c r="F74" s="36"/>
@@ -7726,7 +7750,7 @@
       <c r="U74" s="19"/>
       <c r="V74" s="29"/>
     </row>
-    <row r="75" spans="1:22" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D75" s="42"/>
       <c r="E75" s="36"/>
       <c r="F75" s="36"/>
@@ -7765,7 +7789,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="76" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="6"/>
       <c r="B76" s="6"/>
       <c r="C76" s="11"/>
@@ -7803,7 +7827,7 @@
       <c r="U76" s="19"/>
       <c r="V76" s="29"/>
     </row>
-    <row r="77" spans="1:22" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D77" s="42"/>
       <c r="E77" s="36"/>
       <c r="F77" s="36"/>
@@ -7842,7 +7866,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="78" spans="1:22" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D78" s="42"/>
       <c r="E78" s="36"/>
       <c r="F78" s="36"/>
@@ -7879,7 +7903,7 @@
       <c r="U78" s="19"/>
       <c r="V78" s="29"/>
     </row>
-    <row r="79" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="6"/>
       <c r="B79" s="6"/>
       <c r="C79" s="11"/>
@@ -7919,7 +7943,7 @@
       <c r="U79" s="19"/>
       <c r="V79" s="29"/>
     </row>
-    <row r="80" spans="1:22" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D80" s="42"/>
       <c r="E80" s="36"/>
       <c r="F80" s="36"/>
@@ -7956,7 +7980,7 @@
       <c r="U80" s="19"/>
       <c r="V80" s="29"/>
     </row>
-    <row r="81" spans="1:22" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D81" s="42"/>
       <c r="E81" s="36"/>
       <c r="F81" s="36"/>
@@ -7993,7 +8017,7 @@
       <c r="U81" s="19"/>
       <c r="V81" s="29"/>
     </row>
-    <row r="82" spans="1:22" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D82" s="42"/>
       <c r="E82" s="36"/>
       <c r="F82" s="36"/>
@@ -8030,7 +8054,7 @@
       <c r="U82" s="19"/>
       <c r="V82" s="29"/>
     </row>
-    <row r="83" spans="1:22" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D83" s="42"/>
       <c r="E83" s="36"/>
       <c r="F83" s="36"/>
@@ -8067,7 +8091,7 @@
       <c r="U83" s="19"/>
       <c r="V83" s="29"/>
     </row>
-    <row r="84" spans="1:22" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D84" s="42"/>
       <c r="E84" s="36"/>
       <c r="F84" s="36"/>
@@ -8104,7 +8128,7 @@
       <c r="U84" s="19"/>
       <c r="V84" s="29"/>
     </row>
-    <row r="85" spans="1:22" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D85" s="42"/>
       <c r="E85" s="36"/>
       <c r="F85" s="36"/>
@@ -8139,7 +8163,7 @@
       <c r="U85" s="19"/>
       <c r="V85" s="29"/>
     </row>
-    <row r="86" spans="1:22" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D86" s="42"/>
       <c r="E86" s="36"/>
       <c r="F86" s="36"/>
@@ -8178,7 +8202,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="87" spans="1:22" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D87" s="42"/>
       <c r="E87" s="36"/>
       <c r="F87" s="36"/>
@@ -8213,7 +8237,7 @@
       <c r="U87" s="19"/>
       <c r="V87" s="29"/>
     </row>
-    <row r="88" spans="1:22" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D88" s="42"/>
       <c r="E88" s="36"/>
       <c r="F88" s="36"/>
@@ -8248,7 +8272,7 @@
       <c r="U88" s="19"/>
       <c r="V88" s="29"/>
     </row>
-    <row r="89" spans="1:22" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D89" s="42"/>
       <c r="E89" s="36"/>
       <c r="F89" s="36"/>
@@ -8283,7 +8307,7 @@
       <c r="U89" s="19"/>
       <c r="V89" s="29"/>
     </row>
-    <row r="90" spans="1:22" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D90" s="42"/>
       <c r="E90" s="36"/>
       <c r="F90" s="36"/>
@@ -8322,7 +8346,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="91" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="6"/>
       <c r="B91" s="6"/>
       <c r="C91" s="11"/>
@@ -8364,7 +8388,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="92" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="6"/>
       <c r="B92" s="6"/>
       <c r="C92" s="11"/>
@@ -8404,7 +8428,7 @@
       <c r="U92" s="19"/>
       <c r="V92" s="29"/>
     </row>
-    <row r="93" spans="1:22" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D93" s="42"/>
       <c r="E93" s="36"/>
       <c r="F93" s="36"/>
@@ -14210,7 +14234,7 @@
         <v>137</v>
       </c>
       <c r="T254" s="9" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="U254" s="9"/>
     </row>
@@ -21986,7 +22010,7 @@
         <v>137</v>
       </c>
       <c r="T472" s="9" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="U472" s="9"/>
     </row>
@@ -27472,7 +27496,7 @@
       <c r="T627" s="9"/>
       <c r="U627" s="9"/>
     </row>
-    <row r="628" spans="1:22" s="6" customFormat="1" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="628" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D628" s="42"/>
       <c r="E628" s="36"/>
       <c r="F628" s="36"/>
@@ -30139,7 +30163,7 @@
       <c r="T704" s="9"/>
       <c r="U704" s="9"/>
     </row>
-    <row r="705" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="705" spans="4:22" x14ac:dyDescent="0.25">
       <c r="E705" s="36"/>
       <c r="F705" s="36"/>
       <c r="G705" s="36"/>
@@ -30172,7 +30196,7 @@
       <c r="T705" s="9"/>
       <c r="U705" s="9"/>
     </row>
-    <row r="706" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="706" spans="4:22" x14ac:dyDescent="0.25">
       <c r="E706" s="36"/>
       <c r="F706" s="36"/>
       <c r="G706" s="36"/>
@@ -30210,7 +30234,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="707" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="707" spans="4:22" x14ac:dyDescent="0.25">
       <c r="E707" s="36"/>
       <c r="F707" s="36"/>
       <c r="G707" s="36"/>
@@ -30243,7 +30267,7 @@
       <c r="T707" s="9"/>
       <c r="U707" s="9"/>
     </row>
-    <row r="708" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="708" spans="4:22" x14ac:dyDescent="0.25">
       <c r="E708" s="36"/>
       <c r="F708" s="36"/>
       <c r="G708" s="36"/>
@@ -30276,7 +30300,7 @@
       <c r="T708" s="9"/>
       <c r="U708" s="9"/>
     </row>
-    <row r="709" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="709" spans="4:22" x14ac:dyDescent="0.25">
       <c r="E709" s="36"/>
       <c r="F709" s="36"/>
       <c r="G709" s="36"/>
@@ -30314,7 +30338,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="710" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="710" spans="4:22" x14ac:dyDescent="0.25">
       <c r="E710" s="36"/>
       <c r="F710" s="36"/>
       <c r="G710" s="36"/>
@@ -30347,7 +30371,7 @@
       <c r="T710" s="9"/>
       <c r="U710" s="9"/>
     </row>
-    <row r="711" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="711" spans="4:22" x14ac:dyDescent="0.25">
       <c r="E711" s="36"/>
       <c r="F711" s="36"/>
       <c r="G711" s="36"/>
@@ -30380,7 +30404,7 @@
       <c r="T711" s="9"/>
       <c r="U711" s="9"/>
     </row>
-    <row r="712" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="712" spans="4:22" x14ac:dyDescent="0.25">
       <c r="E712" s="36"/>
       <c r="F712" s="36"/>
       <c r="G712" s="36"/>
@@ -30418,7 +30442,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="713" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="713" spans="4:22" x14ac:dyDescent="0.25">
       <c r="E713" s="36"/>
       <c r="F713" s="36"/>
       <c r="G713" s="36"/>
@@ -30451,7 +30475,7 @@
       <c r="T713" s="9"/>
       <c r="U713" s="9"/>
     </row>
-    <row r="714" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="714" spans="4:22" x14ac:dyDescent="0.25">
       <c r="E714" s="36"/>
       <c r="F714" s="36"/>
       <c r="G714" s="36"/>
@@ -30484,7 +30508,7 @@
       <c r="T714" s="9"/>
       <c r="U714" s="9"/>
     </row>
-    <row r="715" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="715" spans="4:22" x14ac:dyDescent="0.25">
       <c r="E715" s="36"/>
       <c r="F715" s="36"/>
       <c r="G715" s="36"/>
@@ -30517,7 +30541,7 @@
       <c r="T715" s="9"/>
       <c r="U715" s="9"/>
     </row>
-    <row r="716" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="716" spans="4:22" x14ac:dyDescent="0.25">
       <c r="E716" s="36"/>
       <c r="F716" s="36"/>
       <c r="G716" s="36"/>
@@ -30550,7 +30574,7 @@
       <c r="T716" s="9"/>
       <c r="U716" s="9"/>
     </row>
-    <row r="717" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="717" spans="4:22" x14ac:dyDescent="0.25">
       <c r="E717" s="36"/>
       <c r="F717" s="36"/>
       <c r="G717" s="36"/>
@@ -30583,7 +30607,10 @@
       <c r="T717" s="9"/>
       <c r="U717" s="9"/>
     </row>
-    <row r="718" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="718" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="D718" s="71" t="s">
+        <v>117</v>
+      </c>
       <c r="E718" s="36"/>
       <c r="F718" s="36"/>
       <c r="G718" s="36"/>
@@ -30620,7 +30647,7 @@
       </c>
       <c r="U718" s="9"/>
     </row>
-    <row r="719" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="719" spans="4:22" x14ac:dyDescent="0.25">
       <c r="E719" s="36"/>
       <c r="F719" s="36"/>
       <c r="G719" s="36"/>
@@ -30653,7 +30680,7 @@
       <c r="T719" s="9"/>
       <c r="U719" s="9"/>
     </row>
-    <row r="720" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="720" spans="4:22" x14ac:dyDescent="0.25">
       <c r="E720" s="36"/>
       <c r="F720" s="36"/>
       <c r="G720" s="36"/>
@@ -33438,7 +33465,10 @@
       <c r="T800" s="9"/>
       <c r="U800" s="9"/>
     </row>
-    <row r="801" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="801" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="D801" s="71" t="s">
+        <v>1226</v>
+      </c>
       <c r="E801" s="36"/>
       <c r="F801" s="36"/>
       <c r="G801" s="36"/>
@@ -33473,7 +33503,10 @@
       <c r="T801" s="9"/>
       <c r="U801" s="9"/>
     </row>
-    <row r="802" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="802" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="D802" s="71" t="s">
+        <v>1226</v>
+      </c>
       <c r="E802" s="36"/>
       <c r="F802" s="36"/>
       <c r="G802" s="36"/>
@@ -33507,14 +33540,17 @@
       <c r="Q802" s="9"/>
       <c r="R802" s="9"/>
       <c r="S802" s="9" t="s">
-        <v>1221</v>
+        <v>1224</v>
       </c>
       <c r="T802" s="9" t="s">
-        <v>1222</v>
+        <v>1225</v>
       </c>
       <c r="U802" s="9"/>
     </row>
-    <row r="803" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="803" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="D803" s="71" t="s">
+        <v>1226</v>
+      </c>
       <c r="E803" s="36"/>
       <c r="F803" s="36"/>
       <c r="G803" s="36"/>
@@ -33549,7 +33585,7 @@
       <c r="T803" s="9"/>
       <c r="U803" s="9"/>
     </row>
-    <row r="804" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="804" spans="4:22" x14ac:dyDescent="0.25">
       <c r="E804" s="36"/>
       <c r="F804" s="36"/>
       <c r="G804" s="36"/>
@@ -33587,7 +33623,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="805" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="805" spans="4:22" x14ac:dyDescent="0.25">
       <c r="E805" s="36"/>
       <c r="F805" s="36"/>
       <c r="G805" s="36"/>
@@ -33620,7 +33656,7 @@
       <c r="T805" s="9"/>
       <c r="U805" s="9"/>
     </row>
-    <row r="806" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="806" spans="4:22" x14ac:dyDescent="0.25">
       <c r="E806" s="36"/>
       <c r="F806" s="36"/>
       <c r="G806" s="36"/>
@@ -33655,11 +33691,11 @@
         <v>137</v>
       </c>
       <c r="T806" s="9" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="U806" s="9"/>
     </row>
-    <row r="807" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="807" spans="4:22" x14ac:dyDescent="0.25">
       <c r="E807" s="36"/>
       <c r="F807" s="36"/>
       <c r="G807" s="36"/>
@@ -33692,7 +33728,7 @@
       <c r="T807" s="9"/>
       <c r="U807" s="9"/>
     </row>
-    <row r="808" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="808" spans="4:22" x14ac:dyDescent="0.25">
       <c r="E808" s="36"/>
       <c r="F808" s="36"/>
       <c r="G808" s="36"/>
@@ -33725,7 +33761,7 @@
       <c r="T808" s="9"/>
       <c r="U808" s="9"/>
     </row>
-    <row r="809" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="809" spans="4:22" x14ac:dyDescent="0.25">
       <c r="E809" s="36"/>
       <c r="F809" s="36"/>
       <c r="G809" s="36"/>
@@ -33758,7 +33794,7 @@
       <c r="T809" s="9"/>
       <c r="U809" s="9"/>
     </row>
-    <row r="810" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="810" spans="4:22" x14ac:dyDescent="0.25">
       <c r="E810" s="36"/>
       <c r="F810" s="36"/>
       <c r="G810" s="36"/>
@@ -33796,7 +33832,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="811" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="811" spans="4:22" x14ac:dyDescent="0.25">
       <c r="E811" s="36"/>
       <c r="F811" s="36"/>
       <c r="G811" s="36"/>
@@ -33831,7 +33867,7 @@
       <c r="T811" s="9"/>
       <c r="U811" s="9"/>
     </row>
-    <row r="812" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="812" spans="4:22" x14ac:dyDescent="0.25">
       <c r="E812" s="36"/>
       <c r="F812" s="36"/>
       <c r="G812" s="36"/>
@@ -33864,7 +33900,7 @@
       <c r="T812" s="9"/>
       <c r="U812" s="9"/>
     </row>
-    <row r="813" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="813" spans="4:22" x14ac:dyDescent="0.25">
       <c r="E813" s="36"/>
       <c r="F813" s="36"/>
       <c r="G813" s="36"/>
@@ -33897,7 +33933,7 @@
       <c r="T813" s="9"/>
       <c r="U813" s="9"/>
     </row>
-    <row r="814" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="814" spans="4:22" x14ac:dyDescent="0.25">
       <c r="E814" s="36"/>
       <c r="F814" s="36"/>
       <c r="G814" s="36"/>
@@ -33935,7 +33971,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="815" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="815" spans="4:22" x14ac:dyDescent="0.25">
       <c r="E815" s="36"/>
       <c r="F815" s="36"/>
       <c r="G815" s="36"/>
@@ -33968,7 +34004,7 @@
       <c r="T815" s="9"/>
       <c r="U815" s="9"/>
     </row>
-    <row r="816" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="816" spans="4:22" x14ac:dyDescent="0.25">
       <c r="E816" s="36"/>
       <c r="F816" s="36"/>
       <c r="G816" s="36"/>
@@ -34140,7 +34176,7 @@
         <v>137</v>
       </c>
       <c r="T820" s="9" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="U820" s="9"/>
     </row>
@@ -36687,7 +36723,7 @@
         <v>137</v>
       </c>
       <c r="T893" s="9" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="U893" s="9"/>
     </row>
@@ -36790,7 +36826,7 @@
       <c r="T896" s="9"/>
       <c r="U896" s="9"/>
     </row>
-    <row r="897" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="897" spans="4:22" x14ac:dyDescent="0.25">
       <c r="E897" s="36"/>
       <c r="F897" s="36"/>
       <c r="G897" s="36"/>
@@ -36823,7 +36859,7 @@
       <c r="T897" s="9"/>
       <c r="U897" s="9"/>
     </row>
-    <row r="898" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="898" spans="4:22" x14ac:dyDescent="0.25">
       <c r="E898" s="36"/>
       <c r="F898" s="36"/>
       <c r="G898" s="36"/>
@@ -36856,7 +36892,7 @@
       <c r="T898" s="9"/>
       <c r="U898" s="9"/>
     </row>
-    <row r="899" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="899" spans="4:22" x14ac:dyDescent="0.25">
       <c r="E899" s="36"/>
       <c r="F899" s="36"/>
       <c r="G899" s="36"/>
@@ -36889,7 +36925,7 @@
       <c r="T899" s="9"/>
       <c r="U899" s="9"/>
     </row>
-    <row r="900" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="900" spans="4:22" x14ac:dyDescent="0.25">
       <c r="E900" s="36"/>
       <c r="F900" s="36"/>
       <c r="G900" s="36"/>
@@ -36922,7 +36958,7 @@
       <c r="T900" s="9"/>
       <c r="U900" s="9"/>
     </row>
-    <row r="901" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="901" spans="4:22" x14ac:dyDescent="0.25">
       <c r="E901" s="36"/>
       <c r="F901" s="36"/>
       <c r="G901" s="36"/>
@@ -36955,7 +36991,7 @@
       <c r="T901" s="9"/>
       <c r="U901" s="9"/>
     </row>
-    <row r="902" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="902" spans="4:22" x14ac:dyDescent="0.25">
       <c r="E902" s="36"/>
       <c r="F902" s="36"/>
       <c r="G902" s="36"/>
@@ -36990,7 +37026,7 @@
       <c r="T902" s="9"/>
       <c r="U902" s="9"/>
     </row>
-    <row r="903" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="903" spans="4:22" x14ac:dyDescent="0.25">
       <c r="E903" s="36"/>
       <c r="F903" s="36"/>
       <c r="G903" s="36"/>
@@ -37027,7 +37063,7 @@
       <c r="T903" s="9"/>
       <c r="U903" s="9"/>
     </row>
-    <row r="904" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="904" spans="4:22" x14ac:dyDescent="0.25">
       <c r="E904" s="36"/>
       <c r="F904" s="36"/>
       <c r="G904" s="36"/>
@@ -37062,7 +37098,7 @@
       <c r="T904" s="9"/>
       <c r="U904" s="9"/>
     </row>
-    <row r="905" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="905" spans="4:22" x14ac:dyDescent="0.25">
       <c r="E905" s="36"/>
       <c r="F905" s="36"/>
       <c r="G905" s="36"/>
@@ -37102,7 +37138,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="906" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="906" spans="4:22" x14ac:dyDescent="0.25">
       <c r="E906" s="36"/>
       <c r="F906" s="36"/>
       <c r="G906" s="36"/>
@@ -37137,7 +37173,7 @@
       <c r="T906" s="9"/>
       <c r="U906" s="9"/>
     </row>
-    <row r="907" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="907" spans="4:22" x14ac:dyDescent="0.25">
       <c r="E907" s="36"/>
       <c r="F907" s="36"/>
       <c r="G907" s="36"/>
@@ -37172,7 +37208,7 @@
       <c r="T907" s="9"/>
       <c r="U907" s="9"/>
     </row>
-    <row r="908" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="908" spans="4:22" x14ac:dyDescent="0.25">
       <c r="E908" s="36"/>
       <c r="F908" s="36"/>
       <c r="G908" s="36"/>
@@ -37207,7 +37243,10 @@
       <c r="T908" s="9"/>
       <c r="U908" s="9"/>
     </row>
-    <row r="909" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="909" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="D909" s="71" t="s">
+        <v>1227</v>
+      </c>
       <c r="E909" s="36"/>
       <c r="F909" s="36"/>
       <c r="G909" s="36"/>
@@ -37248,7 +37287,10 @@
       </c>
       <c r="U909" s="9"/>
     </row>
-    <row r="910" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="910" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="D910" s="71" t="s">
+        <v>1227</v>
+      </c>
       <c r="E910" s="36"/>
       <c r="F910" s="36"/>
       <c r="G910" s="36"/>
@@ -37283,7 +37325,7 @@
       <c r="T910" s="9"/>
       <c r="U910" s="9"/>
     </row>
-    <row r="911" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="911" spans="4:22" x14ac:dyDescent="0.25">
       <c r="E911" s="36"/>
       <c r="F911" s="36"/>
       <c r="G911" s="36"/>
@@ -37318,7 +37360,7 @@
       <c r="T911" s="9"/>
       <c r="U911" s="9"/>
     </row>
-    <row r="912" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="912" spans="4:22" x14ac:dyDescent="0.25">
       <c r="E912" s="36"/>
       <c r="F912" s="36"/>
       <c r="G912" s="36"/>
@@ -45717,7 +45759,10 @@
       <c r="T1152" s="9"/>
       <c r="U1152" s="9"/>
     </row>
-    <row r="1153" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1153" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="D1153" s="71" t="s">
+        <v>1228</v>
+      </c>
       <c r="E1153" s="36"/>
       <c r="F1153" s="36"/>
       <c r="G1153" s="36"/>
@@ -45755,7 +45800,10 @@
         <v>138</v>
       </c>
     </row>
-    <row r="1154" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1154" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="D1154" s="71" t="s">
+        <v>1228</v>
+      </c>
       <c r="E1154" s="36"/>
       <c r="F1154" s="36"/>
       <c r="G1154" s="36"/>
@@ -45790,7 +45838,10 @@
       <c r="T1154" s="9"/>
       <c r="U1154" s="9"/>
     </row>
-    <row r="1155" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1155" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="D1155" s="71" t="s">
+        <v>1228</v>
+      </c>
       <c r="E1155" s="36"/>
       <c r="F1155" s="36"/>
       <c r="G1155" s="36"/>
@@ -45825,7 +45876,7 @@
       <c r="T1155" s="9"/>
       <c r="U1155" s="9"/>
     </row>
-    <row r="1156" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1156" spans="4:22" x14ac:dyDescent="0.25">
       <c r="E1156" s="36"/>
       <c r="F1156" s="36"/>
       <c r="G1156" s="36"/>
@@ -45865,7 +45916,10 @@
         <v>917</v>
       </c>
     </row>
-    <row r="1157" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1157" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="D1157" s="71" t="s">
+        <v>1228</v>
+      </c>
       <c r="E1157" s="36"/>
       <c r="F1157" s="36"/>
       <c r="G1157" s="36"/>
@@ -45903,7 +45957,10 @@
         <v>144</v>
       </c>
     </row>
-    <row r="1158" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1158" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="D1158" s="71" t="s">
+        <v>1228</v>
+      </c>
       <c r="E1158" s="36"/>
       <c r="F1158" s="36"/>
       <c r="G1158" s="36"/>
@@ -45947,7 +46004,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="1159" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1159" spans="4:22" x14ac:dyDescent="0.25">
       <c r="E1159" s="36"/>
       <c r="F1159" s="36"/>
       <c r="G1159" s="36"/>
@@ -45985,7 +46042,7 @@
         <v>922</v>
       </c>
     </row>
-    <row r="1160" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1160" spans="4:22" x14ac:dyDescent="0.25">
       <c r="E1160" s="36"/>
       <c r="F1160" s="36"/>
       <c r="G1160" s="36"/>
@@ -46018,7 +46075,7 @@
       <c r="T1160" s="9"/>
       <c r="U1160" s="9"/>
     </row>
-    <row r="1161" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1161" spans="4:22" x14ac:dyDescent="0.25">
       <c r="E1161" s="36"/>
       <c r="F1161" s="36"/>
       <c r="G1161" s="36"/>
@@ -46056,7 +46113,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="1162" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1162" spans="4:22" x14ac:dyDescent="0.25">
       <c r="E1162" s="36"/>
       <c r="F1162" s="36"/>
       <c r="G1162" s="36"/>
@@ -46089,7 +46146,7 @@
       <c r="T1162" s="9"/>
       <c r="U1162" s="9"/>
     </row>
-    <row r="1163" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1163" spans="4:22" x14ac:dyDescent="0.25">
       <c r="E1163" s="36"/>
       <c r="F1163" s="36"/>
       <c r="G1163" s="36"/>
@@ -46122,7 +46179,7 @@
       <c r="T1163" s="9"/>
       <c r="U1163" s="9"/>
     </row>
-    <row r="1164" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1164" spans="4:22" x14ac:dyDescent="0.25">
       <c r="E1164" s="36"/>
       <c r="F1164" s="36"/>
       <c r="G1164" s="36"/>
@@ -46155,7 +46212,7 @@
       <c r="T1164" s="9"/>
       <c r="U1164" s="9"/>
     </row>
-    <row r="1165" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1165" spans="4:22" x14ac:dyDescent="0.25">
       <c r="E1165" s="36"/>
       <c r="F1165" s="36"/>
       <c r="G1165" s="36"/>
@@ -46193,7 +46250,7 @@
         <v>927</v>
       </c>
     </row>
-    <row r="1166" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1166" spans="4:22" x14ac:dyDescent="0.25">
       <c r="E1166" s="36"/>
       <c r="F1166" s="36"/>
       <c r="G1166" s="36"/>
@@ -46229,7 +46286,7 @@
       </c>
       <c r="T1166" s="9"/>
     </row>
-    <row r="1167" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1167" spans="4:22" x14ac:dyDescent="0.25">
       <c r="E1167" s="36"/>
       <c r="F1167" s="36"/>
       <c r="G1167" s="36"/>
@@ -46264,7 +46321,7 @@
       <c r="T1167" s="9"/>
       <c r="U1167" s="9"/>
     </row>
-    <row r="1168" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1168" spans="4:22" x14ac:dyDescent="0.25">
       <c r="E1168" s="36"/>
       <c r="F1168" s="36"/>
       <c r="G1168" s="36"/>
@@ -46925,7 +46982,7 @@
         <v>137</v>
       </c>
       <c r="T1186" s="9" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="U1186" s="9"/>
     </row>
@@ -50701,7 +50758,7 @@
       <c r="T1296" s="9"/>
       <c r="U1296" s="9"/>
     </row>
-    <row r="1297" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1297" spans="3:22" x14ac:dyDescent="0.25">
       <c r="E1297" s="36"/>
       <c r="F1297" s="36"/>
       <c r="G1297" s="36"/>
@@ -50738,7 +50795,7 @@
       </c>
       <c r="U1297" s="9"/>
     </row>
-    <row r="1298" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1298" spans="3:22" x14ac:dyDescent="0.25">
       <c r="E1298" s="36"/>
       <c r="F1298" s="36"/>
       <c r="G1298" s="36"/>
@@ -50771,7 +50828,7 @@
       <c r="T1298" s="9"/>
       <c r="U1298" s="9"/>
     </row>
-    <row r="1299" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1299" spans="3:22" x14ac:dyDescent="0.25">
       <c r="E1299" s="36"/>
       <c r="F1299" s="36"/>
       <c r="G1299" s="36"/>
@@ -50804,7 +50861,7 @@
       <c r="T1299" s="9"/>
       <c r="U1299" s="9"/>
     </row>
-    <row r="1300" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1300" spans="3:22" x14ac:dyDescent="0.25">
       <c r="E1300" s="36"/>
       <c r="F1300" s="36"/>
       <c r="G1300" s="36"/>
@@ -50837,7 +50894,7 @@
       <c r="T1300" s="9"/>
       <c r="U1300" s="9"/>
     </row>
-    <row r="1301" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1301" spans="3:22" x14ac:dyDescent="0.25">
       <c r="E1301" s="36"/>
       <c r="F1301" s="36"/>
       <c r="G1301" s="36"/>
@@ -50870,7 +50927,7 @@
       <c r="T1301" s="9"/>
       <c r="U1301" s="9"/>
     </row>
-    <row r="1302" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1302" spans="3:22" x14ac:dyDescent="0.25">
       <c r="E1302" s="36"/>
       <c r="F1302" s="36"/>
       <c r="G1302" s="36"/>
@@ -50903,7 +50960,7 @@
       <c r="T1302" s="9"/>
       <c r="U1302" s="9"/>
     </row>
-    <row r="1303" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1303" spans="3:22" x14ac:dyDescent="0.25">
       <c r="E1303" s="36"/>
       <c r="F1303" s="36"/>
       <c r="G1303" s="36"/>
@@ -50936,7 +50993,7 @@
       <c r="T1303" s="9"/>
       <c r="U1303" s="9"/>
     </row>
-    <row r="1304" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1304" spans="3:22" x14ac:dyDescent="0.25">
       <c r="E1304" s="36"/>
       <c r="F1304" s="36"/>
       <c r="G1304" s="36"/>
@@ -50969,7 +51026,7 @@
       <c r="T1304" s="9"/>
       <c r="U1304" s="9"/>
     </row>
-    <row r="1305" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1305" spans="3:22" x14ac:dyDescent="0.25">
       <c r="E1305" s="36"/>
       <c r="F1305" s="36"/>
       <c r="G1305" s="36"/>
@@ -51002,7 +51059,7 @@
       <c r="T1305" s="9"/>
       <c r="U1305" s="9"/>
     </row>
-    <row r="1306" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1306" spans="3:22" x14ac:dyDescent="0.25">
       <c r="E1306" s="36"/>
       <c r="F1306" s="36"/>
       <c r="G1306" s="36"/>
@@ -51035,7 +51092,7 @@
       <c r="T1306" s="9"/>
       <c r="U1306" s="9"/>
     </row>
-    <row r="1307" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1307" spans="3:22" x14ac:dyDescent="0.25">
       <c r="E1307" s="36"/>
       <c r="F1307" s="36"/>
       <c r="G1307" s="36"/>
@@ -51068,7 +51125,7 @@
       <c r="T1307" s="9"/>
       <c r="U1307" s="9"/>
     </row>
-    <row r="1308" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1308" spans="3:22" x14ac:dyDescent="0.25">
       <c r="E1308" s="36"/>
       <c r="F1308" s="36"/>
       <c r="G1308" s="36"/>
@@ -51106,7 +51163,10 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="1309" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1309" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1309" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1309" s="36"/>
       <c r="F1309" s="58" t="s">
         <v>125</v>
@@ -51142,7 +51202,10 @@
       <c r="T1309" s="9"/>
       <c r="U1309" s="9"/>
     </row>
-    <row r="1310" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1310" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1310" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1310" s="36"/>
       <c r="F1310" s="58" t="s">
         <v>125</v>
@@ -51179,7 +51242,10 @@
       <c r="T1310" s="9"/>
       <c r="U1310" s="9"/>
     </row>
-    <row r="1311" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1311" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1311" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1311" s="36"/>
       <c r="F1311" s="58" t="s">
         <v>125</v>
@@ -51221,7 +51287,10 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="1312" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1312" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1312" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1312" s="36"/>
       <c r="F1312" s="36"/>
       <c r="G1312" s="36"/>
@@ -51254,7 +51323,10 @@
       <c r="T1312" s="9"/>
       <c r="U1312" s="9"/>
     </row>
-    <row r="1313" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1313" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1313" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1313" s="36"/>
       <c r="F1313" s="36"/>
       <c r="G1313" s="36"/>
@@ -51287,7 +51359,10 @@
       <c r="T1313" s="9"/>
       <c r="U1313" s="9"/>
     </row>
-    <row r="1314" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1314" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1314" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1314" s="36"/>
       <c r="F1314" s="36"/>
       <c r="G1314" s="36"/>
@@ -51320,7 +51395,10 @@
       <c r="T1314" s="9"/>
       <c r="U1314" s="9"/>
     </row>
-    <row r="1315" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1315" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1315" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1315" s="36"/>
       <c r="F1315" s="36"/>
       <c r="G1315" s="36"/>
@@ -51353,7 +51431,10 @@
       <c r="T1315" s="9"/>
       <c r="U1315" s="9"/>
     </row>
-    <row r="1316" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1316" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1316" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1316" s="36"/>
       <c r="F1316" s="36"/>
       <c r="G1316" s="36"/>
@@ -51391,7 +51472,10 @@
         <v>1032</v>
       </c>
     </row>
-    <row r="1317" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1317" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1317" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1317" s="36"/>
       <c r="F1317" s="36"/>
       <c r="G1317" s="36"/>
@@ -51424,7 +51508,10 @@
       <c r="T1317" s="9"/>
       <c r="U1317" s="9"/>
     </row>
-    <row r="1318" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1318" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1318" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1318" s="36"/>
       <c r="F1318" s="36"/>
       <c r="G1318" s="36"/>
@@ -51457,7 +51544,10 @@
       <c r="T1318" s="9"/>
       <c r="U1318" s="9"/>
     </row>
-    <row r="1319" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1319" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1319" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1319" s="36"/>
       <c r="F1319" s="36"/>
       <c r="G1319" s="36"/>
@@ -51490,7 +51580,10 @@
       <c r="T1319" s="9"/>
       <c r="U1319" s="9"/>
     </row>
-    <row r="1320" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1320" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1320" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1320" s="36"/>
       <c r="F1320" s="36"/>
       <c r="G1320" s="36"/>
@@ -51523,7 +51616,10 @@
       <c r="T1320" s="9"/>
       <c r="U1320" s="9"/>
     </row>
-    <row r="1321" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1321" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1321" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1321" s="36"/>
       <c r="F1321" s="36"/>
       <c r="G1321" s="36"/>
@@ -51556,7 +51652,10 @@
       <c r="T1321" s="9"/>
       <c r="U1321" s="9"/>
     </row>
-    <row r="1322" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1322" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1322" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1322" s="36"/>
       <c r="F1322" s="36"/>
       <c r="G1322" s="36"/>
@@ -51589,7 +51688,10 @@
       <c r="T1322" s="9"/>
       <c r="U1322" s="9"/>
     </row>
-    <row r="1323" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1323" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1323" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1323" s="36"/>
       <c r="F1323" s="36"/>
       <c r="G1323" s="36"/>
@@ -51622,7 +51724,10 @@
       <c r="T1323" s="9"/>
       <c r="U1323" s="9"/>
     </row>
-    <row r="1324" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1324" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1324" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1324" s="36"/>
       <c r="F1324" s="36"/>
       <c r="G1324" s="36"/>
@@ -51655,7 +51760,10 @@
       <c r="T1324" s="9"/>
       <c r="U1324" s="9"/>
     </row>
-    <row r="1325" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1325" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1325" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1325" s="36"/>
       <c r="F1325" s="36"/>
       <c r="G1325" s="36"/>
@@ -51693,7 +51801,10 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="1326" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1326" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1326" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1326" s="36"/>
       <c r="F1326" s="36"/>
       <c r="G1326" s="36"/>
@@ -51728,7 +51839,10 @@
       <c r="T1326" s="9"/>
       <c r="U1326" s="9"/>
     </row>
-    <row r="1327" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1327" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1327" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1327" s="36"/>
       <c r="F1327" s="36"/>
       <c r="G1327" s="36"/>
@@ -51763,7 +51877,10 @@
       <c r="T1327" s="9"/>
       <c r="U1327" s="9"/>
     </row>
-    <row r="1328" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1328" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1328" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1328" s="36"/>
       <c r="F1328" s="36"/>
       <c r="G1328" s="36"/>
@@ -51803,7 +51920,10 @@
         <v>1041</v>
       </c>
     </row>
-    <row r="1329" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1329" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1329" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1329" s="36"/>
       <c r="F1329" s="36"/>
       <c r="G1329" s="36"/>
@@ -51838,7 +51958,10 @@
       <c r="T1329" s="9"/>
       <c r="U1329" s="9"/>
     </row>
-    <row r="1330" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1330" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1330" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1330" s="36"/>
       <c r="F1330" s="36"/>
       <c r="G1330" s="36"/>
@@ -51878,7 +52001,10 @@
         <v>1043</v>
       </c>
     </row>
-    <row r="1331" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1331" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1331" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1331" s="36"/>
       <c r="F1331" s="36"/>
       <c r="G1331" s="36"/>
@@ -51913,7 +52039,10 @@
       <c r="T1331" s="9"/>
       <c r="U1331" s="9"/>
     </row>
-    <row r="1332" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1332" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1332" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1332" s="36"/>
       <c r="F1332" s="36"/>
       <c r="G1332" s="36"/>
@@ -51948,7 +52077,10 @@
       <c r="T1332" s="9"/>
       <c r="U1332" s="9"/>
     </row>
-    <row r="1333" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1333" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1333" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1333" s="36"/>
       <c r="F1333" s="36"/>
       <c r="G1333" s="36"/>
@@ -51984,7 +52116,10 @@
       </c>
       <c r="T1333" s="9"/>
     </row>
-    <row r="1334" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1334" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1334" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1334" s="36"/>
       <c r="F1334" s="36"/>
       <c r="G1334" s="36"/>
@@ -52023,7 +52158,10 @@
         <v>1048</v>
       </c>
     </row>
-    <row r="1335" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1335" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1335" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1335" s="36"/>
       <c r="F1335" s="36"/>
       <c r="G1335" s="36"/>
@@ -52057,7 +52195,10 @@
       </c>
       <c r="T1335" s="9"/>
     </row>
-    <row r="1336" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1336" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1336" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1336" s="36"/>
       <c r="F1336" s="36"/>
       <c r="G1336" s="36"/>
@@ -52090,7 +52231,10 @@
       <c r="T1336" s="9"/>
       <c r="U1336" s="9"/>
     </row>
-    <row r="1337" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1337" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1337" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1337" s="36"/>
       <c r="F1337" s="36"/>
       <c r="G1337" s="36"/>
@@ -52128,7 +52272,10 @@
         <v>1051</v>
       </c>
     </row>
-    <row r="1338" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1338" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1338" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1338" s="36"/>
       <c r="F1338" s="36"/>
       <c r="G1338" s="36"/>
@@ -52166,7 +52313,10 @@
         <v>1053</v>
       </c>
     </row>
-    <row r="1339" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1339" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1339" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1339" s="36"/>
       <c r="F1339" s="36"/>
       <c r="G1339" s="36"/>
@@ -52204,7 +52354,10 @@
         <v>1055</v>
       </c>
     </row>
-    <row r="1340" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1340" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1340" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1340" s="36"/>
       <c r="F1340" s="36"/>
       <c r="G1340" s="36"/>
@@ -52237,7 +52390,10 @@
       <c r="T1340" s="9"/>
       <c r="U1340" s="9"/>
     </row>
-    <row r="1341" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1341" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1341" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1341" s="36"/>
       <c r="F1341" s="36"/>
       <c r="G1341" s="36"/>
@@ -52270,7 +52426,10 @@
       <c r="T1341" s="9"/>
       <c r="U1341" s="9"/>
     </row>
-    <row r="1342" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1342" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1342" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1342" s="36"/>
       <c r="F1342" s="36"/>
       <c r="G1342" s="36"/>
@@ -52308,7 +52467,10 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="1343" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1343" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1343" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1343" s="36"/>
       <c r="F1343" s="36"/>
       <c r="G1343" s="36"/>
@@ -52346,7 +52508,10 @@
         <v>1055</v>
       </c>
     </row>
-    <row r="1344" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1344" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1344" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1344" s="36"/>
       <c r="F1344" s="36"/>
       <c r="G1344" s="36"/>
@@ -52379,7 +52544,10 @@
       <c r="T1344" s="9"/>
       <c r="U1344" s="9"/>
     </row>
-    <row r="1345" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1345" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1345" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1345" s="36"/>
       <c r="F1345" s="36"/>
       <c r="G1345" s="36"/>
@@ -52412,7 +52580,10 @@
       <c r="T1345" s="9"/>
       <c r="U1345" s="9"/>
     </row>
-    <row r="1346" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1346" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1346" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1346" s="36"/>
       <c r="F1346" s="36"/>
       <c r="G1346" s="36"/>
@@ -52450,7 +52621,10 @@
         <v>1063</v>
       </c>
     </row>
-    <row r="1347" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1347" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1347" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1347" s="36"/>
       <c r="F1347" s="36"/>
       <c r="G1347" s="36"/>
@@ -52488,7 +52662,10 @@
         <v>1065</v>
       </c>
     </row>
-    <row r="1348" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1348" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1348" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1348" s="36"/>
       <c r="F1348" s="36"/>
       <c r="G1348" s="36"/>
@@ -52521,7 +52698,10 @@
       <c r="T1348" s="9"/>
       <c r="U1348" s="9"/>
     </row>
-    <row r="1349" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1349" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1349" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1349" s="36"/>
       <c r="F1349" s="36"/>
       <c r="G1349" s="36"/>
@@ -52554,7 +52734,10 @@
       <c r="T1349" s="9"/>
       <c r="U1349" s="9"/>
     </row>
-    <row r="1350" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1350" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1350" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1350" s="36"/>
       <c r="F1350" s="36"/>
       <c r="G1350" s="36"/>
@@ -52592,7 +52775,10 @@
         <v>1069</v>
       </c>
     </row>
-    <row r="1351" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1351" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1351" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1351" s="36"/>
       <c r="F1351" s="36"/>
       <c r="G1351" s="36"/>
@@ -52625,7 +52811,10 @@
       <c r="T1351" s="9"/>
       <c r="U1351" s="9"/>
     </row>
-    <row r="1352" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1352" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1352" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1352" s="36"/>
       <c r="F1352" s="36"/>
       <c r="G1352" s="36"/>
@@ -52658,7 +52847,10 @@
       <c r="T1352" s="9"/>
       <c r="U1352" s="9"/>
     </row>
-    <row r="1353" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1353" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1353" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1353" s="36"/>
       <c r="F1353" s="36"/>
       <c r="G1353" s="36"/>
@@ -52691,7 +52883,10 @@
       <c r="T1353" s="9"/>
       <c r="U1353" s="9"/>
     </row>
-    <row r="1354" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1354" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1354" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1354" s="36"/>
       <c r="F1354" s="36"/>
       <c r="G1354" s="36"/>
@@ -52729,7 +52924,10 @@
         <v>1073</v>
       </c>
     </row>
-    <row r="1355" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1355" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1355" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1355" s="36"/>
       <c r="F1355" s="36"/>
       <c r="G1355" s="36"/>
@@ -52762,7 +52960,10 @@
       <c r="T1355" s="9"/>
       <c r="U1355" s="9"/>
     </row>
-    <row r="1356" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1356" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1356" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1356" s="36"/>
       <c r="F1356" s="36"/>
       <c r="G1356" s="36"/>
@@ -52800,7 +53001,10 @@
         <v>1055</v>
       </c>
     </row>
-    <row r="1357" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1357" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1357" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1357" s="36"/>
       <c r="F1357" s="36"/>
       <c r="G1357" s="36"/>
@@ -52838,7 +53042,10 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="1358" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1358" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1358" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1358" s="36"/>
       <c r="F1358" s="36"/>
       <c r="G1358" s="36"/>
@@ -52876,7 +53083,10 @@
         <v>1077</v>
       </c>
     </row>
-    <row r="1359" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1359" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1359" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1359" s="36"/>
       <c r="F1359" s="36"/>
       <c r="G1359" s="36"/>
@@ -52911,7 +53121,10 @@
       <c r="T1359" s="9"/>
       <c r="U1359" s="9"/>
     </row>
-    <row r="1360" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1360" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1360" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1360" s="36"/>
       <c r="F1360" s="36"/>
       <c r="G1360" s="36"/>
@@ -52946,7 +53159,10 @@
       <c r="T1360" s="9"/>
       <c r="U1360" s="9"/>
     </row>
-    <row r="1361" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1361" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1361" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1361" s="36"/>
       <c r="F1361" s="36"/>
       <c r="G1361" s="36"/>
@@ -52981,7 +53197,10 @@
       <c r="T1361" s="9"/>
       <c r="U1361" s="9"/>
     </row>
-    <row r="1362" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1362" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1362" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1362" s="36"/>
       <c r="F1362" s="36"/>
       <c r="G1362" s="36"/>
@@ -53021,7 +53240,10 @@
         <v>1079</v>
       </c>
     </row>
-    <row r="1363" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1363" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1363" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1363" s="36"/>
       <c r="F1363" s="36"/>
       <c r="G1363" s="36"/>
@@ -53056,7 +53278,10 @@
       <c r="T1363" s="9"/>
       <c r="U1363" s="9"/>
     </row>
-    <row r="1364" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1364" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1364" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1364" s="36"/>
       <c r="F1364" s="36"/>
       <c r="G1364" s="36"/>
@@ -53089,7 +53314,10 @@
       <c r="T1364" s="9"/>
       <c r="U1364" s="9"/>
     </row>
-    <row r="1365" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1365" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1365" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1365" s="36"/>
       <c r="F1365" s="36"/>
       <c r="G1365" s="36"/>
@@ -53122,7 +53350,10 @@
       <c r="T1365" s="9"/>
       <c r="U1365" s="9"/>
     </row>
-    <row r="1366" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1366" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1366" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1366" s="36"/>
       <c r="F1366" s="36"/>
       <c r="G1366" s="36"/>
@@ -53155,7 +53386,10 @@
       <c r="T1366" s="9"/>
       <c r="U1366" s="9"/>
     </row>
-    <row r="1367" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1367" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1367" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1367" s="36"/>
       <c r="F1367" s="36"/>
       <c r="G1367" s="36"/>
@@ -53188,7 +53422,10 @@
       <c r="T1367" s="9"/>
       <c r="U1367" s="9"/>
     </row>
-    <row r="1368" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1368" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1368" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1368" s="36"/>
       <c r="F1368" s="36"/>
       <c r="G1368" s="36"/>
@@ -53226,7 +53463,10 @@
         <v>1086</v>
       </c>
     </row>
-    <row r="1369" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1369" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1369" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1369" s="36"/>
       <c r="F1369" s="36"/>
       <c r="G1369" s="36"/>
@@ -53261,7 +53501,10 @@
       <c r="T1369" s="9"/>
       <c r="U1369" s="9"/>
     </row>
-    <row r="1370" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1370" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1370" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1370" s="36"/>
       <c r="F1370" s="36"/>
       <c r="G1370" s="36"/>
@@ -53293,14 +53536,17 @@
       <c r="Q1370" s="9"/>
       <c r="R1370" s="9"/>
       <c r="S1370" s="9" t="s">
-        <v>1224</v>
+        <v>1222</v>
       </c>
       <c r="T1370" s="9" t="s">
-        <v>1225</v>
+        <v>1223</v>
       </c>
       <c r="U1370" s="9"/>
     </row>
-    <row r="1371" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1371" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1371" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1371" s="36"/>
       <c r="F1371" s="36"/>
       <c r="G1371" s="36"/>
@@ -53334,7 +53580,10 @@
       <c r="T1371" s="9"/>
       <c r="U1371" s="9"/>
     </row>
-    <row r="1372" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1372" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1372" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1372" s="36"/>
       <c r="F1372" s="36"/>
       <c r="G1372" s="36"/>
@@ -53373,7 +53622,10 @@
       </c>
       <c r="U1372" s="9"/>
     </row>
-    <row r="1373" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1373" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1373" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1373" s="36"/>
       <c r="F1373" s="36"/>
       <c r="G1373" s="36"/>
@@ -53408,7 +53660,10 @@
       <c r="T1373" s="9"/>
       <c r="U1373" s="9"/>
     </row>
-    <row r="1374" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1374" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1374" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1374" s="36"/>
       <c r="F1374" s="36"/>
       <c r="G1374" s="36"/>
@@ -53443,7 +53698,10 @@
       <c r="T1374" s="9"/>
       <c r="U1374" s="9"/>
     </row>
-    <row r="1375" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1375" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1375" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1375" s="36"/>
       <c r="F1375" s="36"/>
       <c r="G1375" s="36"/>
@@ -53476,7 +53734,10 @@
       <c r="T1375" s="9"/>
       <c r="U1375" s="9"/>
     </row>
-    <row r="1376" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1376" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1376" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1376" s="36"/>
       <c r="F1376" s="36"/>
       <c r="G1376" s="36"/>
@@ -53516,7 +53777,10 @@
         <v>1090</v>
       </c>
     </row>
-    <row r="1377" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1377" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1377" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1377" s="36"/>
       <c r="F1377" s="36"/>
       <c r="G1377" s="36"/>
@@ -53549,7 +53813,10 @@
       <c r="T1377" s="9"/>
       <c r="U1377" s="9"/>
     </row>
-    <row r="1378" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1378" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1378" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1378" s="36"/>
       <c r="F1378" s="36"/>
       <c r="G1378" s="36"/>
@@ -53582,7 +53849,10 @@
       <c r="T1378" s="9"/>
       <c r="U1378" s="9"/>
     </row>
-    <row r="1379" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1379" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1379" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1379" s="36"/>
       <c r="F1379" s="36"/>
       <c r="G1379" s="36"/>
@@ -53620,7 +53890,10 @@
         <v>1094</v>
       </c>
     </row>
-    <row r="1380" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1380" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1380" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1380" s="36"/>
       <c r="F1380" s="36"/>
       <c r="G1380" s="36"/>
@@ -53660,7 +53933,10 @@
         <v>1096</v>
       </c>
     </row>
-    <row r="1381" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1381" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1381" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1381" s="36"/>
       <c r="F1381" s="36"/>
       <c r="G1381" s="36"/>
@@ -53700,7 +53976,10 @@
         <v>1098</v>
       </c>
     </row>
-    <row r="1382" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1382" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1382" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1382" s="36"/>
       <c r="F1382" s="36"/>
       <c r="G1382" s="36"/>
@@ -53735,7 +54014,10 @@
       <c r="T1382" s="9"/>
       <c r="U1382" s="9"/>
     </row>
-    <row r="1383" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1383" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1383" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1383" s="36"/>
       <c r="F1383" s="36"/>
       <c r="G1383" s="36"/>
@@ -53770,7 +54052,10 @@
       <c r="T1383" s="9"/>
       <c r="U1383" s="9"/>
     </row>
-    <row r="1384" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1384" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1384" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1384" s="36"/>
       <c r="F1384" s="36"/>
       <c r="G1384" s="36"/>
@@ -53805,7 +54090,10 @@
       <c r="T1384" s="9"/>
       <c r="U1384" s="9"/>
     </row>
-    <row r="1385" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1385" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1385" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1385" s="36"/>
       <c r="F1385" s="36"/>
       <c r="G1385" s="36"/>
@@ -53842,7 +54130,10 @@
         <v>56</v>
       </c>
     </row>
-    <row r="1386" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1386" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1386" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1386" s="36"/>
       <c r="F1386" s="36"/>
       <c r="G1386" s="36"/>
@@ -53875,7 +54166,10 @@
       <c r="T1386" s="9"/>
       <c r="U1386" s="9"/>
     </row>
-    <row r="1387" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1387" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1387" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1387" s="36"/>
       <c r="F1387" s="36"/>
       <c r="G1387" s="36"/>
@@ -53913,7 +54207,10 @@
         <v>1104</v>
       </c>
     </row>
-    <row r="1388" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1388" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1388" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1388" s="36"/>
       <c r="F1388" s="36"/>
       <c r="G1388" s="36"/>
@@ -53946,7 +54243,10 @@
       <c r="T1388" s="9"/>
       <c r="U1388" s="9"/>
     </row>
-    <row r="1389" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1389" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1389" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1389" s="36"/>
       <c r="F1389" s="36"/>
       <c r="G1389" s="36"/>
@@ -53979,7 +54279,10 @@
       <c r="T1389" s="9"/>
       <c r="U1389" s="9"/>
     </row>
-    <row r="1390" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1390" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1390" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1390" s="36"/>
       <c r="F1390" s="36"/>
       <c r="G1390" s="36"/>
@@ -54012,7 +54315,10 @@
       <c r="T1390" s="9"/>
       <c r="U1390" s="9"/>
     </row>
-    <row r="1391" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1391" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1391" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1391" s="36"/>
       <c r="F1391" s="36"/>
       <c r="G1391" s="36"/>
@@ -54045,7 +54351,10 @@
       <c r="T1391" s="9"/>
       <c r="U1391" s="9"/>
     </row>
-    <row r="1392" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1392" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1392" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1392" s="36"/>
       <c r="F1392" s="36"/>
       <c r="G1392" s="36"/>
@@ -54083,7 +54392,10 @@
         <v>1108</v>
       </c>
     </row>
-    <row r="1393" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1393" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1393" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1393" s="36"/>
       <c r="F1393" s="36"/>
       <c r="G1393" s="36"/>
@@ -54121,7 +54433,10 @@
         <v>1110</v>
       </c>
     </row>
-    <row r="1394" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1394" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1394" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1394" s="36"/>
       <c r="F1394" s="36"/>
       <c r="G1394" s="36"/>
@@ -54154,7 +54469,10 @@
       <c r="T1394" s="9"/>
       <c r="U1394" s="9"/>
     </row>
-    <row r="1395" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1395" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1395" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1395" s="36"/>
       <c r="F1395" s="36"/>
       <c r="G1395" s="36"/>
@@ -54189,7 +54507,10 @@
       <c r="T1395" s="9"/>
       <c r="U1395" s="9"/>
     </row>
-    <row r="1396" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1396" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1396" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1396" s="36"/>
       <c r="F1396" s="36"/>
       <c r="G1396" s="36"/>
@@ -54227,7 +54548,10 @@
         <v>1112</v>
       </c>
     </row>
-    <row r="1397" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1397" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1397" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1397" s="36"/>
       <c r="F1397" s="36"/>
       <c r="G1397" s="36"/>
@@ -54260,7 +54584,10 @@
       <c r="T1397" s="9"/>
       <c r="U1397" s="9"/>
     </row>
-    <row r="1398" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1398" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1398" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1398" s="36"/>
       <c r="F1398" s="36"/>
       <c r="G1398" s="36"/>
@@ -54293,7 +54620,10 @@
       <c r="T1398" s="9"/>
       <c r="U1398" s="9"/>
     </row>
-    <row r="1399" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1399" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1399" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1399" s="36"/>
       <c r="F1399" s="36"/>
       <c r="G1399" s="36"/>
@@ -54326,7 +54656,10 @@
       <c r="T1399" s="9"/>
       <c r="U1399" s="9"/>
     </row>
-    <row r="1400" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1400" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1400" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1400" s="36"/>
       <c r="F1400" s="36"/>
       <c r="G1400" s="36"/>
@@ -54359,7 +54692,10 @@
       <c r="T1400" s="9"/>
       <c r="U1400" s="9"/>
     </row>
-    <row r="1401" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1401" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1401" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1401" s="36"/>
       <c r="F1401" s="36"/>
       <c r="G1401" s="36"/>
@@ -54392,7 +54728,10 @@
       <c r="T1401" s="9"/>
       <c r="U1401" s="9"/>
     </row>
-    <row r="1402" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1402" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1402" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1402" s="36"/>
       <c r="F1402" s="36"/>
       <c r="G1402" s="36"/>
@@ -54430,7 +54769,10 @@
         <v>1118</v>
       </c>
     </row>
-    <row r="1403" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1403" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1403" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1403" s="36"/>
       <c r="F1403" s="36"/>
       <c r="G1403" s="36"/>
@@ -54465,7 +54807,10 @@
       <c r="T1403" s="9"/>
       <c r="U1403" s="9"/>
     </row>
-    <row r="1404" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1404" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1404" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1404" s="36"/>
       <c r="F1404" s="36"/>
       <c r="G1404" s="36"/>
@@ -54500,7 +54845,10 @@
       <c r="T1404" s="9"/>
       <c r="U1404" s="9"/>
     </row>
-    <row r="1405" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1405" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1405" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1405" s="36"/>
       <c r="F1405" s="36"/>
       <c r="G1405" s="36"/>
@@ -54535,7 +54883,10 @@
       <c r="T1405" s="9"/>
       <c r="U1405" s="9"/>
     </row>
-    <row r="1406" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1406" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1406" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1406" s="36"/>
       <c r="F1406" s="36"/>
       <c r="G1406" s="36"/>
@@ -54572,7 +54923,10 @@
       <c r="T1406" s="9"/>
       <c r="U1406" s="9"/>
     </row>
-    <row r="1407" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1407" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1407" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1407" s="36"/>
       <c r="F1407" s="36"/>
       <c r="G1407" s="36"/>
@@ -54607,7 +54961,10 @@
       <c r="T1407" s="9"/>
       <c r="U1407" s="9"/>
     </row>
-    <row r="1408" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1408" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1408" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1408" s="36"/>
       <c r="F1408" s="36"/>
       <c r="G1408" s="36"/>
@@ -54642,7 +54999,10 @@
       <c r="T1408" s="9"/>
       <c r="U1408" s="9"/>
     </row>
-    <row r="1409" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1409" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1409" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1409" s="36"/>
       <c r="F1409" s="36"/>
       <c r="G1409" s="36"/>
@@ -54675,7 +55035,10 @@
       <c r="T1409" s="9"/>
       <c r="U1409" s="9"/>
     </row>
-    <row r="1410" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1410" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1410" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1410" s="36"/>
       <c r="F1410" s="36"/>
       <c r="G1410" s="36"/>
@@ -54713,7 +55076,10 @@
         <v>1124</v>
       </c>
     </row>
-    <row r="1411" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1411" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1411" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1411" s="36"/>
       <c r="F1411" s="36"/>
       <c r="G1411" s="36"/>
@@ -54746,7 +55112,10 @@
       <c r="T1411" s="9"/>
       <c r="U1411" s="9"/>
     </row>
-    <row r="1412" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1412" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1412" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1412" s="36"/>
       <c r="F1412" s="36"/>
       <c r="G1412" s="36"/>
@@ -54779,7 +55148,10 @@
       <c r="T1412" s="9"/>
       <c r="U1412" s="9"/>
     </row>
-    <row r="1413" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1413" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1413" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1413" s="36"/>
       <c r="F1413" s="36"/>
       <c r="G1413" s="36"/>
@@ -54817,7 +55189,10 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="1414" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1414" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1414" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1414" s="36"/>
       <c r="F1414" s="36"/>
       <c r="G1414" s="36"/>
@@ -54850,7 +55225,10 @@
       <c r="T1414" s="9"/>
       <c r="U1414" s="9"/>
     </row>
-    <row r="1415" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1415" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1415" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1415" s="36"/>
       <c r="F1415" s="36"/>
       <c r="G1415" s="36"/>
@@ -54883,7 +55261,10 @@
       <c r="T1415" s="9"/>
       <c r="U1415" s="9"/>
     </row>
-    <row r="1416" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1416" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1416" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1416" s="36"/>
       <c r="F1416" s="36"/>
       <c r="G1416" s="36"/>
@@ -54916,7 +55297,10 @@
       <c r="T1416" s="9"/>
       <c r="U1416" s="9"/>
     </row>
-    <row r="1417" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1417" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1417" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1417" s="36"/>
       <c r="F1417" s="36"/>
       <c r="G1417" s="36"/>
@@ -54949,7 +55333,10 @@
       <c r="T1417" s="9"/>
       <c r="U1417" s="9"/>
     </row>
-    <row r="1418" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1418" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1418" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1418" s="36"/>
       <c r="F1418" s="36"/>
       <c r="G1418" s="36"/>
@@ -54984,7 +55371,10 @@
         <v>56</v>
       </c>
     </row>
-    <row r="1419" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1419" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1419" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1419" s="36"/>
       <c r="F1419" s="36"/>
       <c r="G1419" s="36"/>
@@ -55022,7 +55412,10 @@
         <v>1131</v>
       </c>
     </row>
-    <row r="1420" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1420" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1420" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1420" s="36"/>
       <c r="F1420" s="36"/>
       <c r="G1420" s="36"/>
@@ -55060,7 +55453,10 @@
         <v>1133</v>
       </c>
     </row>
-    <row r="1421" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1421" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1421" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1421" s="36"/>
       <c r="F1421" s="36"/>
       <c r="G1421" s="36"/>
@@ -55093,7 +55489,10 @@
       <c r="T1421" s="9"/>
       <c r="U1421" s="9"/>
     </row>
-    <row r="1422" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1422" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1422" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1422" s="36"/>
       <c r="F1422" s="36"/>
       <c r="G1422" s="36"/>
@@ -55126,7 +55525,10 @@
       <c r="T1422" s="9"/>
       <c r="U1422" s="9"/>
     </row>
-    <row r="1423" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1423" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1423" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1423" s="36"/>
       <c r="F1423" s="36"/>
       <c r="G1423" s="36"/>
@@ -55164,7 +55566,10 @@
         <v>1136</v>
       </c>
     </row>
-    <row r="1424" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1424" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1424" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1424" s="36"/>
       <c r="F1424" s="36"/>
       <c r="G1424" s="36"/>
@@ -55198,6 +55603,9 @@
       <c r="U1424" s="9"/>
     </row>
     <row r="1425" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C1425" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1425" s="36"/>
       <c r="F1425" s="36"/>
       <c r="G1425" s="36"/>
@@ -55231,6 +55639,9 @@
       <c r="U1425" s="9"/>
     </row>
     <row r="1426" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C1426" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1426" s="36"/>
       <c r="F1426" s="36"/>
       <c r="G1426" s="36"/>
@@ -55264,6 +55675,9 @@
       <c r="U1426" s="9"/>
     </row>
     <row r="1427" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C1427" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1427" s="36"/>
       <c r="F1427" s="36"/>
       <c r="G1427" s="36"/>
@@ -55302,6 +55716,9 @@
       </c>
     </row>
     <row r="1428" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C1428" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1428" s="36"/>
       <c r="F1428" s="36"/>
       <c r="G1428" s="36"/>
@@ -55335,6 +55752,9 @@
       <c r="U1428" s="9"/>
     </row>
     <row r="1429" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C1429" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1429" s="36"/>
       <c r="F1429" s="36"/>
       <c r="G1429" s="36"/>
@@ -55368,6 +55788,9 @@
       <c r="U1429" s="9"/>
     </row>
     <row r="1430" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C1430" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1430" s="36"/>
       <c r="F1430" s="36"/>
       <c r="G1430" s="36"/>
@@ -55406,6 +55829,9 @@
       </c>
     </row>
     <row r="1431" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C1431" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1431" s="36"/>
       <c r="F1431" s="36"/>
       <c r="G1431" s="36"/>
@@ -55439,6 +55865,9 @@
       <c r="U1431" s="9"/>
     </row>
     <row r="1432" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C1432" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1432" s="36"/>
       <c r="F1432" s="36"/>
       <c r="G1432" s="36"/>
@@ -55477,6 +55906,9 @@
       <c r="B1433" s="2" t="s">
         <v>149</v>
       </c>
+      <c r="C1433" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1433" s="36"/>
       <c r="F1433" s="36"/>
       <c r="G1433" s="36"/>
@@ -55510,6 +55942,9 @@
       <c r="U1433" s="9"/>
     </row>
     <row r="1434" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C1434" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1434" s="36"/>
       <c r="F1434" s="36"/>
       <c r="G1434" s="36"/>
@@ -55546,6 +55981,9 @@
       <c r="B1435" s="2" t="s">
         <v>149</v>
       </c>
+      <c r="C1435" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1435" s="36"/>
       <c r="F1435" s="36"/>
       <c r="G1435" s="36"/>
@@ -55579,6 +56017,9 @@
       <c r="U1435" s="9"/>
     </row>
     <row r="1436" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C1436" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1436" s="36"/>
       <c r="F1436" s="36"/>
       <c r="G1436" s="36"/>
@@ -55617,6 +56058,9 @@
       </c>
     </row>
     <row r="1437" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C1437" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1437" s="36"/>
       <c r="F1437" s="36"/>
       <c r="G1437" s="36"/>
@@ -55650,6 +56094,9 @@
       <c r="U1437" s="9"/>
     </row>
     <row r="1438" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C1438" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1438" s="36"/>
       <c r="F1438" s="36"/>
       <c r="G1438" s="36"/>
@@ -55683,6 +56130,9 @@
       <c r="U1438" s="9"/>
     </row>
     <row r="1439" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C1439" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1439" s="36"/>
       <c r="F1439" s="36"/>
       <c r="G1439" s="36"/>
@@ -55716,6 +56166,9 @@
       <c r="U1439" s="9"/>
     </row>
     <row r="1440" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C1440" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1440" s="36"/>
       <c r="F1440" s="36"/>
       <c r="G1440" s="36"/>
@@ -55749,6 +56202,9 @@
       <c r="U1440" s="9"/>
     </row>
     <row r="1441" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C1441" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1441" s="36"/>
       <c r="F1441" s="36"/>
       <c r="G1441" s="36"/>
@@ -55782,6 +56238,9 @@
       <c r="U1441" s="9"/>
     </row>
     <row r="1442" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C1442" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1442" s="36"/>
       <c r="F1442" s="36"/>
       <c r="G1442" s="36"/>
@@ -55815,6 +56274,9 @@
       <c r="U1442" s="9"/>
     </row>
     <row r="1443" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C1443" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1443" s="36"/>
       <c r="F1443" s="36"/>
       <c r="G1443" s="36"/>
@@ -55853,6 +56315,9 @@
       </c>
     </row>
     <row r="1444" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C1444" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1444" s="36"/>
       <c r="F1444" s="36"/>
       <c r="G1444" s="36"/>
@@ -55889,6 +56354,9 @@
       </c>
     </row>
     <row r="1445" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C1445" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1445" s="36"/>
       <c r="F1445" s="36"/>
       <c r="G1445" s="36"/>
@@ -55924,6 +56392,9 @@
       <c r="U1445" s="9"/>
     </row>
     <row r="1446" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C1446" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1446" s="36"/>
       <c r="F1446" s="36"/>
       <c r="G1446" s="36"/>
@@ -55957,6 +56428,9 @@
       <c r="U1446" s="9"/>
     </row>
     <row r="1447" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C1447" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1447" s="36"/>
       <c r="F1447" s="36"/>
       <c r="G1447" s="36"/>
@@ -55992,6 +56466,9 @@
       <c r="U1447" s="9"/>
     </row>
     <row r="1448" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C1448" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1448" s="36"/>
       <c r="F1448" s="36"/>
       <c r="G1448" s="36"/>
@@ -56025,6 +56502,9 @@
       <c r="U1448" s="9"/>
     </row>
     <row r="1449" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C1449" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1449" s="36"/>
       <c r="F1449" s="36"/>
       <c r="G1449" s="36"/>
@@ -56058,6 +56538,9 @@
       <c r="U1449" s="9"/>
     </row>
     <row r="1450" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C1450" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1450" s="36"/>
       <c r="F1450" s="36"/>
       <c r="G1450" s="36"/>
@@ -56091,6 +56574,9 @@
       <c r="U1450" s="9"/>
     </row>
     <row r="1451" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C1451" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1451" s="36"/>
       <c r="F1451" s="36"/>
       <c r="G1451" s="36"/>
@@ -56124,6 +56610,9 @@
       <c r="U1451" s="9"/>
     </row>
     <row r="1452" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C1452" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1452" s="36"/>
       <c r="F1452" s="36"/>
       <c r="G1452" s="36"/>
@@ -56157,6 +56646,9 @@
       <c r="U1452" s="9"/>
     </row>
     <row r="1453" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C1453" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1453" s="36"/>
       <c r="F1453" s="36"/>
       <c r="G1453" s="36"/>
@@ -56192,6 +56684,9 @@
       <c r="U1453" s="9"/>
     </row>
     <row r="1454" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C1454" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1454" s="36"/>
       <c r="F1454" s="36"/>
       <c r="G1454" s="36"/>
@@ -56232,6 +56727,9 @@
       </c>
     </row>
     <row r="1455" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C1455" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1455" s="36"/>
       <c r="F1455" s="36"/>
       <c r="G1455" s="36"/>
@@ -56268,6 +56766,9 @@
       <c r="B1456" s="2" t="s">
         <v>149</v>
       </c>
+      <c r="C1456" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1456" s="36"/>
       <c r="F1456" s="36"/>
       <c r="G1456" s="36"/>
@@ -56300,7 +56801,10 @@
       <c r="T1456" s="9"/>
       <c r="U1456" s="9"/>
     </row>
-    <row r="1457" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1457" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1457" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1457" s="36"/>
       <c r="F1457" s="36"/>
       <c r="G1457" s="36"/>
@@ -56333,7 +56837,10 @@
       <c r="T1457" s="9"/>
       <c r="U1457" s="9"/>
     </row>
-    <row r="1458" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1458" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1458" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1458" s="36"/>
       <c r="F1458" s="36"/>
       <c r="G1458" s="36"/>
@@ -56366,7 +56873,10 @@
       <c r="T1458" s="9"/>
       <c r="U1458" s="9"/>
     </row>
-    <row r="1459" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1459" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1459" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1459" s="36"/>
       <c r="F1459" s="36"/>
       <c r="G1459" s="58" t="s">
@@ -56405,7 +56915,10 @@
       <c r="T1459" s="9"/>
       <c r="U1459" s="9"/>
     </row>
-    <row r="1460" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1460" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1460" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1460" s="36"/>
       <c r="F1460" s="36"/>
       <c r="G1460" s="58" t="s">
@@ -56442,7 +56955,10 @@
       <c r="T1460" s="9"/>
       <c r="U1460" s="9"/>
     </row>
-    <row r="1461" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1461" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1461" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1461" s="58" t="s">
         <v>118</v>
       </c>
@@ -56485,7 +57001,10 @@
       </c>
       <c r="U1461" s="9"/>
     </row>
-    <row r="1462" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1462" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1462" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1462" s="58" t="s">
         <v>118</v>
       </c>
@@ -56522,7 +57041,10 @@
       <c r="T1462" s="9"/>
       <c r="U1462" s="9"/>
     </row>
-    <row r="1463" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1463" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1463" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1463" s="36"/>
       <c r="F1463" s="36"/>
       <c r="G1463" s="36"/>
@@ -56557,7 +57079,10 @@
       <c r="T1463" s="9"/>
       <c r="U1463" s="9"/>
     </row>
-    <row r="1464" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1464" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1464" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1464" s="36"/>
       <c r="F1464" s="36"/>
       <c r="G1464" s="36"/>
@@ -56592,7 +57117,10 @@
         <v>134</v>
       </c>
     </row>
-    <row r="1465" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1465" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1465" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1465" s="36"/>
       <c r="F1465" s="36"/>
       <c r="G1465" s="36"/>
@@ -56625,7 +57153,10 @@
       <c r="T1465" s="9"/>
       <c r="U1465" s="9"/>
     </row>
-    <row r="1466" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1466" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1466" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1466" s="36"/>
       <c r="F1466" s="36"/>
       <c r="G1466" s="36"/>
@@ -56658,7 +57189,10 @@
       <c r="T1466" s="9"/>
       <c r="U1466" s="9"/>
     </row>
-    <row r="1467" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1467" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1467" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1467" s="36"/>
       <c r="F1467" s="36"/>
       <c r="G1467" s="36"/>
@@ -56696,7 +57230,10 @@
         <v>1170</v>
       </c>
     </row>
-    <row r="1468" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1468" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1468" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1468" s="36"/>
       <c r="F1468" s="36"/>
       <c r="G1468" s="36"/>
@@ -56729,7 +57266,10 @@
       <c r="T1468" s="9"/>
       <c r="U1468" s="9"/>
     </row>
-    <row r="1469" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1469" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1469" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1469" s="36"/>
       <c r="F1469" s="36"/>
       <c r="G1469" s="36"/>
@@ -56762,7 +57302,10 @@
       <c r="T1469" s="9"/>
       <c r="U1469" s="9"/>
     </row>
-    <row r="1470" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1470" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1470" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1470" s="36"/>
       <c r="F1470" s="36"/>
       <c r="G1470" s="36"/>
@@ -56795,7 +57338,10 @@
       <c r="T1470" s="9"/>
       <c r="U1470" s="9"/>
     </row>
-    <row r="1471" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1471" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1471" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1471" s="36"/>
       <c r="F1471" s="36"/>
       <c r="G1471" s="36"/>
@@ -56830,7 +57376,10 @@
         <v>57</v>
       </c>
     </row>
-    <row r="1472" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1472" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1472" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1472" s="36"/>
       <c r="F1472" s="36"/>
       <c r="G1472" s="36"/>
@@ -56863,7 +57412,10 @@
       <c r="T1472" s="9"/>
       <c r="U1472" s="9"/>
     </row>
-    <row r="1473" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1473" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1473" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1473" s="36"/>
       <c r="F1473" s="36"/>
       <c r="G1473" s="36"/>
@@ -56898,7 +57450,10 @@
         <v>63</v>
       </c>
     </row>
-    <row r="1474" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1474" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1474" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1474" s="36"/>
       <c r="F1474" s="36"/>
       <c r="G1474" s="36"/>
@@ -56938,7 +57493,10 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="1475" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1475" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1475" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1475" s="36"/>
       <c r="F1475" s="36"/>
       <c r="G1475" s="36"/>
@@ -56973,7 +57531,10 @@
       <c r="T1475" s="9"/>
       <c r="U1475" s="9"/>
     </row>
-    <row r="1476" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1476" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1476" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1476" s="36"/>
       <c r="F1476" s="36"/>
       <c r="G1476" s="36"/>
@@ -57008,7 +57569,10 @@
       <c r="T1476" s="9"/>
       <c r="U1476" s="9"/>
     </row>
-    <row r="1477" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1477" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1477" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1477" s="36"/>
       <c r="F1477" s="36"/>
       <c r="G1477" s="36"/>
@@ -57043,7 +57607,10 @@
       <c r="T1477" s="9"/>
       <c r="U1477" s="9"/>
     </row>
-    <row r="1478" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1478" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1478" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1478" s="36"/>
       <c r="F1478" s="36"/>
       <c r="G1478" s="36"/>
@@ -57078,7 +57645,10 @@
       <c r="T1478" s="9"/>
       <c r="U1478" s="9"/>
     </row>
-    <row r="1479" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1479" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1479" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1479" s="36"/>
       <c r="F1479" s="36"/>
       <c r="G1479" s="36"/>
@@ -57113,7 +57683,10 @@
       <c r="T1479" s="9"/>
       <c r="U1479" s="9"/>
     </row>
-    <row r="1480" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1480" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1480" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1480" s="36"/>
       <c r="F1480" s="36"/>
       <c r="G1480" s="36"/>
@@ -57148,7 +57721,10 @@
       <c r="T1480" s="9"/>
       <c r="U1480" s="9"/>
     </row>
-    <row r="1481" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1481" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1481" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1481" s="36"/>
       <c r="F1481" s="36"/>
       <c r="G1481" s="36"/>
@@ -57183,7 +57759,10 @@
       <c r="T1481" s="9"/>
       <c r="U1481" s="9"/>
     </row>
-    <row r="1482" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1482" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1482" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1482" s="36"/>
       <c r="F1482" s="36"/>
       <c r="G1482" s="36"/>
@@ -57221,7 +57800,10 @@
         <v>1179</v>
       </c>
     </row>
-    <row r="1483" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1483" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1483" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1483" s="58" t="s">
         <v>120</v>
       </c>
@@ -57256,7 +57838,10 @@
       <c r="T1483" s="9"/>
       <c r="U1483" s="9"/>
     </row>
-    <row r="1484" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1484" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1484" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1484" s="58" t="s">
         <v>120</v>
       </c>
@@ -57291,7 +57876,10 @@
       <c r="T1484" s="9"/>
       <c r="U1484" s="9"/>
     </row>
-    <row r="1485" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1485" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1485" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1485" s="36"/>
       <c r="F1485" s="36"/>
       <c r="G1485" s="36"/>
@@ -57325,7 +57913,10 @@
       </c>
       <c r="T1485" s="9"/>
     </row>
-    <row r="1486" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1486" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1486" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1486" s="36"/>
       <c r="F1486" s="36"/>
       <c r="G1486" s="36"/>
@@ -57358,7 +57949,10 @@
       <c r="T1486" s="9"/>
       <c r="U1486" s="9"/>
     </row>
-    <row r="1487" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1487" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1487" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1487" s="36"/>
       <c r="F1487" s="36"/>
       <c r="G1487" s="36"/>
@@ -57393,7 +57987,10 @@
         <v>56</v>
       </c>
     </row>
-    <row r="1488" spans="5:22" x14ac:dyDescent="0.25">
+    <row r="1488" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1488" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1488" s="36"/>
       <c r="F1488" s="36"/>
       <c r="G1488" s="36"/>
@@ -57432,6 +58029,9 @@
       </c>
     </row>
     <row r="1489" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C1489" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1489" s="36"/>
       <c r="F1489" s="36"/>
       <c r="G1489" s="36"/>
@@ -57467,6 +58067,9 @@
       <c r="U1489" s="9"/>
     </row>
     <row r="1490" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C1490" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1490" s="36"/>
       <c r="F1490" s="36"/>
       <c r="G1490" s="36"/>
@@ -57505,6 +58108,9 @@
       </c>
     </row>
     <row r="1491" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C1491" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1491" s="36"/>
       <c r="F1491" s="36"/>
       <c r="G1491" s="36"/>
@@ -57543,6 +58149,9 @@
       </c>
     </row>
     <row r="1492" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C1492" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1492" s="36"/>
       <c r="F1492" s="36"/>
       <c r="G1492" s="36"/>
@@ -57576,6 +58185,9 @@
       <c r="U1492" s="9"/>
     </row>
     <row r="1493" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C1493" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1493" s="36"/>
       <c r="F1493" s="36"/>
       <c r="G1493" s="36"/>
@@ -57609,6 +58221,9 @@
       <c r="U1493" s="9"/>
     </row>
     <row r="1494" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C1494" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1494" s="36"/>
       <c r="F1494" s="36"/>
       <c r="G1494" s="36"/>
@@ -57642,6 +58257,9 @@
       <c r="U1494" s="9"/>
     </row>
     <row r="1495" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C1495" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1495" s="36"/>
       <c r="F1495" s="36"/>
       <c r="G1495" s="36"/>
@@ -57675,6 +58293,9 @@
       <c r="U1495" s="9"/>
     </row>
     <row r="1496" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C1496" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1496" s="36"/>
       <c r="F1496" s="36"/>
       <c r="G1496" s="36"/>
@@ -57708,6 +58329,9 @@
       <c r="U1496" s="9"/>
     </row>
     <row r="1497" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C1497" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1497" s="36"/>
       <c r="F1497" s="36"/>
       <c r="G1497" s="36"/>
@@ -57741,6 +58365,9 @@
       <c r="U1497" s="9"/>
     </row>
     <row r="1498" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C1498" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1498" s="36"/>
       <c r="F1498" s="36"/>
       <c r="G1498" s="36"/>
@@ -57775,6 +58402,9 @@
       <c r="T1498" s="9"/>
     </row>
     <row r="1499" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C1499" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1499" s="36"/>
       <c r="F1499" s="36"/>
       <c r="G1499" s="36"/>
@@ -57808,6 +58438,9 @@
       <c r="U1499" s="9"/>
     </row>
     <row r="1500" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C1500" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1500" s="36"/>
       <c r="F1500" s="36"/>
       <c r="G1500" s="36"/>
@@ -57841,6 +58474,9 @@
       <c r="U1500" s="9"/>
     </row>
     <row r="1501" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C1501" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1501" s="36"/>
       <c r="F1501" s="36"/>
       <c r="G1501" s="36"/>
@@ -57877,6 +58513,9 @@
       <c r="B1502" s="2" t="s">
         <v>148</v>
       </c>
+      <c r="C1502" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1502" s="36"/>
       <c r="F1502" s="36"/>
       <c r="G1502" s="36"/>
@@ -57915,6 +58554,9 @@
       </c>
     </row>
     <row r="1503" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C1503" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1503" s="36"/>
       <c r="F1503" s="58" t="s">
         <v>124</v>
@@ -57950,6 +58592,9 @@
       <c r="U1503" s="9"/>
     </row>
     <row r="1504" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C1504" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1504" s="36"/>
       <c r="F1504" s="58" t="s">
         <v>124</v>
@@ -57986,7 +58631,10 @@
         <v>57</v>
       </c>
     </row>
-    <row r="1505" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="1505" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1505" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1505" s="36"/>
       <c r="F1505" s="36"/>
       <c r="G1505" s="36"/>
@@ -58024,7 +58672,10 @@
         <v>1198</v>
       </c>
     </row>
-    <row r="1506" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="1506" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1506" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1506" s="36"/>
       <c r="F1506" s="36"/>
       <c r="G1506" s="36"/>
@@ -58059,7 +58710,10 @@
         <v>63</v>
       </c>
     </row>
-    <row r="1507" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="1507" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1507" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1507" s="36"/>
       <c r="F1507" s="36"/>
       <c r="G1507" s="36"/>
@@ -58092,7 +58746,10 @@
       <c r="T1507" s="9"/>
       <c r="U1507" s="9"/>
     </row>
-    <row r="1508" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="1508" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1508" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1508" s="36"/>
       <c r="F1508" s="36"/>
       <c r="G1508" s="36"/>
@@ -58127,7 +58784,10 @@
       <c r="T1508" s="9"/>
       <c r="U1508" s="9"/>
     </row>
-    <row r="1509" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="1509" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1509" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1509" s="36"/>
       <c r="F1509" s="36"/>
       <c r="G1509" s="36"/>
@@ -58160,7 +58820,10 @@
       <c r="T1509" s="9"/>
       <c r="U1509" s="9"/>
     </row>
-    <row r="1510" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="1510" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1510" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1510" s="36"/>
       <c r="F1510" s="36"/>
       <c r="G1510" s="36"/>
@@ -58200,7 +58863,10 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="1511" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="1511" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1511" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1511" s="36"/>
       <c r="F1511" s="36"/>
       <c r="G1511" s="36"/>
@@ -58233,7 +58899,10 @@
       <c r="T1511" s="9"/>
       <c r="U1511" s="9"/>
     </row>
-    <row r="1512" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="1512" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1512" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1512" s="36"/>
       <c r="F1512" s="36"/>
       <c r="G1512" s="36"/>
@@ -58266,7 +58935,10 @@
       <c r="T1512" s="9"/>
       <c r="U1512" s="9"/>
     </row>
-    <row r="1513" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="1513" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1513" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1513" s="36"/>
       <c r="F1513" s="36"/>
       <c r="G1513" s="36"/>
@@ -58304,7 +58976,10 @@
         <v>1203</v>
       </c>
     </row>
-    <row r="1514" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="1514" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1514" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1514" s="36"/>
       <c r="F1514" s="36"/>
       <c r="G1514" s="58" t="s">
@@ -58339,7 +59014,10 @@
       <c r="T1514" s="9"/>
       <c r="U1514" s="9"/>
     </row>
-    <row r="1515" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="1515" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1515" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1515" s="36"/>
       <c r="F1515" s="36"/>
       <c r="G1515" s="58" t="s">
@@ -58374,7 +59052,10 @@
       <c r="T1515" s="9"/>
       <c r="U1515" s="9"/>
     </row>
-    <row r="1516" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="1516" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1516" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1516" s="36"/>
       <c r="F1516" s="36"/>
       <c r="G1516" s="58" t="s">
@@ -58409,7 +59090,10 @@
       <c r="T1516" s="9"/>
       <c r="U1516" s="9"/>
     </row>
-    <row r="1517" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="1517" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1517" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="D1517" s="45"/>
       <c r="E1517" s="36"/>
       <c r="F1517" s="36"/>
@@ -58448,7 +59132,10 @@
         <v>1205</v>
       </c>
     </row>
-    <row r="1518" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="1518" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1518" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1518" s="36"/>
       <c r="F1518" s="36"/>
       <c r="G1518" s="36"/>
@@ -58481,7 +59168,10 @@
       <c r="T1518" s="9"/>
       <c r="U1518" s="9"/>
     </row>
-    <row r="1519" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="1519" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1519" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1519" s="36"/>
       <c r="F1519" s="36"/>
       <c r="G1519" s="36"/>
@@ -58514,7 +59204,10 @@
       <c r="T1519" s="9"/>
       <c r="U1519" s="9"/>
     </row>
-    <row r="1520" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="1520" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1520" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1520" s="36"/>
       <c r="F1520" s="36"/>
       <c r="G1520" s="36"/>
@@ -58548,6 +59241,9 @@
       <c r="U1520" s="9"/>
     </row>
     <row r="1521" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C1521" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1521" s="36"/>
       <c r="F1521" s="36"/>
       <c r="G1521" s="36"/>
@@ -58590,6 +59286,9 @@
       </c>
     </row>
     <row r="1522" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C1522" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1522" s="36"/>
       <c r="F1522" s="36"/>
       <c r="G1522" s="36"/>
@@ -58627,6 +59326,9 @@
       <c r="U1522" s="9"/>
     </row>
     <row r="1523" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C1523" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1523" s="36"/>
       <c r="F1523" s="36"/>
       <c r="G1523" s="36"/>
@@ -58663,6 +59365,9 @@
       <c r="B1524" s="2" t="s">
         <v>148</v>
       </c>
+      <c r="C1524" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1524" s="36"/>
       <c r="F1524" s="36"/>
       <c r="G1524" s="36"/>
@@ -58696,6 +59401,9 @@
       <c r="U1524" s="9"/>
     </row>
     <row r="1525" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C1525" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1525" s="36"/>
       <c r="F1525" s="36"/>
       <c r="G1525" s="36"/>
@@ -58731,6 +59439,9 @@
       <c r="U1525" s="9"/>
     </row>
     <row r="1526" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C1526" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1526" s="36"/>
       <c r="F1526" s="36"/>
       <c r="G1526" s="36"/>
@@ -58767,6 +59478,9 @@
       <c r="B1527" s="2" t="s">
         <v>148</v>
       </c>
+      <c r="C1527" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1527" s="36"/>
       <c r="F1527" s="36"/>
       <c r="G1527" s="36"/>
@@ -58803,6 +59517,9 @@
       <c r="B1528" s="2" t="s">
         <v>148</v>
       </c>
+      <c r="C1528" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1528" s="36"/>
       <c r="F1528" s="36"/>
       <c r="G1528" s="36"/>
@@ -58836,6 +59553,9 @@
       <c r="U1528" s="9"/>
     </row>
     <row r="1529" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C1529" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1529" s="36"/>
       <c r="F1529" s="36"/>
       <c r="G1529" s="36"/>
@@ -58873,6 +59593,9 @@
       <c r="U1529" s="9"/>
     </row>
     <row r="1530" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C1530" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1530" s="36"/>
       <c r="F1530" s="36"/>
       <c r="G1530" s="36"/>
@@ -58911,6 +59634,9 @@
       </c>
     </row>
     <row r="1531" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C1531" s="72" t="s">
+        <v>1229</v>
+      </c>
       <c r="E1531" s="36"/>
       <c r="F1531" s="36"/>
       <c r="G1531" s="36"/>

</xml_diff>

<commit_message>
Padam Templates, Ghana Maala edits 15/12/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Raja Files/Padam Inputs/TS 1.1 Padam Input Template.xlsx
+++ b/TS Jatai Working/Raja Files/Padam Inputs/TS 1.1 Padam Input Template.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4460" uniqueCount="1230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4462" uniqueCount="1232">
   <si>
     <t>PS</t>
   </si>
@@ -3695,12 +3695,6 @@
     <t>S</t>
   </si>
   <si>
-    <t>UW,UA</t>
-  </si>
-  <si>
-    <t>P,N[v]</t>
-  </si>
-  <si>
     <t>Vis%N</t>
   </si>
   <si>
@@ -3717,19 +3711,37 @@
   </si>
   <si>
     <t>alopa</t>
+  </si>
+  <si>
+    <t>N%Vis</t>
+  </si>
+  <si>
+    <t>S%N[Sh]</t>
+  </si>
+  <si>
+    <t>UW%UA</t>
+  </si>
+  <si>
+    <t>P%N[v]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -3859,7 +3871,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3869,6 +3881,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3900,210 +3918,216 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="19" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4391,7 +4415,7 @@
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="E1529" sqref="E1529"/>
+      <selection pane="bottomLeft" activeCell="R1363" sqref="R1363"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -22007,10 +22031,10 @@
       <c r="Q472" s="9"/>
       <c r="R472" s="9"/>
       <c r="S472" s="9" t="s">
-        <v>137</v>
+        <v>1228</v>
       </c>
       <c r="T472" s="9" t="s">
-        <v>1221</v>
+        <v>1229</v>
       </c>
       <c r="U472" s="9"/>
     </row>
@@ -33467,7 +33491,7 @@
     </row>
     <row r="801" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D801" s="71" t="s">
-        <v>1226</v>
+        <v>1224</v>
       </c>
       <c r="E801" s="36"/>
       <c r="F801" s="36"/>
@@ -33505,7 +33529,7 @@
     </row>
     <row r="802" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D802" s="71" t="s">
-        <v>1226</v>
+        <v>1224</v>
       </c>
       <c r="E802" s="36"/>
       <c r="F802" s="36"/>
@@ -33540,16 +33564,16 @@
       <c r="Q802" s="9"/>
       <c r="R802" s="9"/>
       <c r="S802" s="9" t="s">
-        <v>1224</v>
+        <v>1222</v>
       </c>
       <c r="T802" s="9" t="s">
-        <v>1225</v>
+        <v>1223</v>
       </c>
       <c r="U802" s="9"/>
     </row>
     <row r="803" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D803" s="71" t="s">
-        <v>1226</v>
+        <v>1224</v>
       </c>
       <c r="E803" s="36"/>
       <c r="F803" s="36"/>
@@ -37245,7 +37269,7 @@
     </row>
     <row r="909" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D909" s="71" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
       <c r="E909" s="36"/>
       <c r="F909" s="36"/>
@@ -37289,7 +37313,7 @@
     </row>
     <row r="910" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D910" s="71" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
       <c r="E910" s="36"/>
       <c r="F910" s="36"/>
@@ -43206,7 +43230,7 @@
       <c r="S1080" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="T1080" s="9" t="s">
+      <c r="T1080" s="74" t="s">
         <v>142</v>
       </c>
       <c r="U1080" s="9"/>
@@ -45761,7 +45785,7 @@
     </row>
     <row r="1153" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D1153" s="71" t="s">
-        <v>1228</v>
+        <v>1226</v>
       </c>
       <c r="E1153" s="36"/>
       <c r="F1153" s="36"/>
@@ -45802,7 +45826,7 @@
     </row>
     <row r="1154" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D1154" s="71" t="s">
-        <v>1228</v>
+        <v>1226</v>
       </c>
       <c r="E1154" s="36"/>
       <c r="F1154" s="36"/>
@@ -45840,7 +45864,7 @@
     </row>
     <row r="1155" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D1155" s="71" t="s">
-        <v>1228</v>
+        <v>1226</v>
       </c>
       <c r="E1155" s="36"/>
       <c r="F1155" s="36"/>
@@ -45918,7 +45942,7 @@
     </row>
     <row r="1157" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D1157" s="71" t="s">
-        <v>1228</v>
+        <v>1226</v>
       </c>
       <c r="E1157" s="36"/>
       <c r="F1157" s="36"/>
@@ -45959,7 +45983,7 @@
     </row>
     <row r="1158" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D1158" s="71" t="s">
-        <v>1228</v>
+        <v>1226</v>
       </c>
       <c r="E1158" s="36"/>
       <c r="F1158" s="36"/>
@@ -51165,7 +51189,7 @@
     </row>
     <row r="1309" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1309" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1309" s="36"/>
       <c r="F1309" s="58" t="s">
@@ -51204,7 +51228,7 @@
     </row>
     <row r="1310" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1310" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1310" s="36"/>
       <c r="F1310" s="58" t="s">
@@ -51244,7 +51268,7 @@
     </row>
     <row r="1311" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1311" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1311" s="36"/>
       <c r="F1311" s="58" t="s">
@@ -51289,7 +51313,7 @@
     </row>
     <row r="1312" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1312" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1312" s="36"/>
       <c r="F1312" s="36"/>
@@ -51325,7 +51349,7 @@
     </row>
     <row r="1313" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1313" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1313" s="36"/>
       <c r="F1313" s="36"/>
@@ -51361,7 +51385,7 @@
     </row>
     <row r="1314" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1314" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1314" s="36"/>
       <c r="F1314" s="36"/>
@@ -51397,7 +51421,7 @@
     </row>
     <row r="1315" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1315" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1315" s="36"/>
       <c r="F1315" s="36"/>
@@ -51433,7 +51457,7 @@
     </row>
     <row r="1316" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1316" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1316" s="36"/>
       <c r="F1316" s="36"/>
@@ -51474,7 +51498,7 @@
     </row>
     <row r="1317" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1317" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1317" s="36"/>
       <c r="F1317" s="36"/>
@@ -51510,7 +51534,7 @@
     </row>
     <row r="1318" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1318" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1318" s="36"/>
       <c r="F1318" s="36"/>
@@ -51546,7 +51570,7 @@
     </row>
     <row r="1319" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1319" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1319" s="36"/>
       <c r="F1319" s="36"/>
@@ -51582,7 +51606,7 @@
     </row>
     <row r="1320" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1320" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1320" s="36"/>
       <c r="F1320" s="36"/>
@@ -51618,7 +51642,7 @@
     </row>
     <row r="1321" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1321" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1321" s="36"/>
       <c r="F1321" s="36"/>
@@ -51654,7 +51678,7 @@
     </row>
     <row r="1322" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1322" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1322" s="36"/>
       <c r="F1322" s="36"/>
@@ -51690,7 +51714,7 @@
     </row>
     <row r="1323" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1323" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1323" s="36"/>
       <c r="F1323" s="36"/>
@@ -51726,7 +51750,7 @@
     </row>
     <row r="1324" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1324" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1324" s="36"/>
       <c r="F1324" s="36"/>
@@ -51762,7 +51786,7 @@
     </row>
     <row r="1325" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1325" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1325" s="36"/>
       <c r="F1325" s="36"/>
@@ -51803,7 +51827,7 @@
     </row>
     <row r="1326" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1326" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1326" s="36"/>
       <c r="F1326" s="36"/>
@@ -51841,7 +51865,7 @@
     </row>
     <row r="1327" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1327" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1327" s="36"/>
       <c r="F1327" s="36"/>
@@ -51879,7 +51903,7 @@
     </row>
     <row r="1328" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1328" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1328" s="36"/>
       <c r="F1328" s="36"/>
@@ -51922,7 +51946,7 @@
     </row>
     <row r="1329" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1329" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1329" s="36"/>
       <c r="F1329" s="36"/>
@@ -51960,7 +51984,7 @@
     </row>
     <row r="1330" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1330" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1330" s="36"/>
       <c r="F1330" s="36"/>
@@ -52003,7 +52027,7 @@
     </row>
     <row r="1331" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1331" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1331" s="36"/>
       <c r="F1331" s="36"/>
@@ -52041,7 +52065,7 @@
     </row>
     <row r="1332" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1332" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1332" s="36"/>
       <c r="F1332" s="36"/>
@@ -52079,7 +52103,7 @@
     </row>
     <row r="1333" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1333" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1333" s="36"/>
       <c r="F1333" s="36"/>
@@ -52118,7 +52142,7 @@
     </row>
     <row r="1334" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1334" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1334" s="36"/>
       <c r="F1334" s="36"/>
@@ -52160,7 +52184,7 @@
     </row>
     <row r="1335" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1335" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1335" s="36"/>
       <c r="F1335" s="36"/>
@@ -52197,7 +52221,7 @@
     </row>
     <row r="1336" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1336" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1336" s="36"/>
       <c r="F1336" s="36"/>
@@ -52233,7 +52257,7 @@
     </row>
     <row r="1337" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1337" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1337" s="36"/>
       <c r="F1337" s="36"/>
@@ -52274,7 +52298,7 @@
     </row>
     <row r="1338" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1338" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1338" s="36"/>
       <c r="F1338" s="36"/>
@@ -52315,7 +52339,7 @@
     </row>
     <row r="1339" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1339" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1339" s="36"/>
       <c r="F1339" s="36"/>
@@ -52356,7 +52380,7 @@
     </row>
     <row r="1340" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1340" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1340" s="36"/>
       <c r="F1340" s="36"/>
@@ -52392,7 +52416,7 @@
     </row>
     <row r="1341" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1341" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1341" s="36"/>
       <c r="F1341" s="36"/>
@@ -52428,7 +52452,7 @@
     </row>
     <row r="1342" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1342" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1342" s="36"/>
       <c r="F1342" s="36"/>
@@ -52469,7 +52493,7 @@
     </row>
     <row r="1343" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1343" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1343" s="36"/>
       <c r="F1343" s="36"/>
@@ -52510,7 +52534,7 @@
     </row>
     <row r="1344" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1344" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1344" s="36"/>
       <c r="F1344" s="36"/>
@@ -52546,7 +52570,7 @@
     </row>
     <row r="1345" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1345" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1345" s="36"/>
       <c r="F1345" s="36"/>
@@ -52582,7 +52606,7 @@
     </row>
     <row r="1346" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1346" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1346" s="36"/>
       <c r="F1346" s="36"/>
@@ -52623,7 +52647,7 @@
     </row>
     <row r="1347" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1347" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1347" s="36"/>
       <c r="F1347" s="36"/>
@@ -52664,7 +52688,7 @@
     </row>
     <row r="1348" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1348" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1348" s="36"/>
       <c r="F1348" s="36"/>
@@ -52700,7 +52724,7 @@
     </row>
     <row r="1349" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1349" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1349" s="36"/>
       <c r="F1349" s="36"/>
@@ -52736,7 +52760,7 @@
     </row>
     <row r="1350" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1350" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1350" s="36"/>
       <c r="F1350" s="36"/>
@@ -52777,7 +52801,7 @@
     </row>
     <row r="1351" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1351" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1351" s="36"/>
       <c r="F1351" s="36"/>
@@ -52813,7 +52837,7 @@
     </row>
     <row r="1352" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1352" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1352" s="36"/>
       <c r="F1352" s="36"/>
@@ -52849,7 +52873,7 @@
     </row>
     <row r="1353" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1353" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1353" s="36"/>
       <c r="F1353" s="36"/>
@@ -52885,7 +52909,7 @@
     </row>
     <row r="1354" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1354" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1354" s="36"/>
       <c r="F1354" s="36"/>
@@ -52926,7 +52950,7 @@
     </row>
     <row r="1355" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1355" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1355" s="36"/>
       <c r="F1355" s="36"/>
@@ -52962,7 +52986,7 @@
     </row>
     <row r="1356" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1356" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1356" s="36"/>
       <c r="F1356" s="36"/>
@@ -53003,7 +53027,7 @@
     </row>
     <row r="1357" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1357" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1357" s="36"/>
       <c r="F1357" s="36"/>
@@ -53044,7 +53068,7 @@
     </row>
     <row r="1358" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1358" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1358" s="36"/>
       <c r="F1358" s="36"/>
@@ -53085,7 +53109,7 @@
     </row>
     <row r="1359" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1359" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1359" s="36"/>
       <c r="F1359" s="36"/>
@@ -53123,7 +53147,7 @@
     </row>
     <row r="1360" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1360" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1360" s="36"/>
       <c r="F1360" s="36"/>
@@ -53161,7 +53185,7 @@
     </row>
     <row r="1361" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1361" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1361" s="36"/>
       <c r="F1361" s="36"/>
@@ -53199,7 +53223,7 @@
     </row>
     <row r="1362" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1362" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1362" s="36"/>
       <c r="F1362" s="36"/>
@@ -53242,7 +53266,7 @@
     </row>
     <row r="1363" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1363" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1363" s="36"/>
       <c r="F1363" s="36"/>
@@ -53280,7 +53304,7 @@
     </row>
     <row r="1364" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1364" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1364" s="36"/>
       <c r="F1364" s="36"/>
@@ -53316,7 +53340,7 @@
     </row>
     <row r="1365" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1365" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1365" s="36"/>
       <c r="F1365" s="36"/>
@@ -53352,7 +53376,7 @@
     </row>
     <row r="1366" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1366" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1366" s="36"/>
       <c r="F1366" s="36"/>
@@ -53388,7 +53412,7 @@
     </row>
     <row r="1367" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1367" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1367" s="36"/>
       <c r="F1367" s="36"/>
@@ -53424,7 +53448,7 @@
     </row>
     <row r="1368" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1368" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1368" s="36"/>
       <c r="F1368" s="36"/>
@@ -53465,7 +53489,7 @@
     </row>
     <row r="1369" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1369" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1369" s="36"/>
       <c r="F1369" s="36"/>
@@ -53503,9 +53527,11 @@
     </row>
     <row r="1370" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1370" s="72" t="s">
-        <v>1229</v>
-      </c>
-      <c r="E1370" s="36"/>
+        <v>1227</v>
+      </c>
+      <c r="E1370" s="73" t="s">
+        <v>118</v>
+      </c>
       <c r="F1370" s="36"/>
       <c r="G1370" s="36"/>
       <c r="H1370" s="58" t="s">
@@ -53536,18 +53562,20 @@
       <c r="Q1370" s="9"/>
       <c r="R1370" s="9"/>
       <c r="S1370" s="9" t="s">
-        <v>1222</v>
+        <v>1230</v>
       </c>
       <c r="T1370" s="9" t="s">
-        <v>1223</v>
+        <v>1231</v>
       </c>
       <c r="U1370" s="9"/>
     </row>
     <row r="1371" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1371" s="72" t="s">
-        <v>1229</v>
-      </c>
-      <c r="E1371" s="36"/>
+        <v>1227</v>
+      </c>
+      <c r="E1371" s="73" t="s">
+        <v>118</v>
+      </c>
       <c r="F1371" s="36"/>
       <c r="G1371" s="36"/>
       <c r="H1371" s="58" t="s">
@@ -53582,7 +53610,7 @@
     </row>
     <row r="1372" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1372" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1372" s="36"/>
       <c r="F1372" s="36"/>
@@ -53624,7 +53652,7 @@
     </row>
     <row r="1373" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1373" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1373" s="36"/>
       <c r="F1373" s="36"/>
@@ -53662,7 +53690,7 @@
     </row>
     <row r="1374" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1374" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1374" s="36"/>
       <c r="F1374" s="36"/>
@@ -53700,7 +53728,7 @@
     </row>
     <row r="1375" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1375" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1375" s="36"/>
       <c r="F1375" s="36"/>
@@ -53736,7 +53764,7 @@
     </row>
     <row r="1376" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1376" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1376" s="36"/>
       <c r="F1376" s="36"/>
@@ -53779,7 +53807,7 @@
     </row>
     <row r="1377" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1377" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1377" s="36"/>
       <c r="F1377" s="36"/>
@@ -53815,7 +53843,7 @@
     </row>
     <row r="1378" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1378" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1378" s="36"/>
       <c r="F1378" s="36"/>
@@ -53851,7 +53879,7 @@
     </row>
     <row r="1379" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1379" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1379" s="36"/>
       <c r="F1379" s="36"/>
@@ -53892,7 +53920,7 @@
     </row>
     <row r="1380" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1380" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1380" s="36"/>
       <c r="F1380" s="36"/>
@@ -53935,7 +53963,7 @@
     </row>
     <row r="1381" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1381" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1381" s="36"/>
       <c r="F1381" s="36"/>
@@ -53978,7 +54006,7 @@
     </row>
     <row r="1382" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1382" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1382" s="36"/>
       <c r="F1382" s="36"/>
@@ -54016,7 +54044,7 @@
     </row>
     <row r="1383" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1383" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1383" s="36"/>
       <c r="F1383" s="36"/>
@@ -54054,7 +54082,7 @@
     </row>
     <row r="1384" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1384" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1384" s="36"/>
       <c r="F1384" s="36"/>
@@ -54092,7 +54120,7 @@
     </row>
     <row r="1385" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1385" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1385" s="36"/>
       <c r="F1385" s="36"/>
@@ -54132,7 +54160,7 @@
     </row>
     <row r="1386" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1386" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1386" s="36"/>
       <c r="F1386" s="36"/>
@@ -54168,7 +54196,7 @@
     </row>
     <row r="1387" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1387" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1387" s="36"/>
       <c r="F1387" s="36"/>
@@ -54209,7 +54237,7 @@
     </row>
     <row r="1388" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1388" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1388" s="36"/>
       <c r="F1388" s="36"/>
@@ -54245,7 +54273,7 @@
     </row>
     <row r="1389" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1389" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1389" s="36"/>
       <c r="F1389" s="36"/>
@@ -54281,7 +54309,7 @@
     </row>
     <row r="1390" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1390" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1390" s="36"/>
       <c r="F1390" s="36"/>
@@ -54317,7 +54345,7 @@
     </row>
     <row r="1391" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1391" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1391" s="36"/>
       <c r="F1391" s="36"/>
@@ -54353,7 +54381,7 @@
     </row>
     <row r="1392" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1392" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1392" s="36"/>
       <c r="F1392" s="36"/>
@@ -54394,7 +54422,7 @@
     </row>
     <row r="1393" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1393" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1393" s="36"/>
       <c r="F1393" s="36"/>
@@ -54435,7 +54463,7 @@
     </row>
     <row r="1394" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1394" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1394" s="36"/>
       <c r="F1394" s="36"/>
@@ -54471,7 +54499,7 @@
     </row>
     <row r="1395" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1395" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1395" s="36"/>
       <c r="F1395" s="36"/>
@@ -54509,7 +54537,7 @@
     </row>
     <row r="1396" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1396" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1396" s="36"/>
       <c r="F1396" s="36"/>
@@ -54550,7 +54578,7 @@
     </row>
     <row r="1397" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1397" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1397" s="36"/>
       <c r="F1397" s="36"/>
@@ -54586,7 +54614,7 @@
     </row>
     <row r="1398" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1398" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1398" s="36"/>
       <c r="F1398" s="36"/>
@@ -54622,7 +54650,7 @@
     </row>
     <row r="1399" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1399" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1399" s="36"/>
       <c r="F1399" s="36"/>
@@ -54658,7 +54686,7 @@
     </row>
     <row r="1400" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1400" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1400" s="36"/>
       <c r="F1400" s="36"/>
@@ -54694,7 +54722,7 @@
     </row>
     <row r="1401" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1401" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1401" s="36"/>
       <c r="F1401" s="36"/>
@@ -54730,7 +54758,7 @@
     </row>
     <row r="1402" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1402" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1402" s="36"/>
       <c r="F1402" s="36"/>
@@ -54771,7 +54799,7 @@
     </row>
     <row r="1403" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1403" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1403" s="36"/>
       <c r="F1403" s="36"/>
@@ -54809,7 +54837,7 @@
     </row>
     <row r="1404" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1404" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1404" s="36"/>
       <c r="F1404" s="36"/>
@@ -54847,7 +54875,7 @@
     </row>
     <row r="1405" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1405" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1405" s="36"/>
       <c r="F1405" s="36"/>
@@ -54885,7 +54913,7 @@
     </row>
     <row r="1406" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1406" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1406" s="36"/>
       <c r="F1406" s="36"/>
@@ -54925,7 +54953,7 @@
     </row>
     <row r="1407" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1407" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1407" s="36"/>
       <c r="F1407" s="36"/>
@@ -54963,7 +54991,7 @@
     </row>
     <row r="1408" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1408" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1408" s="36"/>
       <c r="F1408" s="36"/>
@@ -55001,7 +55029,7 @@
     </row>
     <row r="1409" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1409" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1409" s="36"/>
       <c r="F1409" s="36"/>
@@ -55037,7 +55065,7 @@
     </row>
     <row r="1410" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1410" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1410" s="36"/>
       <c r="F1410" s="36"/>
@@ -55078,7 +55106,7 @@
     </row>
     <row r="1411" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1411" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1411" s="36"/>
       <c r="F1411" s="36"/>
@@ -55114,7 +55142,7 @@
     </row>
     <row r="1412" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1412" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1412" s="36"/>
       <c r="F1412" s="36"/>
@@ -55150,7 +55178,7 @@
     </row>
     <row r="1413" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1413" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1413" s="36"/>
       <c r="F1413" s="36"/>
@@ -55191,7 +55219,7 @@
     </row>
     <row r="1414" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1414" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1414" s="36"/>
       <c r="F1414" s="36"/>
@@ -55227,7 +55255,7 @@
     </row>
     <row r="1415" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1415" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1415" s="36"/>
       <c r="F1415" s="36"/>
@@ -55263,7 +55291,7 @@
     </row>
     <row r="1416" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1416" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1416" s="36"/>
       <c r="F1416" s="36"/>
@@ -55299,7 +55327,7 @@
     </row>
     <row r="1417" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1417" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1417" s="36"/>
       <c r="F1417" s="36"/>
@@ -55335,7 +55363,7 @@
     </row>
     <row r="1418" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1418" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1418" s="36"/>
       <c r="F1418" s="36"/>
@@ -55373,7 +55401,7 @@
     </row>
     <row r="1419" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1419" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1419" s="36"/>
       <c r="F1419" s="36"/>
@@ -55414,7 +55442,7 @@
     </row>
     <row r="1420" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1420" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1420" s="36"/>
       <c r="F1420" s="36"/>
@@ -55455,7 +55483,7 @@
     </row>
     <row r="1421" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1421" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1421" s="36"/>
       <c r="F1421" s="36"/>
@@ -55491,7 +55519,7 @@
     </row>
     <row r="1422" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1422" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1422" s="36"/>
       <c r="F1422" s="36"/>
@@ -55527,7 +55555,7 @@
     </row>
     <row r="1423" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1423" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1423" s="36"/>
       <c r="F1423" s="36"/>
@@ -55568,7 +55596,7 @@
     </row>
     <row r="1424" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1424" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1424" s="36"/>
       <c r="F1424" s="36"/>
@@ -55604,7 +55632,7 @@
     </row>
     <row r="1425" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C1425" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1425" s="36"/>
       <c r="F1425" s="36"/>
@@ -55640,7 +55668,7 @@
     </row>
     <row r="1426" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C1426" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1426" s="36"/>
       <c r="F1426" s="36"/>
@@ -55676,7 +55704,7 @@
     </row>
     <row r="1427" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C1427" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1427" s="36"/>
       <c r="F1427" s="36"/>
@@ -55717,7 +55745,7 @@
     </row>
     <row r="1428" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C1428" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1428" s="36"/>
       <c r="F1428" s="36"/>
@@ -55753,7 +55781,7 @@
     </row>
     <row r="1429" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C1429" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1429" s="36"/>
       <c r="F1429" s="36"/>
@@ -55789,7 +55817,7 @@
     </row>
     <row r="1430" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C1430" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1430" s="36"/>
       <c r="F1430" s="36"/>
@@ -55830,7 +55858,7 @@
     </row>
     <row r="1431" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C1431" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1431" s="36"/>
       <c r="F1431" s="36"/>
@@ -55866,7 +55894,7 @@
     </row>
     <row r="1432" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C1432" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1432" s="36"/>
       <c r="F1432" s="36"/>
@@ -55907,7 +55935,7 @@
         <v>149</v>
       </c>
       <c r="C1433" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1433" s="36"/>
       <c r="F1433" s="36"/>
@@ -55943,7 +55971,7 @@
     </row>
     <row r="1434" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C1434" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1434" s="36"/>
       <c r="F1434" s="36"/>
@@ -55982,7 +56010,7 @@
         <v>149</v>
       </c>
       <c r="C1435" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1435" s="36"/>
       <c r="F1435" s="36"/>
@@ -56018,7 +56046,7 @@
     </row>
     <row r="1436" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C1436" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1436" s="36"/>
       <c r="F1436" s="36"/>
@@ -56059,7 +56087,7 @@
     </row>
     <row r="1437" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C1437" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1437" s="36"/>
       <c r="F1437" s="36"/>
@@ -56095,7 +56123,7 @@
     </row>
     <row r="1438" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C1438" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1438" s="36"/>
       <c r="F1438" s="36"/>
@@ -56131,7 +56159,7 @@
     </row>
     <row r="1439" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C1439" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1439" s="36"/>
       <c r="F1439" s="36"/>
@@ -56167,7 +56195,7 @@
     </row>
     <row r="1440" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C1440" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1440" s="36"/>
       <c r="F1440" s="36"/>
@@ -56203,7 +56231,7 @@
     </row>
     <row r="1441" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C1441" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1441" s="36"/>
       <c r="F1441" s="36"/>
@@ -56239,7 +56267,7 @@
     </row>
     <row r="1442" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C1442" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1442" s="36"/>
       <c r="F1442" s="36"/>
@@ -56275,7 +56303,7 @@
     </row>
     <row r="1443" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C1443" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1443" s="36"/>
       <c r="F1443" s="36"/>
@@ -56316,7 +56344,7 @@
     </row>
     <row r="1444" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C1444" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1444" s="36"/>
       <c r="F1444" s="36"/>
@@ -56355,7 +56383,7 @@
     </row>
     <row r="1445" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C1445" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1445" s="36"/>
       <c r="F1445" s="36"/>
@@ -56393,7 +56421,7 @@
     </row>
     <row r="1446" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C1446" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1446" s="36"/>
       <c r="F1446" s="36"/>
@@ -56429,7 +56457,7 @@
     </row>
     <row r="1447" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C1447" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1447" s="36"/>
       <c r="F1447" s="36"/>
@@ -56467,7 +56495,7 @@
     </row>
     <row r="1448" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C1448" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1448" s="36"/>
       <c r="F1448" s="36"/>
@@ -56503,7 +56531,7 @@
     </row>
     <row r="1449" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C1449" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1449" s="36"/>
       <c r="F1449" s="36"/>
@@ -56539,7 +56567,7 @@
     </row>
     <row r="1450" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C1450" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1450" s="36"/>
       <c r="F1450" s="36"/>
@@ -56575,7 +56603,7 @@
     </row>
     <row r="1451" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C1451" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1451" s="36"/>
       <c r="F1451" s="36"/>
@@ -56611,7 +56639,7 @@
     </row>
     <row r="1452" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C1452" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1452" s="36"/>
       <c r="F1452" s="36"/>
@@ -56647,7 +56675,7 @@
     </row>
     <row r="1453" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C1453" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1453" s="36"/>
       <c r="F1453" s="36"/>
@@ -56685,7 +56713,7 @@
     </row>
     <row r="1454" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C1454" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1454" s="36"/>
       <c r="F1454" s="36"/>
@@ -56728,7 +56756,7 @@
     </row>
     <row r="1455" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C1455" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1455" s="36"/>
       <c r="F1455" s="36"/>
@@ -56767,7 +56795,7 @@
         <v>149</v>
       </c>
       <c r="C1456" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1456" s="36"/>
       <c r="F1456" s="36"/>
@@ -56803,7 +56831,7 @@
     </row>
     <row r="1457" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1457" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1457" s="36"/>
       <c r="F1457" s="36"/>
@@ -56839,7 +56867,7 @@
     </row>
     <row r="1458" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1458" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1458" s="36"/>
       <c r="F1458" s="36"/>
@@ -56875,7 +56903,7 @@
     </row>
     <row r="1459" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1459" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1459" s="36"/>
       <c r="F1459" s="36"/>
@@ -56917,7 +56945,7 @@
     </row>
     <row r="1460" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1460" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1460" s="36"/>
       <c r="F1460" s="36"/>
@@ -56957,7 +56985,7 @@
     </row>
     <row r="1461" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1461" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1461" s="58" t="s">
         <v>118</v>
@@ -57003,7 +57031,7 @@
     </row>
     <row r="1462" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1462" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1462" s="58" t="s">
         <v>118</v>
@@ -57043,7 +57071,7 @@
     </row>
     <row r="1463" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1463" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1463" s="36"/>
       <c r="F1463" s="36"/>
@@ -57081,7 +57109,7 @@
     </row>
     <row r="1464" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1464" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1464" s="36"/>
       <c r="F1464" s="36"/>
@@ -57119,7 +57147,7 @@
     </row>
     <row r="1465" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1465" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1465" s="36"/>
       <c r="F1465" s="36"/>
@@ -57155,7 +57183,7 @@
     </row>
     <row r="1466" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1466" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1466" s="36"/>
       <c r="F1466" s="36"/>
@@ -57191,7 +57219,7 @@
     </row>
     <row r="1467" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1467" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1467" s="36"/>
       <c r="F1467" s="36"/>
@@ -57232,7 +57260,7 @@
     </row>
     <row r="1468" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1468" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1468" s="36"/>
       <c r="F1468" s="36"/>
@@ -57268,7 +57296,7 @@
     </row>
     <row r="1469" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1469" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1469" s="36"/>
       <c r="F1469" s="36"/>
@@ -57304,7 +57332,7 @@
     </row>
     <row r="1470" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1470" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1470" s="36"/>
       <c r="F1470" s="36"/>
@@ -57340,7 +57368,7 @@
     </row>
     <row r="1471" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1471" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1471" s="36"/>
       <c r="F1471" s="36"/>
@@ -57378,7 +57406,7 @@
     </row>
     <row r="1472" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1472" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1472" s="36"/>
       <c r="F1472" s="36"/>
@@ -57414,7 +57442,7 @@
     </row>
     <row r="1473" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1473" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1473" s="36"/>
       <c r="F1473" s="36"/>
@@ -57452,7 +57480,7 @@
     </row>
     <row r="1474" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1474" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1474" s="36"/>
       <c r="F1474" s="36"/>
@@ -57495,7 +57523,7 @@
     </row>
     <row r="1475" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1475" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1475" s="36"/>
       <c r="F1475" s="36"/>
@@ -57533,7 +57561,7 @@
     </row>
     <row r="1476" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1476" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1476" s="36"/>
       <c r="F1476" s="36"/>
@@ -57571,7 +57599,7 @@
     </row>
     <row r="1477" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1477" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1477" s="36"/>
       <c r="F1477" s="36"/>
@@ -57609,7 +57637,7 @@
     </row>
     <row r="1478" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1478" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1478" s="36"/>
       <c r="F1478" s="36"/>
@@ -57647,7 +57675,7 @@
     </row>
     <row r="1479" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1479" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1479" s="36"/>
       <c r="F1479" s="36"/>
@@ -57685,7 +57713,7 @@
     </row>
     <row r="1480" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1480" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1480" s="36"/>
       <c r="F1480" s="36"/>
@@ -57723,7 +57751,7 @@
     </row>
     <row r="1481" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1481" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1481" s="36"/>
       <c r="F1481" s="36"/>
@@ -57761,7 +57789,7 @@
     </row>
     <row r="1482" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1482" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1482" s="36"/>
       <c r="F1482" s="36"/>
@@ -57802,7 +57830,7 @@
     </row>
     <row r="1483" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1483" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1483" s="58" t="s">
         <v>120</v>
@@ -57840,7 +57868,7 @@
     </row>
     <row r="1484" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1484" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1484" s="58" t="s">
         <v>120</v>
@@ -57878,7 +57906,7 @@
     </row>
     <row r="1485" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1485" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1485" s="36"/>
       <c r="F1485" s="36"/>
@@ -57915,7 +57943,7 @@
     </row>
     <row r="1486" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1486" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1486" s="36"/>
       <c r="F1486" s="36"/>
@@ -57951,7 +57979,7 @@
     </row>
     <row r="1487" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1487" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1487" s="36"/>
       <c r="F1487" s="36"/>
@@ -57989,7 +58017,7 @@
     </row>
     <row r="1488" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1488" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1488" s="36"/>
       <c r="F1488" s="36"/>
@@ -58030,7 +58058,7 @@
     </row>
     <row r="1489" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C1489" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1489" s="36"/>
       <c r="F1489" s="36"/>
@@ -58068,7 +58096,7 @@
     </row>
     <row r="1490" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C1490" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1490" s="36"/>
       <c r="F1490" s="36"/>
@@ -58109,7 +58137,7 @@
     </row>
     <row r="1491" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C1491" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1491" s="36"/>
       <c r="F1491" s="36"/>
@@ -58150,7 +58178,7 @@
     </row>
     <row r="1492" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C1492" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1492" s="36"/>
       <c r="F1492" s="36"/>
@@ -58186,7 +58214,7 @@
     </row>
     <row r="1493" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C1493" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1493" s="36"/>
       <c r="F1493" s="36"/>
@@ -58222,7 +58250,7 @@
     </row>
     <row r="1494" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C1494" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1494" s="36"/>
       <c r="F1494" s="36"/>
@@ -58258,7 +58286,7 @@
     </row>
     <row r="1495" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C1495" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1495" s="36"/>
       <c r="F1495" s="36"/>
@@ -58294,7 +58322,7 @@
     </row>
     <row r="1496" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C1496" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1496" s="36"/>
       <c r="F1496" s="36"/>
@@ -58330,7 +58358,7 @@
     </row>
     <row r="1497" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C1497" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1497" s="36"/>
       <c r="F1497" s="36"/>
@@ -58366,7 +58394,7 @@
     </row>
     <row r="1498" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C1498" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1498" s="36"/>
       <c r="F1498" s="36"/>
@@ -58403,7 +58431,7 @@
     </row>
     <row r="1499" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C1499" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1499" s="36"/>
       <c r="F1499" s="36"/>
@@ -58439,7 +58467,7 @@
     </row>
     <row r="1500" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C1500" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1500" s="36"/>
       <c r="F1500" s="36"/>
@@ -58475,7 +58503,7 @@
     </row>
     <row r="1501" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C1501" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1501" s="36"/>
       <c r="F1501" s="36"/>
@@ -58514,7 +58542,7 @@
         <v>148</v>
       </c>
       <c r="C1502" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1502" s="36"/>
       <c r="F1502" s="36"/>
@@ -58555,7 +58583,7 @@
     </row>
     <row r="1503" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C1503" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1503" s="36"/>
       <c r="F1503" s="58" t="s">
@@ -58593,7 +58621,7 @@
     </row>
     <row r="1504" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C1504" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1504" s="36"/>
       <c r="F1504" s="58" t="s">
@@ -58633,7 +58661,7 @@
     </row>
     <row r="1505" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1505" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1505" s="36"/>
       <c r="F1505" s="36"/>
@@ -58674,7 +58702,7 @@
     </row>
     <row r="1506" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1506" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1506" s="36"/>
       <c r="F1506" s="36"/>
@@ -58712,7 +58740,7 @@
     </row>
     <row r="1507" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1507" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1507" s="36"/>
       <c r="F1507" s="36"/>
@@ -58748,7 +58776,7 @@
     </row>
     <row r="1508" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1508" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1508" s="36"/>
       <c r="F1508" s="36"/>
@@ -58786,7 +58814,7 @@
     </row>
     <row r="1509" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1509" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1509" s="36"/>
       <c r="F1509" s="36"/>
@@ -58822,7 +58850,7 @@
     </row>
     <row r="1510" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1510" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1510" s="36"/>
       <c r="F1510" s="36"/>
@@ -58865,7 +58893,7 @@
     </row>
     <row r="1511" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1511" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1511" s="36"/>
       <c r="F1511" s="36"/>
@@ -58901,7 +58929,7 @@
     </row>
     <row r="1512" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1512" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1512" s="36"/>
       <c r="F1512" s="36"/>
@@ -58937,7 +58965,7 @@
     </row>
     <row r="1513" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1513" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1513" s="36"/>
       <c r="F1513" s="36"/>
@@ -58978,7 +59006,7 @@
     </row>
     <row r="1514" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1514" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1514" s="36"/>
       <c r="F1514" s="36"/>
@@ -59016,7 +59044,7 @@
     </row>
     <row r="1515" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1515" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1515" s="36"/>
       <c r="F1515" s="36"/>
@@ -59054,7 +59082,7 @@
     </row>
     <row r="1516" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1516" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1516" s="36"/>
       <c r="F1516" s="36"/>
@@ -59092,7 +59120,7 @@
     </row>
     <row r="1517" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1517" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="D1517" s="45"/>
       <c r="E1517" s="36"/>
@@ -59134,7 +59162,7 @@
     </row>
     <row r="1518" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1518" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1518" s="36"/>
       <c r="F1518" s="36"/>
@@ -59170,7 +59198,7 @@
     </row>
     <row r="1519" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1519" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1519" s="36"/>
       <c r="F1519" s="36"/>
@@ -59206,7 +59234,7 @@
     </row>
     <row r="1520" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1520" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1520" s="36"/>
       <c r="F1520" s="36"/>
@@ -59242,7 +59270,7 @@
     </row>
     <row r="1521" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C1521" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1521" s="36"/>
       <c r="F1521" s="36"/>
@@ -59287,7 +59315,7 @@
     </row>
     <row r="1522" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C1522" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1522" s="36"/>
       <c r="F1522" s="36"/>
@@ -59327,7 +59355,7 @@
     </row>
     <row r="1523" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C1523" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1523" s="36"/>
       <c r="F1523" s="36"/>
@@ -59366,7 +59394,7 @@
         <v>148</v>
       </c>
       <c r="C1524" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1524" s="36"/>
       <c r="F1524" s="36"/>
@@ -59402,7 +59430,7 @@
     </row>
     <row r="1525" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C1525" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1525" s="36"/>
       <c r="F1525" s="36"/>
@@ -59440,7 +59468,7 @@
     </row>
     <row r="1526" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C1526" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1526" s="36"/>
       <c r="F1526" s="36"/>
@@ -59479,7 +59507,7 @@
         <v>148</v>
       </c>
       <c r="C1527" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1527" s="36"/>
       <c r="F1527" s="36"/>
@@ -59518,7 +59546,7 @@
         <v>148</v>
       </c>
       <c r="C1528" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1528" s="36"/>
       <c r="F1528" s="36"/>
@@ -59554,7 +59582,7 @@
     </row>
     <row r="1529" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C1529" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1529" s="36"/>
       <c r="F1529" s="36"/>
@@ -59594,7 +59622,7 @@
     </row>
     <row r="1530" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C1530" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1530" s="36"/>
       <c r="F1530" s="36"/>
@@ -59635,7 +59663,7 @@
     </row>
     <row r="1531" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C1531" s="72" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E1531" s="36"/>
       <c r="F1531" s="36"/>

</xml_diff>

<commit_message>
TS Padam Input related 22/12/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Raja Files/Padam Inputs/TS 1.1 Padam Input Template.xlsx
+++ b/TS Jatai Working/Raja Files/Padam Inputs/TS 1.1 Padam Input Template.xlsx
@@ -4424,10 +4424,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V1580"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A254" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A549" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="B268" sqref="B268"/>
+      <selection pane="bottomLeft" activeCell="O558" sqref="O558"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Changes to Padam Template Kramam etc 24/01/2021
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Raja Files/Padam Inputs/TS 1.1 Padam Input Template.xlsx
+++ b/TS Jatai Working/Raja Files/Padam Inputs/TS 1.1 Padam Input Template.xlsx
@@ -4421,10 +4421,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V1580"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A769" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A580" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="N771" sqref="N771"/>
+      <selection pane="bottomLeft" activeCell="I633" sqref="I633"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Various Padam/Jatai/Ghana Maala files - 01/03/2021
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Raja Files/Padam Inputs/TS 1.1 Padam Input Template.xlsx
+++ b/TS Jatai Working/Raja Files/Padam Inputs/TS 1.1 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\Raja Files\Padam Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06C6CA1A-7ACE-4DCD-9BAC-737CCF54297D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ECEECFD-984D-4DDA-9DC6-78B63B66E4AA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4428,10 +4428,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V1579"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1188" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1398" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="N1075" sqref="N1075"/>
+      <selection pane="bottomLeft" activeCell="T1463" sqref="T1463"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Template files changed 03/03/2021
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Raja Files/Padam Inputs/TS 1.1 Padam Input Template.xlsx
+++ b/TS Jatai Working/Raja Files/Padam Inputs/TS 1.1 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\Raja Files\Padam Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ECEECFD-984D-4DDA-9DC6-78B63B66E4AA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{946073F1-D339-4002-B2F5-F96549A55485}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4429,7 +4429,7 @@
   <dimension ref="A1:V1579"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1398" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A798" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="T1463" sqref="T1463"/>
     </sheetView>

</xml_diff>

<commit_message>
Padam Input Template Raja output changes 09/03/2021
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Raja Files/Padam Inputs/TS 1.1 Padam Input Template.xlsx
+++ b/TS Jatai Working/Raja Files/Padam Inputs/TS 1.1 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\Raja Files\Padam Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1206B947-15AC-4B70-83D4-7EE0E7F89CCA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E26BB024-3C00-4699-AD93-BF5BC2F08B75}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4441,10 +4441,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W1580"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A574" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1520" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="N1080" sqref="N1080"/>
+      <selection pane="bottomLeft" activeCell="N50" sqref="N50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>

</xml_diff>